<commit_message>
mise a jour du cahier des charges, planing, contenu version
</commit_message>
<xml_diff>
--- a/documentation/3_2_Modele_PlanningLundiMardi.xlsx
+++ b/documentation/3_2_Modele_PlanningLundiMardi.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11122"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Emf\306\306project-G4\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/gabriel_beer_studentfr_ch/Documents/EMF/Informatique EMF/Troisième année/306/306project-G4/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A30F631-669B-4B85-80D9-41CC652520C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:1_{9A30F631-669B-4B85-80D9-41CC652520C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C825F6B-FBEE-EF4A-A437-817D91B600B1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-2180" windowWidth="38400" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Planning!$A:$C,Planning!$1:$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Planning!$A$1:$CE$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Planning!$A$1:$CE$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Tâches</t>
   </si>
@@ -117,67 +117,7 @@
     <t xml:space="preserve">Compte rendu du Kick-off </t>
   </si>
   <si>
-    <t>Création des diagrammes de cas d’utilisation</t>
-  </si>
-  <si>
-    <t>Création du diagramme d'activité</t>
-  </si>
-  <si>
-    <t>Création du diagramme de classes</t>
-  </si>
-  <si>
-    <t>Création du diagramme de séquence</t>
-  </si>
-  <si>
-    <t>Création du modèle ER</t>
-  </si>
-  <si>
-    <t>Mise en place du projet backend</t>
-  </si>
-  <si>
-    <t>Connexion aux capteurs Phidget</t>
-  </si>
-  <si>
-    <t>Lecture des valeurs de température + humidité</t>
-  </si>
-  <si>
-    <t>Création de l'API REST</t>
-  </si>
-  <si>
-    <t>Sauvegarde des données dans la base de données</t>
-  </si>
-  <si>
-    <t>Système d’alertes</t>
-  </si>
-  <si>
-    <t>Tests unitaires simples backend</t>
-  </si>
-  <si>
-    <t>Mise en place du projet frontend</t>
-  </si>
-  <si>
-    <t>Page tableau de bord</t>
-  </si>
-  <si>
-    <t>Page détail d'une salle</t>
-  </si>
-  <si>
-    <t>Page modification des seuils</t>
-  </si>
-  <si>
-    <t>Intégration visuelle</t>
-  </si>
-  <si>
-    <t>Tests front + vérification sur mobile</t>
-  </si>
-  <si>
     <t>Connexion des API au frontend</t>
-  </si>
-  <si>
-    <t>Vérification du rafraîchissement des données</t>
-  </si>
-  <si>
-    <t>Tests d’affichage des alertes</t>
   </si>
   <si>
     <t>Tests fonctionnels complets</t>
@@ -235,6 +175,39 @@
   </si>
   <si>
     <t>Création du diagramme useCase</t>
+  </si>
+  <si>
+    <t>Mise en place du backend web</t>
+  </si>
+  <si>
+    <t>Installatioin de l'os sur le(s) rpi</t>
+  </si>
+  <si>
+    <t>Connexion des capteurs phidget</t>
+  </si>
+  <si>
+    <t>Création du programme pour rpi</t>
+  </si>
+  <si>
+    <t>Création système d’alertes</t>
+  </si>
+  <si>
+    <t>Mise en place du frontend web</t>
+  </si>
+  <si>
+    <t>Tests front + vérification sur navigateur mobile</t>
+  </si>
+  <si>
+    <t>Tests des alertes</t>
+  </si>
+  <si>
+    <t>Création système login</t>
+  </si>
+  <si>
+    <t>Création de lhistorique capteurs</t>
+  </si>
+  <si>
+    <t>Vérification et fix du rafraîchissement des données</t>
   </si>
 </sst>
 </file>
@@ -379,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -778,12 +751,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -944,6 +928,50 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" textRotation="90"/>
       <protection locked="0"/>
@@ -996,51 +1024,39 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1048,29 +1064,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{0E09CA26-D57B-4FEF-A8F4-4CB706A0B1E1}"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1111,14 +1105,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>19844</xdr:colOff>
+      <xdr:colOff>19845</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>93135</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>148828</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1134,8 +1128,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3785394" y="679450"/>
-          <a:ext cx="1631156" cy="5228828"/>
+          <a:off x="4126178" y="702733"/>
+          <a:ext cx="911490" cy="5542095"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1542,41 +1536,63 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1F3DDA15-6875-2149-842D-93584F9F0ADA}">
+  <we:reference id="wa200009404" version="1.0.0.3" store="fr-FR" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200009404" version="1.0.0.3" store="WA200009404" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="Office.AutoShowTaskpaneWithDocument" value="true"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CF43"/>
+  <dimension ref="A1:CF35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="94" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="O6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29:CE29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="42.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="6.54296875" style="3" customWidth="1"/>
-    <col min="4" max="83" width="2.1796875" style="2" customWidth="1"/>
-    <col min="84" max="84" width="3.1796875" style="3" customWidth="1"/>
-    <col min="85" max="297" width="9.1796875" style="3" customWidth="1"/>
-    <col min="298" max="16384" width="11.54296875" style="3"/>
+    <col min="1" max="1" width="47.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="3" customWidth="1"/>
+    <col min="4" max="83" width="2.1640625" style="2" customWidth="1"/>
+    <col min="84" max="84" width="3.1640625" style="3" customWidth="1"/>
+    <col min="85" max="297" width="9.1640625" style="3" customWidth="1"/>
+    <col min="298" max="16384" width="11.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" ht="23" x14ac:dyDescent="0.5">
-      <c r="A1" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
+    <row r="1" spans="1:84" ht="23" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1611,177 +1627,177 @@
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
     </row>
-    <row r="2" spans="1:84" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:84" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61"/>
-      <c r="V2" s="61"/>
-      <c r="W2" s="61"/>
-      <c r="X2" s="61"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="61"/>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="61"/>
-      <c r="AC2" s="61"/>
-      <c r="AD2" s="61"/>
-      <c r="AE2" s="61"/>
-      <c r="AF2" s="61"/>
-      <c r="AG2" s="61"/>
-      <c r="AH2" s="61"/>
-      <c r="AI2" s="61"/>
-      <c r="AJ2" s="61"/>
-      <c r="AK2" s="61"/>
-      <c r="AL2" s="61"/>
-      <c r="AM2" s="61"/>
-      <c r="AN2" s="61"/>
-      <c r="AO2" s="61"/>
-      <c r="AP2" s="61"/>
-      <c r="AQ2" s="61"/>
-      <c r="AR2" s="61"/>
-      <c r="AS2" s="61"/>
-      <c r="AT2" s="61"/>
-      <c r="AU2" s="61"/>
-      <c r="AV2" s="61"/>
-      <c r="AW2" s="61"/>
-      <c r="AX2" s="61"/>
-      <c r="AY2" s="61"/>
-      <c r="AZ2" s="61"/>
-      <c r="BA2" s="61"/>
-      <c r="BB2" s="61"/>
-      <c r="BC2" s="61"/>
-      <c r="BD2" s="61"/>
-      <c r="BE2" s="61"/>
-      <c r="BF2" s="61"/>
-      <c r="BG2" s="61"/>
-      <c r="BH2" s="61"/>
-      <c r="BI2" s="61"/>
-      <c r="BJ2" s="61"/>
-      <c r="BK2" s="61"/>
-      <c r="BL2" s="61"/>
-      <c r="BM2" s="61"/>
-      <c r="BN2" s="61"/>
-      <c r="BO2" s="61"/>
-      <c r="BP2" s="61"/>
-      <c r="BQ2" s="61"/>
-      <c r="BR2" s="61"/>
-      <c r="BS2" s="61"/>
-      <c r="BT2" s="61"/>
-      <c r="BU2" s="61"/>
-      <c r="BV2" s="61"/>
-      <c r="BW2" s="61"/>
-      <c r="BX2" s="61"/>
-      <c r="BY2" s="61"/>
-      <c r="BZ2" s="61"/>
-      <c r="CA2" s="61"/>
-      <c r="CB2" s="61"/>
-      <c r="CC2" s="61"/>
-      <c r="CD2" s="61"/>
-      <c r="CE2" s="61"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="52"/>
+      <c r="V2" s="52"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="52"/>
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="52"/>
+      <c r="AD2" s="52"/>
+      <c r="AE2" s="52"/>
+      <c r="AF2" s="52"/>
+      <c r="AG2" s="52"/>
+      <c r="AH2" s="52"/>
+      <c r="AI2" s="52"/>
+      <c r="AJ2" s="52"/>
+      <c r="AK2" s="52"/>
+      <c r="AL2" s="52"/>
+      <c r="AM2" s="52"/>
+      <c r="AN2" s="52"/>
+      <c r="AO2" s="52"/>
+      <c r="AP2" s="52"/>
+      <c r="AQ2" s="52"/>
+      <c r="AR2" s="52"/>
+      <c r="AS2" s="52"/>
+      <c r="AT2" s="52"/>
+      <c r="AU2" s="52"/>
+      <c r="AV2" s="52"/>
+      <c r="AW2" s="52"/>
+      <c r="AX2" s="52"/>
+      <c r="AY2" s="52"/>
+      <c r="AZ2" s="52"/>
+      <c r="BA2" s="52"/>
+      <c r="BB2" s="52"/>
+      <c r="BC2" s="52"/>
+      <c r="BD2" s="52"/>
+      <c r="BE2" s="52"/>
+      <c r="BF2" s="52"/>
+      <c r="BG2" s="52"/>
+      <c r="BH2" s="52"/>
+      <c r="BI2" s="52"/>
+      <c r="BJ2" s="52"/>
+      <c r="BK2" s="52"/>
+      <c r="BL2" s="52"/>
+      <c r="BM2" s="52"/>
+      <c r="BN2" s="52"/>
+      <c r="BO2" s="52"/>
+      <c r="BP2" s="52"/>
+      <c r="BQ2" s="52"/>
+      <c r="BR2" s="52"/>
+      <c r="BS2" s="52"/>
+      <c r="BT2" s="52"/>
+      <c r="BU2" s="52"/>
+      <c r="BV2" s="52"/>
+      <c r="BW2" s="52"/>
+      <c r="BX2" s="52"/>
+      <c r="BY2" s="52"/>
+      <c r="BZ2" s="52"/>
+      <c r="CA2" s="52"/>
+      <c r="CB2" s="52"/>
+      <c r="CC2" s="52"/>
+      <c r="CD2" s="52"/>
+      <c r="CE2" s="52"/>
     </row>
-    <row r="3" spans="1:84" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="62"/>
-      <c r="S3" s="62"/>
-      <c r="T3" s="62"/>
-      <c r="U3" s="62"/>
-      <c r="V3" s="62"/>
-      <c r="W3" s="62"/>
-      <c r="X3" s="62"/>
-      <c r="Y3" s="62"/>
-      <c r="Z3" s="62"/>
-      <c r="AA3" s="62"/>
-      <c r="AB3" s="62"/>
-      <c r="AC3" s="62"/>
-      <c r="AD3" s="62"/>
-      <c r="AE3" s="62"/>
-      <c r="AF3" s="62"/>
-      <c r="AG3" s="62"/>
-      <c r="AH3" s="62"/>
-      <c r="AI3" s="62"/>
-      <c r="AJ3" s="62"/>
-      <c r="AK3" s="62"/>
-      <c r="AL3" s="62"/>
-      <c r="AM3" s="62"/>
-      <c r="AN3" s="62"/>
-      <c r="AO3" s="62"/>
-      <c r="AP3" s="62"/>
-      <c r="AQ3" s="62"/>
-      <c r="AR3" s="62"/>
-      <c r="AS3" s="62"/>
-      <c r="AT3" s="62"/>
-      <c r="AU3" s="62"/>
-      <c r="AV3" s="62"/>
-      <c r="AW3" s="62"/>
-      <c r="AX3" s="62"/>
-      <c r="AY3" s="62"/>
-      <c r="AZ3" s="62"/>
-      <c r="BA3" s="62"/>
-      <c r="BB3" s="62"/>
-      <c r="BC3" s="62"/>
-      <c r="BD3" s="62"/>
-      <c r="BE3" s="62"/>
-      <c r="BF3" s="62"/>
-      <c r="BG3" s="62"/>
-      <c r="BH3" s="62"/>
-      <c r="BI3" s="62"/>
-      <c r="BJ3" s="62"/>
-      <c r="BK3" s="62"/>
-      <c r="BL3" s="62"/>
-      <c r="BM3" s="62"/>
-      <c r="BN3" s="62"/>
-      <c r="BO3" s="62"/>
-      <c r="BP3" s="62"/>
-      <c r="BQ3" s="62"/>
-      <c r="BR3" s="62"/>
-      <c r="BS3" s="62"/>
-      <c r="BT3" s="62"/>
-      <c r="BU3" s="62"/>
-      <c r="BV3" s="62"/>
-      <c r="BW3" s="62"/>
-      <c r="BX3" s="62"/>
-      <c r="BY3" s="62"/>
-      <c r="BZ3" s="62"/>
-      <c r="CA3" s="62"/>
-      <c r="CB3" s="62"/>
-      <c r="CC3" s="62"/>
-      <c r="CD3" s="62"/>
-      <c r="CE3" s="62"/>
+    <row r="3" spans="1:84" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53"/>
+      <c r="X3" s="53"/>
+      <c r="Y3" s="53"/>
+      <c r="Z3" s="53"/>
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="53"/>
+      <c r="AC3" s="53"/>
+      <c r="AD3" s="53"/>
+      <c r="AE3" s="53"/>
+      <c r="AF3" s="53"/>
+      <c r="AG3" s="53"/>
+      <c r="AH3" s="53"/>
+      <c r="AI3" s="53"/>
+      <c r="AJ3" s="53"/>
+      <c r="AK3" s="53"/>
+      <c r="AL3" s="53"/>
+      <c r="AM3" s="53"/>
+      <c r="AN3" s="53"/>
+      <c r="AO3" s="53"/>
+      <c r="AP3" s="53"/>
+      <c r="AQ3" s="53"/>
+      <c r="AR3" s="53"/>
+      <c r="AS3" s="53"/>
+      <c r="AT3" s="53"/>
+      <c r="AU3" s="53"/>
+      <c r="AV3" s="53"/>
+      <c r="AW3" s="53"/>
+      <c r="AX3" s="53"/>
+      <c r="AY3" s="53"/>
+      <c r="AZ3" s="53"/>
+      <c r="BA3" s="53"/>
+      <c r="BB3" s="53"/>
+      <c r="BC3" s="53"/>
+      <c r="BD3" s="53"/>
+      <c r="BE3" s="53"/>
+      <c r="BF3" s="53"/>
+      <c r="BG3" s="53"/>
+      <c r="BH3" s="53"/>
+      <c r="BI3" s="53"/>
+      <c r="BJ3" s="53"/>
+      <c r="BK3" s="53"/>
+      <c r="BL3" s="53"/>
+      <c r="BM3" s="53"/>
+      <c r="BN3" s="53"/>
+      <c r="BO3" s="53"/>
+      <c r="BP3" s="53"/>
+      <c r="BQ3" s="53"/>
+      <c r="BR3" s="53"/>
+      <c r="BS3" s="53"/>
+      <c r="BT3" s="53"/>
+      <c r="BU3" s="53"/>
+      <c r="BV3" s="53"/>
+      <c r="BW3" s="53"/>
+      <c r="BX3" s="53"/>
+      <c r="BY3" s="53"/>
+      <c r="BZ3" s="53"/>
+      <c r="CA3" s="53"/>
+      <c r="CB3" s="53"/>
+      <c r="CC3" s="53"/>
+      <c r="CD3" s="53"/>
+      <c r="CE3" s="53"/>
     </row>
-    <row r="4" spans="1:84" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="46" t="s">
+    <row r="4" spans="1:84" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="57" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="26" t="s">
@@ -1790,132 +1806,132 @@
       <c r="C4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="57" t="s">
+      <c r="D4" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="59">
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="48">
         <v>45992</v>
       </c>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="57" t="s">
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="59">
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="48">
         <v>45993</v>
       </c>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="60"/>
-      <c r="T4" s="57" t="s">
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="58"/>
-      <c r="X4" s="59">
+      <c r="U4" s="51"/>
+      <c r="V4" s="51"/>
+      <c r="W4" s="51"/>
+      <c r="X4" s="48">
         <v>45999</v>
       </c>
-      <c r="Y4" s="59"/>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="60"/>
-      <c r="AB4" s="57" t="s">
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="49"/>
+      <c r="AB4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="AC4" s="58"/>
-      <c r="AD4" s="58"/>
-      <c r="AE4" s="58"/>
-      <c r="AF4" s="59">
+      <c r="AC4" s="51"/>
+      <c r="AD4" s="51"/>
+      <c r="AE4" s="51"/>
+      <c r="AF4" s="48">
         <v>46000</v>
       </c>
-      <c r="AG4" s="59"/>
-      <c r="AH4" s="59"/>
-      <c r="AI4" s="60"/>
-      <c r="AJ4" s="57" t="s">
+      <c r="AG4" s="48"/>
+      <c r="AH4" s="48"/>
+      <c r="AI4" s="49"/>
+      <c r="AJ4" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="AK4" s="58"/>
-      <c r="AL4" s="58"/>
-      <c r="AM4" s="58"/>
-      <c r="AN4" s="59">
+      <c r="AK4" s="51"/>
+      <c r="AL4" s="51"/>
+      <c r="AM4" s="51"/>
+      <c r="AN4" s="48">
         <v>46006</v>
       </c>
-      <c r="AO4" s="59"/>
-      <c r="AP4" s="59"/>
-      <c r="AQ4" s="60"/>
-      <c r="AR4" s="57" t="s">
+      <c r="AO4" s="48"/>
+      <c r="AP4" s="48"/>
+      <c r="AQ4" s="49"/>
+      <c r="AR4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="AS4" s="58"/>
-      <c r="AT4" s="58"/>
-      <c r="AU4" s="58"/>
-      <c r="AV4" s="59">
+      <c r="AS4" s="51"/>
+      <c r="AT4" s="51"/>
+      <c r="AU4" s="51"/>
+      <c r="AV4" s="48">
         <v>46007</v>
       </c>
-      <c r="AW4" s="59"/>
-      <c r="AX4" s="59"/>
-      <c r="AY4" s="60"/>
-      <c r="AZ4" s="57" t="s">
+      <c r="AW4" s="48"/>
+      <c r="AX4" s="48"/>
+      <c r="AY4" s="49"/>
+      <c r="AZ4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="BA4" s="58"/>
-      <c r="BB4" s="58"/>
-      <c r="BC4" s="58"/>
-      <c r="BD4" s="59">
+      <c r="BA4" s="51"/>
+      <c r="BB4" s="51"/>
+      <c r="BC4" s="51"/>
+      <c r="BD4" s="48">
         <v>46027</v>
       </c>
-      <c r="BE4" s="59"/>
-      <c r="BF4" s="59"/>
-      <c r="BG4" s="60"/>
-      <c r="BH4" s="57" t="s">
+      <c r="BE4" s="48"/>
+      <c r="BF4" s="48"/>
+      <c r="BG4" s="49"/>
+      <c r="BH4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="BI4" s="58"/>
-      <c r="BJ4" s="58"/>
-      <c r="BK4" s="58"/>
-      <c r="BL4" s="59">
+      <c r="BI4" s="51"/>
+      <c r="BJ4" s="51"/>
+      <c r="BK4" s="51"/>
+      <c r="BL4" s="48">
         <v>46028</v>
       </c>
-      <c r="BM4" s="59"/>
-      <c r="BN4" s="59"/>
-      <c r="BO4" s="60"/>
-      <c r="BP4" s="57" t="s">
+      <c r="BM4" s="48"/>
+      <c r="BN4" s="48"/>
+      <c r="BO4" s="49"/>
+      <c r="BP4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="BQ4" s="58"/>
-      <c r="BR4" s="58"/>
-      <c r="BS4" s="58"/>
-      <c r="BT4" s="59">
+      <c r="BQ4" s="51"/>
+      <c r="BR4" s="51"/>
+      <c r="BS4" s="51"/>
+      <c r="BT4" s="48">
         <v>46034</v>
       </c>
-      <c r="BU4" s="59"/>
-      <c r="BV4" s="59"/>
-      <c r="BW4" s="60"/>
-      <c r="BX4" s="57" t="s">
+      <c r="BU4" s="48"/>
+      <c r="BV4" s="48"/>
+      <c r="BW4" s="49"/>
+      <c r="BX4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="BY4" s="58"/>
-      <c r="BZ4" s="58"/>
-      <c r="CA4" s="58"/>
-      <c r="CB4" s="59">
+      <c r="BY4" s="51"/>
+      <c r="BZ4" s="51"/>
+      <c r="CA4" s="51"/>
+      <c r="CB4" s="48">
         <v>46035</v>
       </c>
-      <c r="CC4" s="59"/>
-      <c r="CD4" s="59"/>
-      <c r="CE4" s="60"/>
-      <c r="CF4" s="44" t="s">
+      <c r="CC4" s="48"/>
+      <c r="CD4" s="48"/>
+      <c r="CE4" s="49"/>
+      <c r="CF4" s="55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:84" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
+    <row r="5" spans="1:84" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="58"/>
       <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
@@ -2162,14 +2178,14 @@
       <c r="CE5" s="7">
         <v>8</v>
       </c>
-      <c r="CF5" s="44"/>
+      <c r="CF5" s="55"/>
     </row>
-    <row r="6" spans="1:84" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:84" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="30"/>
@@ -2188,16 +2204,16 @@
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
       <c r="S6" s="11"/>
-      <c r="T6" s="48" t="s">
+      <c r="T6" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="49"/>
-      <c r="V6" s="49"/>
-      <c r="W6" s="49"/>
-      <c r="X6" s="49"/>
-      <c r="Y6" s="49"/>
-      <c r="Z6" s="49"/>
-      <c r="AA6" s="50"/>
+      <c r="U6" s="60"/>
+      <c r="V6" s="60"/>
+      <c r="W6" s="60"/>
+      <c r="X6" s="60"/>
+      <c r="Y6" s="60"/>
+      <c r="Z6" s="60"/>
+      <c r="AA6" s="61"/>
       <c r="AB6" s="12"/>
       <c r="AC6" s="10"/>
       <c r="AD6" s="10"/>
@@ -2254,14 +2270,14 @@
       <c r="CC6" s="10"/>
       <c r="CD6" s="10"/>
       <c r="CE6" s="11"/>
-      <c r="CF6" s="44"/>
+      <c r="CF6" s="55"/>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="15"/>
@@ -2270,24 +2286,24 @@
       <c r="G7" s="16"/>
       <c r="H7" s="32"/>
       <c r="I7" s="32"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="16"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
       <c r="N7" s="16"/>
       <c r="O7" s="16"/>
       <c r="P7" s="16"/>
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
       <c r="S7" s="17"/>
-      <c r="T7" s="51"/>
-      <c r="U7" s="52"/>
-      <c r="V7" s="52"/>
-      <c r="W7" s="52"/>
-      <c r="X7" s="52"/>
-      <c r="Y7" s="52"/>
-      <c r="Z7" s="52"/>
-      <c r="AA7" s="53"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="63"/>
+      <c r="W7" s="63"/>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="63"/>
+      <c r="Z7" s="63"/>
+      <c r="AA7" s="64"/>
       <c r="AB7" s="15"/>
       <c r="AC7" s="16"/>
       <c r="AD7" s="16"/>
@@ -2344,40 +2360,40 @@
       <c r="CC7" s="16"/>
       <c r="CD7" s="16"/>
       <c r="CE7" s="17"/>
-      <c r="CF7" s="44"/>
+      <c r="CF7" s="55"/>
     </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="15"/>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
       <c r="P8" s="16"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
       <c r="S8" s="17"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="52"/>
-      <c r="W8" s="52"/>
-      <c r="X8" s="52"/>
-      <c r="Y8" s="52"/>
-      <c r="Z8" s="52"/>
-      <c r="AA8" s="53"/>
+      <c r="T8" s="62"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="63"/>
+      <c r="W8" s="63"/>
+      <c r="X8" s="63"/>
+      <c r="Y8" s="63"/>
+      <c r="Z8" s="63"/>
+      <c r="AA8" s="64"/>
       <c r="AB8" s="15"/>
       <c r="AC8" s="16"/>
       <c r="AD8" s="16"/>
@@ -2434,15 +2450,13 @@
       <c r="CC8" s="16"/>
       <c r="CD8" s="16"/>
       <c r="CE8" s="17"/>
-      <c r="CF8" s="44"/>
+      <c r="CF8" s="55"/>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>40</v>
-      </c>
+      <c r="B9" s="24"/>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
@@ -2454,20 +2468,20 @@
       <c r="K9" s="17"/>
       <c r="L9" s="15"/>
       <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
       <c r="S9" s="17"/>
-      <c r="T9" s="51"/>
-      <c r="U9" s="52"/>
-      <c r="V9" s="52"/>
-      <c r="W9" s="52"/>
-      <c r="X9" s="52"/>
-      <c r="Y9" s="52"/>
-      <c r="Z9" s="52"/>
-      <c r="AA9" s="53"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="63"/>
+      <c r="X9" s="63"/>
+      <c r="Y9" s="63"/>
+      <c r="Z9" s="63"/>
+      <c r="AA9" s="64"/>
       <c r="AB9" s="15"/>
       <c r="AC9" s="16"/>
       <c r="AD9" s="16"/>
@@ -2524,40 +2538,40 @@
       <c r="CC9" s="16"/>
       <c r="CD9" s="16"/>
       <c r="CE9" s="17"/>
-      <c r="CF9" s="44"/>
+      <c r="CF9" s="55"/>
     </row>
-    <row r="10" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A10" s="39" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="16"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="45"/>
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="P10" s="16"/>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
       <c r="S10" s="17"/>
-      <c r="T10" s="51"/>
-      <c r="U10" s="52"/>
-      <c r="V10" s="52"/>
-      <c r="W10" s="52"/>
-      <c r="X10" s="52"/>
-      <c r="Y10" s="52"/>
-      <c r="Z10" s="52"/>
-      <c r="AA10" s="53"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="63"/>
+      <c r="W10" s="63"/>
+      <c r="X10" s="63"/>
+      <c r="Y10" s="63"/>
+      <c r="Z10" s="63"/>
+      <c r="AA10" s="64"/>
       <c r="AB10" s="15"/>
       <c r="AC10" s="16"/>
       <c r="AD10" s="16"/>
@@ -2614,13 +2628,13 @@
       <c r="CC10" s="16"/>
       <c r="CD10" s="16"/>
       <c r="CE10" s="17"/>
-      <c r="CF10" s="44"/>
+      <c r="CF10" s="55"/>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A11" s="66" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="39"/>
+    <row r="11" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A11" s="68" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="24"/>
       <c r="C11" s="14"/>
       <c r="D11" s="15"/>
       <c r="E11" s="16"/>
@@ -2638,34 +2652,34 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
       <c r="S11" s="17"/>
-      <c r="T11" s="51"/>
-      <c r="U11" s="52"/>
-      <c r="V11" s="52"/>
-      <c r="W11" s="52"/>
-      <c r="X11" s="52"/>
-      <c r="Y11" s="52"/>
-      <c r="Z11" s="52"/>
-      <c r="AA11" s="53"/>
-      <c r="AB11" s="15"/>
-      <c r="AC11" s="16"/>
-      <c r="AD11" s="16"/>
-      <c r="AE11" s="16"/>
+      <c r="T11" s="62"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="63"/>
+      <c r="W11" s="63"/>
+      <c r="X11" s="63"/>
+      <c r="Y11" s="63"/>
+      <c r="Z11" s="63"/>
+      <c r="AA11" s="64"/>
+      <c r="AB11" s="69"/>
+      <c r="AC11" s="69"/>
+      <c r="AD11" s="69"/>
+      <c r="AE11" s="69"/>
       <c r="AF11" s="16"/>
       <c r="AG11" s="16"/>
       <c r="AH11" s="16"/>
       <c r="AI11" s="17"/>
-      <c r="AJ11" s="15"/>
-      <c r="AK11" s="16"/>
-      <c r="AL11" s="16"/>
-      <c r="AM11" s="16"/>
-      <c r="AN11" s="16"/>
-      <c r="AO11" s="16"/>
-      <c r="AP11" s="16"/>
-      <c r="AQ11" s="17"/>
-      <c r="AR11" s="15"/>
-      <c r="AS11" s="16"/>
-      <c r="AT11" s="16"/>
-      <c r="AU11" s="16"/>
+      <c r="AJ11" s="69"/>
+      <c r="AK11" s="69"/>
+      <c r="AL11" s="69"/>
+      <c r="AM11" s="69"/>
+      <c r="AN11" s="69"/>
+      <c r="AO11" s="69"/>
+      <c r="AP11" s="69"/>
+      <c r="AQ11" s="69"/>
+      <c r="AR11" s="69"/>
+      <c r="AS11" s="69"/>
+      <c r="AT11" s="69"/>
+      <c r="AU11" s="69"/>
       <c r="AV11" s="16"/>
       <c r="AW11" s="16"/>
       <c r="AX11" s="16"/>
@@ -2702,13 +2716,13 @@
       <c r="CC11" s="16"/>
       <c r="CD11" s="16"/>
       <c r="CE11" s="17"/>
-      <c r="CF11" s="44"/>
+      <c r="CF11" s="55"/>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="39"/>
+    <row r="12" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A12" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="24"/>
       <c r="C12" s="14"/>
       <c r="D12" s="15"/>
       <c r="E12" s="16"/>
@@ -2726,46 +2740,46 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
       <c r="S12" s="17"/>
-      <c r="T12" s="51"/>
-      <c r="U12" s="52"/>
-      <c r="V12" s="52"/>
-      <c r="W12" s="52"/>
-      <c r="X12" s="52"/>
-      <c r="Y12" s="52"/>
-      <c r="Z12" s="52"/>
-      <c r="AA12" s="53"/>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="16"/>
-      <c r="AD12" s="16"/>
-      <c r="AE12" s="16"/>
-      <c r="AF12" s="16"/>
-      <c r="AG12" s="16"/>
-      <c r="AH12" s="16"/>
-      <c r="AI12" s="17"/>
-      <c r="AJ12" s="15"/>
-      <c r="AK12" s="16"/>
-      <c r="AL12" s="16"/>
-      <c r="AM12" s="16"/>
-      <c r="AN12" s="16"/>
-      <c r="AO12" s="16"/>
-      <c r="AP12" s="16"/>
-      <c r="AQ12" s="17"/>
-      <c r="AR12" s="15"/>
-      <c r="AS12" s="16"/>
-      <c r="AT12" s="16"/>
-      <c r="AU12" s="16"/>
+      <c r="T12" s="62"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="63"/>
+      <c r="W12" s="63"/>
+      <c r="X12" s="63"/>
+      <c r="Y12" s="63"/>
+      <c r="Z12" s="63"/>
+      <c r="AA12" s="64"/>
+      <c r="AB12" s="72"/>
+      <c r="AC12" s="72"/>
+      <c r="AD12" s="73"/>
+      <c r="AE12" s="73"/>
+      <c r="AF12" s="74"/>
+      <c r="AG12" s="74"/>
+      <c r="AH12" s="74"/>
+      <c r="AI12" s="75"/>
+      <c r="AJ12" s="72"/>
+      <c r="AK12" s="73"/>
+      <c r="AL12" s="73"/>
+      <c r="AM12" s="73"/>
+      <c r="AN12" s="73"/>
+      <c r="AO12" s="73"/>
+      <c r="AP12" s="73"/>
+      <c r="AQ12" s="76"/>
+      <c r="AR12" s="72"/>
+      <c r="AS12" s="73"/>
+      <c r="AT12" s="73"/>
+      <c r="AU12" s="73"/>
       <c r="AV12" s="16"/>
       <c r="AW12" s="16"/>
       <c r="AX12" s="16"/>
       <c r="AY12" s="17"/>
-      <c r="AZ12" s="15"/>
-      <c r="BA12" s="16"/>
-      <c r="BB12" s="16"/>
-      <c r="BC12" s="16"/>
-      <c r="BD12" s="16"/>
-      <c r="BE12" s="16"/>
-      <c r="BF12" s="16"/>
-      <c r="BG12" s="17"/>
+      <c r="AZ12" s="3"/>
+      <c r="BA12" s="3"/>
+      <c r="BB12" s="3"/>
+      <c r="BC12" s="69"/>
+      <c r="BD12" s="69"/>
+      <c r="BE12" s="69"/>
+      <c r="BF12" s="69"/>
+      <c r="BG12" s="69"/>
       <c r="BH12" s="15"/>
       <c r="BI12" s="16"/>
       <c r="BJ12" s="16"/>
@@ -2790,11 +2804,11 @@
       <c r="CC12" s="16"/>
       <c r="CD12" s="16"/>
       <c r="CE12" s="17"/>
-      <c r="CF12" s="44"/>
+      <c r="CF12" s="55"/>
     </row>
-    <row r="13" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>18</v>
+    <row r="13" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A13" s="68" t="s">
+        <v>28</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="14"/>
@@ -2814,16 +2828,16 @@
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
       <c r="S13" s="17"/>
-      <c r="T13" s="51"/>
-      <c r="U13" s="52"/>
-      <c r="V13" s="52"/>
-      <c r="W13" s="52"/>
-      <c r="X13" s="52"/>
-      <c r="Y13" s="52"/>
-      <c r="Z13" s="52"/>
-      <c r="AA13" s="53"/>
-      <c r="AB13" s="15"/>
-      <c r="AC13" s="16"/>
+      <c r="T13" s="62"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="63"/>
+      <c r="W13" s="63"/>
+      <c r="X13" s="63"/>
+      <c r="Y13" s="63"/>
+      <c r="Z13" s="63"/>
+      <c r="AA13" s="64"/>
+      <c r="AB13" s="70"/>
+      <c r="AC13" s="70"/>
       <c r="AD13" s="16"/>
       <c r="AE13" s="16"/>
       <c r="AF13" s="16"/>
@@ -2878,11 +2892,11 @@
       <c r="CC13" s="16"/>
       <c r="CD13" s="16"/>
       <c r="CE13" s="17"/>
-      <c r="CF13" s="44"/>
+      <c r="CF13" s="55"/>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>19</v>
+    <row r="14" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A14" s="68" t="s">
+        <v>29</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="14"/>
@@ -2902,17 +2916,17 @@
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
       <c r="S14" s="17"/>
-      <c r="T14" s="51"/>
-      <c r="U14" s="52"/>
-      <c r="V14" s="52"/>
-      <c r="W14" s="52"/>
-      <c r="X14" s="52"/>
-      <c r="Y14" s="52"/>
-      <c r="Z14" s="52"/>
-      <c r="AA14" s="53"/>
+      <c r="T14" s="62"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="63"/>
+      <c r="W14" s="63"/>
+      <c r="X14" s="63"/>
+      <c r="Y14" s="63"/>
+      <c r="Z14" s="63"/>
+      <c r="AA14" s="64"/>
       <c r="AB14" s="15"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="16"/>
+      <c r="AD14" s="32"/>
       <c r="AE14" s="16"/>
       <c r="AF14" s="16"/>
       <c r="AG14" s="16"/>
@@ -2966,11 +2980,11 @@
       <c r="CC14" s="16"/>
       <c r="CD14" s="16"/>
       <c r="CE14" s="17"/>
-      <c r="CF14" s="44"/>
+      <c r="CF14" s="55"/>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>20</v>
+    <row r="15" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A15" s="68" t="s">
+        <v>30</v>
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="14"/>
@@ -2990,40 +3004,40 @@
       <c r="Q15" s="16"/>
       <c r="R15" s="16"/>
       <c r="S15" s="17"/>
-      <c r="T15" s="51"/>
-      <c r="U15" s="52"/>
-      <c r="V15" s="52"/>
-      <c r="W15" s="52"/>
-      <c r="X15" s="52"/>
-      <c r="Y15" s="52"/>
-      <c r="Z15" s="52"/>
-      <c r="AA15" s="53"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="63"/>
+      <c r="V15" s="63"/>
+      <c r="W15" s="63"/>
+      <c r="X15" s="63"/>
+      <c r="Y15" s="63"/>
+      <c r="Z15" s="63"/>
+      <c r="AA15" s="64"/>
       <c r="AB15" s="15"/>
       <c r="AC15" s="16"/>
       <c r="AD15" s="16"/>
-      <c r="AE15" s="16"/>
+      <c r="AE15" s="32"/>
       <c r="AF15" s="16"/>
       <c r="AG15" s="16"/>
       <c r="AH15" s="16"/>
       <c r="AI15" s="17"/>
-      <c r="AJ15" s="15"/>
-      <c r="AK15" s="16"/>
-      <c r="AL15" s="16"/>
-      <c r="AM15" s="16"/>
-      <c r="AN15" s="16"/>
-      <c r="AO15" s="16"/>
-      <c r="AP15" s="16"/>
-      <c r="AQ15" s="17"/>
-      <c r="AR15" s="15"/>
-      <c r="AS15" s="16"/>
-      <c r="AT15" s="16"/>
-      <c r="AU15" s="16"/>
+      <c r="AJ15" s="70"/>
+      <c r="AK15" s="70"/>
+      <c r="AL15" s="70"/>
+      <c r="AM15" s="70"/>
+      <c r="AN15" s="70"/>
+      <c r="AO15" s="70"/>
+      <c r="AP15" s="70"/>
+      <c r="AQ15" s="70"/>
+      <c r="AR15" s="70"/>
+      <c r="AS15" s="70"/>
+      <c r="AT15" s="70"/>
+      <c r="AU15" s="70"/>
       <c r="AV15" s="16"/>
       <c r="AW15" s="16"/>
       <c r="AX15" s="16"/>
       <c r="AY15" s="17"/>
-      <c r="AZ15" s="15"/>
-      <c r="BA15" s="16"/>
+      <c r="AZ15" s="70"/>
+      <c r="BA15" s="70"/>
       <c r="BB15" s="16"/>
       <c r="BC15" s="16"/>
       <c r="BD15" s="16"/>
@@ -3054,11 +3068,11 @@
       <c r="CC15" s="16"/>
       <c r="CD15" s="16"/>
       <c r="CE15" s="17"/>
-      <c r="CF15" s="44"/>
+      <c r="CF15" s="55"/>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>21</v>
+    <row r="16" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A16" s="68" t="s">
+        <v>36</v>
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="14"/>
@@ -3078,14 +3092,14 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
       <c r="S16" s="17"/>
-      <c r="T16" s="51"/>
-      <c r="U16" s="52"/>
-      <c r="V16" s="52"/>
-      <c r="W16" s="52"/>
-      <c r="X16" s="52"/>
-      <c r="Y16" s="52"/>
-      <c r="Z16" s="52"/>
-      <c r="AA16" s="53"/>
+      <c r="T16" s="62"/>
+      <c r="U16" s="63"/>
+      <c r="V16" s="63"/>
+      <c r="W16" s="63"/>
+      <c r="X16" s="63"/>
+      <c r="Y16" s="63"/>
+      <c r="Z16" s="63"/>
+      <c r="AA16" s="64"/>
       <c r="AB16" s="15"/>
       <c r="AC16" s="16"/>
       <c r="AD16" s="16"/>
@@ -3110,26 +3124,26 @@
       <c r="AW16" s="16"/>
       <c r="AX16" s="16"/>
       <c r="AY16" s="17"/>
-      <c r="AZ16" s="15"/>
-      <c r="BA16" s="16"/>
-      <c r="BB16" s="16"/>
-      <c r="BC16" s="16"/>
-      <c r="BD16" s="16"/>
-      <c r="BE16" s="16"/>
-      <c r="BF16" s="16"/>
-      <c r="BG16" s="17"/>
-      <c r="BH16" s="15"/>
-      <c r="BI16" s="16"/>
-      <c r="BJ16" s="16"/>
-      <c r="BK16" s="16"/>
+      <c r="AZ16" s="45"/>
+      <c r="BA16" s="45"/>
+      <c r="BB16" s="45"/>
+      <c r="BC16" s="45"/>
+      <c r="BD16" s="45"/>
+      <c r="BE16" s="45"/>
+      <c r="BF16" s="45"/>
+      <c r="BG16" s="45"/>
+      <c r="BH16" s="45"/>
+      <c r="BI16" s="45"/>
+      <c r="BJ16" s="71"/>
+      <c r="BK16" s="71"/>
       <c r="BL16" s="16"/>
       <c r="BM16" s="16"/>
       <c r="BN16" s="16"/>
       <c r="BO16" s="17"/>
-      <c r="BP16" s="15"/>
-      <c r="BQ16" s="16"/>
-      <c r="BR16" s="16"/>
-      <c r="BS16" s="16"/>
+      <c r="BP16" s="71"/>
+      <c r="BQ16" s="71"/>
+      <c r="BR16" s="3"/>
+      <c r="BS16" s="3"/>
       <c r="BT16" s="16"/>
       <c r="BU16" s="16"/>
       <c r="BV16" s="16"/>
@@ -3142,11 +3156,11 @@
       <c r="CC16" s="16"/>
       <c r="CD16" s="16"/>
       <c r="CE16" s="17"/>
-      <c r="CF16" s="44"/>
+      <c r="CF16" s="55"/>
     </row>
-    <row r="17" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>22</v>
+    <row r="17" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A17" s="68" t="s">
+        <v>31</v>
       </c>
       <c r="B17" s="24"/>
       <c r="C17" s="14"/>
@@ -3166,14 +3180,14 @@
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
       <c r="S17" s="17"/>
-      <c r="T17" s="51"/>
-      <c r="U17" s="52"/>
-      <c r="V17" s="52"/>
-      <c r="W17" s="52"/>
-      <c r="X17" s="52"/>
-      <c r="Y17" s="52"/>
-      <c r="Z17" s="52"/>
-      <c r="AA17" s="53"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="63"/>
+      <c r="V17" s="63"/>
+      <c r="W17" s="63"/>
+      <c r="X17" s="63"/>
+      <c r="Y17" s="63"/>
+      <c r="Z17" s="63"/>
+      <c r="AA17" s="64"/>
       <c r="AB17" s="15"/>
       <c r="AC17" s="16"/>
       <c r="AD17" s="16"/>
@@ -3206,18 +3220,18 @@
       <c r="BE17" s="16"/>
       <c r="BF17" s="16"/>
       <c r="BG17" s="17"/>
-      <c r="BH17" s="15"/>
-      <c r="BI17" s="16"/>
-      <c r="BJ17" s="16"/>
-      <c r="BK17" s="16"/>
+      <c r="BH17" s="69"/>
+      <c r="BI17" s="69"/>
+      <c r="BJ17" s="69"/>
+      <c r="BK17" s="69"/>
       <c r="BL17" s="16"/>
       <c r="BM17" s="16"/>
       <c r="BN17" s="16"/>
       <c r="BO17" s="17"/>
-      <c r="BP17" s="15"/>
-      <c r="BQ17" s="16"/>
-      <c r="BR17" s="16"/>
-      <c r="BS17" s="16"/>
+      <c r="BP17" s="69"/>
+      <c r="BQ17" s="44"/>
+      <c r="BR17" s="69"/>
+      <c r="BS17" s="44"/>
       <c r="BT17" s="16"/>
       <c r="BU17" s="16"/>
       <c r="BV17" s="16"/>
@@ -3230,11 +3244,11 @@
       <c r="CC17" s="16"/>
       <c r="CD17" s="16"/>
       <c r="CE17" s="17"/>
-      <c r="CF17" s="44"/>
+      <c r="CF17" s="55"/>
     </row>
-    <row r="18" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>23</v>
+    <row r="18" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A18" s="68" t="s">
+        <v>32</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="14"/>
@@ -3254,40 +3268,40 @@
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
       <c r="S18" s="17"/>
-      <c r="T18" s="51"/>
-      <c r="U18" s="52"/>
-      <c r="V18" s="52"/>
-      <c r="W18" s="52"/>
-      <c r="X18" s="52"/>
-      <c r="Y18" s="52"/>
-      <c r="Z18" s="52"/>
-      <c r="AA18" s="53"/>
-      <c r="AB18" s="15"/>
-      <c r="AC18" s="16"/>
-      <c r="AD18" s="16"/>
-      <c r="AE18" s="16"/>
+      <c r="T18" s="62"/>
+      <c r="U18" s="63"/>
+      <c r="V18" s="63"/>
+      <c r="W18" s="63"/>
+      <c r="X18" s="63"/>
+      <c r="Y18" s="63"/>
+      <c r="Z18" s="63"/>
+      <c r="AA18" s="64"/>
+      <c r="AB18" s="71"/>
+      <c r="AC18" s="71"/>
+      <c r="AD18" s="71"/>
+      <c r="AE18" s="71"/>
       <c r="AF18" s="16"/>
       <c r="AG18" s="16"/>
       <c r="AH18" s="16"/>
       <c r="AI18" s="17"/>
-      <c r="AJ18" s="15"/>
-      <c r="AK18" s="16"/>
-      <c r="AL18" s="16"/>
-      <c r="AM18" s="16"/>
-      <c r="AN18" s="16"/>
-      <c r="AO18" s="16"/>
-      <c r="AP18" s="16"/>
-      <c r="AQ18" s="17"/>
-      <c r="AR18" s="15"/>
-      <c r="AS18" s="16"/>
-      <c r="AT18" s="16"/>
-      <c r="AU18" s="16"/>
+      <c r="AJ18" s="71"/>
+      <c r="AK18" s="71"/>
+      <c r="AL18" s="71"/>
+      <c r="AM18" s="71"/>
+      <c r="AN18" s="71"/>
+      <c r="AO18" s="71"/>
+      <c r="AP18" s="71"/>
+      <c r="AQ18" s="71"/>
+      <c r="AR18" s="71"/>
+      <c r="AS18" s="71"/>
+      <c r="AT18" s="71"/>
+      <c r="AU18" s="71"/>
       <c r="AV18" s="16"/>
       <c r="AW18" s="16"/>
       <c r="AX18" s="16"/>
       <c r="AY18" s="17"/>
-      <c r="AZ18" s="15"/>
-      <c r="BA18" s="16"/>
+      <c r="AZ18" s="72"/>
+      <c r="BA18" s="72"/>
       <c r="BB18" s="16"/>
       <c r="BC18" s="16"/>
       <c r="BD18" s="16"/>
@@ -3318,11 +3332,11 @@
       <c r="CC18" s="16"/>
       <c r="CD18" s="16"/>
       <c r="CE18" s="17"/>
-      <c r="CF18" s="44"/>
+      <c r="CF18" s="55"/>
     </row>
-    <row r="19" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>24</v>
+    <row r="19" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A19" s="68" t="s">
+        <v>33</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="14"/>
@@ -3342,14 +3356,14 @@
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
       <c r="S19" s="17"/>
-      <c r="T19" s="51"/>
-      <c r="U19" s="52"/>
-      <c r="V19" s="52"/>
-      <c r="W19" s="52"/>
-      <c r="X19" s="52"/>
-      <c r="Y19" s="52"/>
-      <c r="Z19" s="52"/>
-      <c r="AA19" s="53"/>
+      <c r="T19" s="62"/>
+      <c r="U19" s="63"/>
+      <c r="V19" s="63"/>
+      <c r="W19" s="63"/>
+      <c r="X19" s="63"/>
+      <c r="Y19" s="63"/>
+      <c r="Z19" s="63"/>
+      <c r="AA19" s="64"/>
       <c r="AB19" s="15"/>
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
@@ -3382,16 +3396,16 @@
       <c r="BE19" s="16"/>
       <c r="BF19" s="16"/>
       <c r="BG19" s="17"/>
-      <c r="BH19" s="15"/>
-      <c r="BI19" s="16"/>
-      <c r="BJ19" s="16"/>
-      <c r="BK19" s="16"/>
+      <c r="BH19" s="70"/>
+      <c r="BI19" s="70"/>
+      <c r="BJ19" s="70"/>
+      <c r="BK19" s="70"/>
       <c r="BL19" s="16"/>
       <c r="BM19" s="16"/>
       <c r="BN19" s="16"/>
       <c r="BO19" s="17"/>
-      <c r="BP19" s="15"/>
-      <c r="BQ19" s="16"/>
+      <c r="BP19" s="70"/>
+      <c r="BQ19" s="70"/>
       <c r="BR19" s="16"/>
       <c r="BS19" s="16"/>
       <c r="BT19" s="16"/>
@@ -3406,11 +3420,11 @@
       <c r="CC19" s="16"/>
       <c r="CD19" s="16"/>
       <c r="CE19" s="17"/>
-      <c r="CF19" s="44"/>
+      <c r="CF19" s="55"/>
     </row>
-    <row r="20" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A20" s="13" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="14"/>
@@ -3430,14 +3444,14 @@
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
       <c r="S20" s="17"/>
-      <c r="T20" s="51"/>
-      <c r="U20" s="52"/>
-      <c r="V20" s="52"/>
-      <c r="W20" s="52"/>
-      <c r="X20" s="52"/>
-      <c r="Y20" s="52"/>
-      <c r="Z20" s="52"/>
-      <c r="AA20" s="53"/>
+      <c r="T20" s="62"/>
+      <c r="U20" s="63"/>
+      <c r="V20" s="63"/>
+      <c r="W20" s="63"/>
+      <c r="X20" s="63"/>
+      <c r="Y20" s="63"/>
+      <c r="Z20" s="63"/>
+      <c r="AA20" s="64"/>
       <c r="AB20" s="15"/>
       <c r="AC20" s="16"/>
       <c r="AD20" s="16"/>
@@ -3462,9 +3476,9 @@
       <c r="AW20" s="16"/>
       <c r="AX20" s="16"/>
       <c r="AY20" s="17"/>
-      <c r="AZ20" s="15"/>
-      <c r="BA20" s="16"/>
-      <c r="BB20" s="16"/>
+      <c r="AZ20" s="69"/>
+      <c r="BA20" s="69"/>
+      <c r="BB20" s="69"/>
       <c r="BC20" s="16"/>
       <c r="BD20" s="16"/>
       <c r="BE20" s="16"/>
@@ -3494,11 +3508,11 @@
       <c r="CC20" s="16"/>
       <c r="CD20" s="16"/>
       <c r="CE20" s="17"/>
-      <c r="CF20" s="44"/>
+      <c r="CF20" s="55"/>
     </row>
-    <row r="21" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>26</v>
+    <row r="21" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A21" s="68" t="s">
+        <v>37</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="14"/>
@@ -3518,14 +3532,14 @@
       <c r="Q21" s="16"/>
       <c r="R21" s="16"/>
       <c r="S21" s="17"/>
-      <c r="T21" s="51"/>
-      <c r="U21" s="52"/>
-      <c r="V21" s="52"/>
-      <c r="W21" s="52"/>
-      <c r="X21" s="52"/>
-      <c r="Y21" s="52"/>
-      <c r="Z21" s="52"/>
-      <c r="AA21" s="53"/>
+      <c r="T21" s="62"/>
+      <c r="U21" s="63"/>
+      <c r="V21" s="63"/>
+      <c r="W21" s="63"/>
+      <c r="X21" s="63"/>
+      <c r="Y21" s="63"/>
+      <c r="Z21" s="63"/>
+      <c r="AA21" s="64"/>
       <c r="AB21" s="15"/>
       <c r="AC21" s="16"/>
       <c r="AD21" s="16"/>
@@ -3553,11 +3567,11 @@
       <c r="AZ21" s="15"/>
       <c r="BA21" s="16"/>
       <c r="BB21" s="16"/>
-      <c r="BC21" s="16"/>
-      <c r="BD21" s="16"/>
-      <c r="BE21" s="16"/>
-      <c r="BF21" s="16"/>
-      <c r="BG21" s="17"/>
+      <c r="BC21" s="32"/>
+      <c r="BD21" s="32"/>
+      <c r="BE21" s="32"/>
+      <c r="BF21" s="32"/>
+      <c r="BG21" s="32"/>
       <c r="BH21" s="15"/>
       <c r="BI21" s="16"/>
       <c r="BJ21" s="16"/>
@@ -3582,11 +3596,11 @@
       <c r="CC21" s="16"/>
       <c r="CD21" s="16"/>
       <c r="CE21" s="17"/>
-      <c r="CF21" s="44"/>
+      <c r="CF21" s="55"/>
     </row>
-    <row r="22" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>27</v>
+    <row r="22" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A22" s="68" t="s">
+        <v>34</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="14"/>
@@ -3606,14 +3620,14 @@
       <c r="Q22" s="16"/>
       <c r="R22" s="16"/>
       <c r="S22" s="17"/>
-      <c r="T22" s="51"/>
-      <c r="U22" s="52"/>
-      <c r="V22" s="52"/>
-      <c r="W22" s="52"/>
-      <c r="X22" s="52"/>
-      <c r="Y22" s="52"/>
-      <c r="Z22" s="52"/>
-      <c r="AA22" s="53"/>
+      <c r="T22" s="62"/>
+      <c r="U22" s="63"/>
+      <c r="V22" s="63"/>
+      <c r="W22" s="63"/>
+      <c r="X22" s="63"/>
+      <c r="Y22" s="63"/>
+      <c r="Z22" s="63"/>
+      <c r="AA22" s="64"/>
       <c r="AB22" s="15"/>
       <c r="AC22" s="16"/>
       <c r="AD22" s="16"/>
@@ -3658,10 +3672,10 @@
       <c r="BQ22" s="16"/>
       <c r="BR22" s="16"/>
       <c r="BS22" s="16"/>
-      <c r="BT22" s="16"/>
-      <c r="BU22" s="16"/>
-      <c r="BV22" s="16"/>
-      <c r="BW22" s="17"/>
+      <c r="BT22" s="37"/>
+      <c r="BU22" s="37"/>
+      <c r="BV22" s="37"/>
+      <c r="BW22" s="38"/>
       <c r="BX22" s="15"/>
       <c r="BY22" s="16"/>
       <c r="BZ22" s="16"/>
@@ -3670,11 +3684,11 @@
       <c r="CC22" s="16"/>
       <c r="CD22" s="16"/>
       <c r="CE22" s="17"/>
-      <c r="CF22" s="44"/>
+      <c r="CF22" s="55"/>
     </row>
-    <row r="23" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A23" s="13" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B23" s="24"/>
       <c r="C23" s="14"/>
@@ -3694,14 +3708,14 @@
       <c r="Q23" s="16"/>
       <c r="R23" s="16"/>
       <c r="S23" s="17"/>
-      <c r="T23" s="51"/>
-      <c r="U23" s="52"/>
-      <c r="V23" s="52"/>
-      <c r="W23" s="52"/>
-      <c r="X23" s="52"/>
-      <c r="Y23" s="52"/>
-      <c r="Z23" s="52"/>
-      <c r="AA23" s="53"/>
+      <c r="T23" s="62"/>
+      <c r="U23" s="63"/>
+      <c r="V23" s="63"/>
+      <c r="W23" s="63"/>
+      <c r="X23" s="63"/>
+      <c r="Y23" s="63"/>
+      <c r="Z23" s="63"/>
+      <c r="AA23" s="64"/>
       <c r="AB23" s="15"/>
       <c r="AC23" s="16"/>
       <c r="AD23" s="16"/>
@@ -3746,10 +3760,10 @@
       <c r="BQ23" s="16"/>
       <c r="BR23" s="16"/>
       <c r="BS23" s="16"/>
-      <c r="BT23" s="16"/>
-      <c r="BU23" s="16"/>
-      <c r="BV23" s="16"/>
-      <c r="BW23" s="17"/>
+      <c r="BT23" s="37"/>
+      <c r="BU23" s="37"/>
+      <c r="BV23" s="37"/>
+      <c r="BW23" s="38"/>
       <c r="BX23" s="15"/>
       <c r="BY23" s="16"/>
       <c r="BZ23" s="16"/>
@@ -3758,100 +3772,97 @@
       <c r="CC23" s="16"/>
       <c r="CD23" s="16"/>
       <c r="CE23" s="17"/>
-      <c r="CF23" s="44"/>
+      <c r="CF23" s="55"/>
     </row>
-    <row r="24" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="14"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="51"/>
-      <c r="U24" s="52"/>
-      <c r="V24" s="52"/>
-      <c r="W24" s="52"/>
-      <c r="X24" s="52"/>
-      <c r="Y24" s="52"/>
-      <c r="Z24" s="52"/>
-      <c r="AA24" s="53"/>
-      <c r="AB24" s="15"/>
-      <c r="AC24" s="16"/>
-      <c r="AD24" s="16"/>
-      <c r="AE24" s="16"/>
-      <c r="AF24" s="16"/>
-      <c r="AG24" s="16"/>
-      <c r="AH24" s="16"/>
-      <c r="AI24" s="17"/>
-      <c r="AJ24" s="15"/>
-      <c r="AK24" s="16"/>
-      <c r="AL24" s="16"/>
-      <c r="AM24" s="16"/>
-      <c r="AN24" s="16"/>
-      <c r="AO24" s="16"/>
-      <c r="AP24" s="16"/>
-      <c r="AQ24" s="17"/>
-      <c r="AR24" s="15"/>
-      <c r="AS24" s="16"/>
-      <c r="AT24" s="16"/>
-      <c r="AU24" s="16"/>
-      <c r="AV24" s="16"/>
-      <c r="AW24" s="16"/>
-      <c r="AX24" s="16"/>
-      <c r="AY24" s="17"/>
-      <c r="AZ24" s="15"/>
-      <c r="BA24" s="16"/>
-      <c r="BB24" s="16"/>
-      <c r="BC24" s="16"/>
-      <c r="BD24" s="16"/>
-      <c r="BE24" s="16"/>
-      <c r="BF24" s="16"/>
-      <c r="BG24" s="17"/>
-      <c r="BH24" s="15"/>
-      <c r="BI24" s="16"/>
-      <c r="BJ24" s="16"/>
-      <c r="BK24" s="16"/>
-      <c r="BL24" s="16"/>
-      <c r="BM24" s="16"/>
-      <c r="BN24" s="16"/>
-      <c r="BO24" s="17"/>
-      <c r="BP24" s="15"/>
-      <c r="BQ24" s="16"/>
-      <c r="BR24" s="16"/>
-      <c r="BS24" s="16"/>
-      <c r="BT24" s="16"/>
-      <c r="BU24" s="16"/>
-      <c r="BV24" s="16"/>
-      <c r="BW24" s="17"/>
-      <c r="BX24" s="15"/>
-      <c r="BY24" s="16"/>
-      <c r="BZ24" s="16"/>
-      <c r="CA24" s="16"/>
-      <c r="CB24" s="16"/>
-      <c r="CC24" s="16"/>
-      <c r="CD24" s="16"/>
-      <c r="CE24" s="17"/>
-      <c r="CF24" s="44"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="62"/>
+      <c r="U24" s="63"/>
+      <c r="V24" s="63"/>
+      <c r="W24" s="63"/>
+      <c r="X24" s="63"/>
+      <c r="Y24" s="63"/>
+      <c r="Z24" s="63"/>
+      <c r="AA24" s="64"/>
+      <c r="AB24" s="36"/>
+      <c r="AC24" s="37"/>
+      <c r="AD24" s="37"/>
+      <c r="AE24" s="37"/>
+      <c r="AF24" s="37"/>
+      <c r="AG24" s="37"/>
+      <c r="AH24" s="37"/>
+      <c r="AI24" s="38"/>
+      <c r="AJ24" s="36"/>
+      <c r="AK24" s="37"/>
+      <c r="AL24" s="37"/>
+      <c r="AM24" s="37"/>
+      <c r="AN24" s="37"/>
+      <c r="AO24" s="37"/>
+      <c r="AP24" s="37"/>
+      <c r="AQ24" s="38"/>
+      <c r="AR24" s="36"/>
+      <c r="AS24" s="37"/>
+      <c r="AT24" s="37"/>
+      <c r="AU24" s="37"/>
+      <c r="AV24" s="37"/>
+      <c r="AW24" s="37"/>
+      <c r="AX24" s="37"/>
+      <c r="AY24" s="38"/>
+      <c r="AZ24" s="36"/>
+      <c r="BA24" s="37"/>
+      <c r="BB24" s="37"/>
+      <c r="BC24" s="37"/>
+      <c r="BD24" s="37"/>
+      <c r="BE24" s="37"/>
+      <c r="BF24" s="37"/>
+      <c r="BG24" s="38"/>
+      <c r="BH24" s="36"/>
+      <c r="BI24" s="37"/>
+      <c r="BJ24" s="37"/>
+      <c r="BK24" s="37"/>
+      <c r="BL24" s="37"/>
+      <c r="BM24" s="37"/>
+      <c r="BN24" s="37"/>
+      <c r="BO24" s="38"/>
+      <c r="BP24" s="36"/>
+      <c r="BQ24" s="37"/>
+      <c r="BR24" s="37"/>
+      <c r="BS24" s="37"/>
+      <c r="BT24" s="37"/>
+      <c r="BU24" s="37"/>
+      <c r="BV24" s="37"/>
+      <c r="BW24" s="38"/>
+      <c r="BX24" s="36"/>
+      <c r="BY24" s="37"/>
+      <c r="BZ24" s="37"/>
+      <c r="CA24" s="37"/>
+      <c r="CB24" s="37"/>
+      <c r="CC24" s="37"/>
+      <c r="CD24" s="37"/>
+      <c r="CE24" s="38"/>
+      <c r="CF24" s="55"/>
     </row>
-    <row r="25" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>30</v>
-      </c>
+    <row r="25" spans="1:84" x14ac:dyDescent="0.15">
       <c r="B25" s="24"/>
       <c r="C25" s="14"/>
       <c r="D25" s="15"/>
@@ -3870,14 +3881,14 @@
       <c r="Q25" s="16"/>
       <c r="R25" s="16"/>
       <c r="S25" s="17"/>
-      <c r="T25" s="51"/>
-      <c r="U25" s="52"/>
-      <c r="V25" s="52"/>
-      <c r="W25" s="52"/>
-      <c r="X25" s="52"/>
-      <c r="Y25" s="52"/>
-      <c r="Z25" s="52"/>
-      <c r="AA25" s="53"/>
+      <c r="T25" s="62"/>
+      <c r="U25" s="63"/>
+      <c r="V25" s="63"/>
+      <c r="W25" s="63"/>
+      <c r="X25" s="63"/>
+      <c r="Y25" s="63"/>
+      <c r="Z25" s="63"/>
+      <c r="AA25" s="64"/>
       <c r="AB25" s="15"/>
       <c r="AC25" s="16"/>
       <c r="AD25" s="16"/>
@@ -3934,12 +3945,10 @@
       <c r="CC25" s="16"/>
       <c r="CD25" s="16"/>
       <c r="CE25" s="17"/>
-      <c r="CF25" s="44"/>
+      <c r="CF25" s="55"/>
     </row>
-    <row r="26" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>31</v>
-      </c>
+    <row r="26" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A26" s="13"/>
       <c r="B26" s="24"/>
       <c r="C26" s="14"/>
       <c r="D26" s="15"/>
@@ -3958,14 +3967,14 @@
       <c r="Q26" s="16"/>
       <c r="R26" s="16"/>
       <c r="S26" s="17"/>
-      <c r="T26" s="51"/>
-      <c r="U26" s="52"/>
-      <c r="V26" s="52"/>
-      <c r="W26" s="52"/>
-      <c r="X26" s="52"/>
-      <c r="Y26" s="52"/>
-      <c r="Z26" s="52"/>
-      <c r="AA26" s="53"/>
+      <c r="T26" s="62"/>
+      <c r="U26" s="63"/>
+      <c r="V26" s="63"/>
+      <c r="W26" s="63"/>
+      <c r="X26" s="63"/>
+      <c r="Y26" s="63"/>
+      <c r="Z26" s="63"/>
+      <c r="AA26" s="64"/>
       <c r="AB26" s="15"/>
       <c r="AC26" s="16"/>
       <c r="AD26" s="16"/>
@@ -4022,12 +4031,10 @@
       <c r="CC26" s="16"/>
       <c r="CD26" s="16"/>
       <c r="CE26" s="17"/>
-      <c r="CF26" s="44"/>
+      <c r="CF26" s="55"/>
     </row>
-    <row r="27" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>32</v>
-      </c>
+    <row r="27" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A27" s="13"/>
       <c r="B27" s="24"/>
       <c r="C27" s="14"/>
       <c r="D27" s="15"/>
@@ -4046,14 +4053,14 @@
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
       <c r="S27" s="17"/>
-      <c r="T27" s="51"/>
-      <c r="U27" s="52"/>
-      <c r="V27" s="52"/>
-      <c r="W27" s="52"/>
-      <c r="X27" s="52"/>
-      <c r="Y27" s="52"/>
-      <c r="Z27" s="52"/>
-      <c r="AA27" s="53"/>
+      <c r="T27" s="62"/>
+      <c r="U27" s="63"/>
+      <c r="V27" s="63"/>
+      <c r="W27" s="63"/>
+      <c r="X27" s="63"/>
+      <c r="Y27" s="63"/>
+      <c r="Z27" s="63"/>
+      <c r="AA27" s="64"/>
       <c r="AB27" s="15"/>
       <c r="AC27" s="16"/>
       <c r="AD27" s="16"/>
@@ -4110,912 +4117,215 @@
       <c r="CC27" s="16"/>
       <c r="CD27" s="16"/>
       <c r="CE27" s="17"/>
-      <c r="CF27" s="44"/>
+      <c r="CF27" s="55"/>
     </row>
-    <row r="28" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="17"/>
-      <c r="T28" s="51"/>
-      <c r="U28" s="52"/>
-      <c r="V28" s="52"/>
-      <c r="W28" s="52"/>
-      <c r="X28" s="52"/>
-      <c r="Y28" s="52"/>
-      <c r="Z28" s="52"/>
-      <c r="AA28" s="53"/>
-      <c r="AB28" s="15"/>
-      <c r="AC28" s="16"/>
-      <c r="AD28" s="16"/>
-      <c r="AE28" s="16"/>
-      <c r="AF28" s="16"/>
-      <c r="AG28" s="16"/>
-      <c r="AH28" s="16"/>
-      <c r="AI28" s="17"/>
-      <c r="AJ28" s="15"/>
-      <c r="AK28" s="16"/>
-      <c r="AL28" s="16"/>
-      <c r="AM28" s="16"/>
-      <c r="AN28" s="16"/>
-      <c r="AO28" s="16"/>
-      <c r="AP28" s="16"/>
-      <c r="AQ28" s="17"/>
-      <c r="AR28" s="15"/>
-      <c r="AS28" s="16"/>
-      <c r="AT28" s="16"/>
-      <c r="AU28" s="16"/>
-      <c r="AV28" s="16"/>
-      <c r="AW28" s="16"/>
-      <c r="AX28" s="16"/>
-      <c r="AY28" s="17"/>
-      <c r="AZ28" s="15"/>
-      <c r="BA28" s="16"/>
-      <c r="BB28" s="16"/>
-      <c r="BC28" s="16"/>
-      <c r="BD28" s="16"/>
-      <c r="BE28" s="16"/>
-      <c r="BF28" s="16"/>
-      <c r="BG28" s="17"/>
-      <c r="BH28" s="15"/>
-      <c r="BI28" s="16"/>
-      <c r="BJ28" s="16"/>
-      <c r="BK28" s="16"/>
-      <c r="BL28" s="16"/>
-      <c r="BM28" s="16"/>
-      <c r="BN28" s="16"/>
-      <c r="BO28" s="17"/>
-      <c r="BP28" s="15"/>
-      <c r="BQ28" s="16"/>
-      <c r="BR28" s="16"/>
-      <c r="BS28" s="16"/>
-      <c r="BT28" s="16"/>
-      <c r="BU28" s="16"/>
-      <c r="BV28" s="16"/>
-      <c r="BW28" s="17"/>
-      <c r="BX28" s="15"/>
-      <c r="BY28" s="16"/>
-      <c r="BZ28" s="16"/>
-      <c r="CA28" s="16"/>
-      <c r="CB28" s="16"/>
-      <c r="CC28" s="16"/>
-      <c r="CD28" s="16"/>
-      <c r="CE28" s="17"/>
-      <c r="CF28" s="44"/>
+    <row r="28" spans="1:84" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="18"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="65"/>
+      <c r="U28" s="66"/>
+      <c r="V28" s="66"/>
+      <c r="W28" s="66"/>
+      <c r="X28" s="66"/>
+      <c r="Y28" s="66"/>
+      <c r="Z28" s="66"/>
+      <c r="AA28" s="67"/>
+      <c r="AB28" s="20"/>
+      <c r="AC28" s="21"/>
+      <c r="AD28" s="21"/>
+      <c r="AE28" s="21"/>
+      <c r="AF28" s="21"/>
+      <c r="AG28" s="21"/>
+      <c r="AH28" s="21"/>
+      <c r="AI28" s="22"/>
+      <c r="AJ28" s="20"/>
+      <c r="AK28" s="21"/>
+      <c r="AL28" s="21"/>
+      <c r="AM28" s="21"/>
+      <c r="AN28" s="21"/>
+      <c r="AO28" s="21"/>
+      <c r="AP28" s="21"/>
+      <c r="AQ28" s="22"/>
+      <c r="AR28" s="20"/>
+      <c r="AS28" s="21"/>
+      <c r="AT28" s="21"/>
+      <c r="AU28" s="21"/>
+      <c r="AV28" s="21"/>
+      <c r="AW28" s="21"/>
+      <c r="AX28" s="21"/>
+      <c r="AY28" s="22"/>
+      <c r="AZ28" s="20"/>
+      <c r="BA28" s="21"/>
+      <c r="BB28" s="21"/>
+      <c r="BC28" s="21"/>
+      <c r="BD28" s="21"/>
+      <c r="BE28" s="21"/>
+      <c r="BF28" s="21"/>
+      <c r="BG28" s="22"/>
+      <c r="BH28" s="20"/>
+      <c r="BI28" s="21"/>
+      <c r="BJ28" s="21"/>
+      <c r="BK28" s="21"/>
+      <c r="BL28" s="21"/>
+      <c r="BM28" s="21"/>
+      <c r="BN28" s="21"/>
+      <c r="BO28" s="22"/>
+      <c r="BP28" s="20"/>
+      <c r="BQ28" s="21"/>
+      <c r="BR28" s="21"/>
+      <c r="BS28" s="21"/>
+      <c r="BT28" s="21"/>
+      <c r="BU28" s="21"/>
+      <c r="BV28" s="21"/>
+      <c r="BW28" s="22"/>
+      <c r="BX28" s="20"/>
+      <c r="BY28" s="21"/>
+      <c r="BZ28" s="21"/>
+      <c r="CA28" s="21"/>
+      <c r="CB28" s="21"/>
+      <c r="CC28" s="21"/>
+      <c r="CD28" s="21"/>
+      <c r="CE28" s="22"/>
+      <c r="CF28" s="55"/>
     </row>
-    <row r="29" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="17"/>
-      <c r="T29" s="51"/>
-      <c r="U29" s="52"/>
-      <c r="V29" s="52"/>
-      <c r="W29" s="52"/>
-      <c r="X29" s="52"/>
-      <c r="Y29" s="52"/>
-      <c r="Z29" s="52"/>
-      <c r="AA29" s="53"/>
-      <c r="AB29" s="15"/>
-      <c r="AC29" s="16"/>
-      <c r="AD29" s="16"/>
-      <c r="AE29" s="16"/>
-      <c r="AF29" s="16"/>
-      <c r="AG29" s="16"/>
-      <c r="AH29" s="16"/>
-      <c r="AI29" s="17"/>
-      <c r="AJ29" s="15"/>
-      <c r="AK29" s="16"/>
-      <c r="AL29" s="16"/>
-      <c r="AM29" s="16"/>
-      <c r="AN29" s="16"/>
-      <c r="AO29" s="16"/>
-      <c r="AP29" s="16"/>
-      <c r="AQ29" s="17"/>
-      <c r="AR29" s="15"/>
-      <c r="AS29" s="16"/>
-      <c r="AT29" s="16"/>
-      <c r="AU29" s="16"/>
-      <c r="AV29" s="16"/>
-      <c r="AW29" s="16"/>
-      <c r="AX29" s="16"/>
-      <c r="AY29" s="17"/>
-      <c r="AZ29" s="15"/>
-      <c r="BA29" s="16"/>
-      <c r="BB29" s="16"/>
-      <c r="BC29" s="16"/>
-      <c r="BD29" s="16"/>
-      <c r="BE29" s="16"/>
-      <c r="BF29" s="16"/>
-      <c r="BG29" s="17"/>
-      <c r="BH29" s="15"/>
-      <c r="BI29" s="16"/>
-      <c r="BJ29" s="16"/>
-      <c r="BK29" s="16"/>
-      <c r="BL29" s="16"/>
-      <c r="BM29" s="16"/>
-      <c r="BN29" s="16"/>
-      <c r="BO29" s="17"/>
-      <c r="BP29" s="15"/>
-      <c r="BQ29" s="16"/>
-      <c r="BR29" s="16"/>
-      <c r="BS29" s="16"/>
-      <c r="BT29" s="16"/>
-      <c r="BU29" s="16"/>
-      <c r="BV29" s="16"/>
-      <c r="BW29" s="17"/>
-      <c r="BX29" s="15"/>
-      <c r="BY29" s="16"/>
-      <c r="BZ29" s="16"/>
-      <c r="CA29" s="16"/>
-      <c r="CB29" s="16"/>
-      <c r="CC29" s="16"/>
-      <c r="CD29" s="16"/>
-      <c r="CE29" s="17"/>
-      <c r="CF29" s="44"/>
+    <row r="29" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="A29" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="56"/>
+      <c r="S29" s="56"/>
+      <c r="T29" s="56"/>
+      <c r="U29" s="56"/>
+      <c r="V29" s="56"/>
+      <c r="W29" s="56"/>
+      <c r="X29" s="56"/>
+      <c r="Y29" s="56"/>
+      <c r="Z29" s="56"/>
+      <c r="AA29" s="56"/>
+      <c r="AB29" s="56"/>
+      <c r="AC29" s="56"/>
+      <c r="AD29" s="56"/>
+      <c r="AE29" s="56"/>
+      <c r="AF29" s="56"/>
+      <c r="AG29" s="56"/>
+      <c r="AH29" s="56"/>
+      <c r="AI29" s="56"/>
+      <c r="AJ29" s="56"/>
+      <c r="AK29" s="56"/>
+      <c r="AL29" s="56"/>
+      <c r="AM29" s="56"/>
+      <c r="AN29" s="56"/>
+      <c r="AO29" s="56"/>
+      <c r="AP29" s="56"/>
+      <c r="AQ29" s="56"/>
+      <c r="AR29" s="56"/>
+      <c r="AS29" s="56"/>
+      <c r="AT29" s="56"/>
+      <c r="AU29" s="56"/>
+      <c r="AV29" s="56"/>
+      <c r="AW29" s="56"/>
+      <c r="AX29" s="56"/>
+      <c r="AY29" s="56"/>
+      <c r="AZ29" s="56"/>
+      <c r="BA29" s="56"/>
+      <c r="BB29" s="56"/>
+      <c r="BC29" s="56"/>
+      <c r="BD29" s="56"/>
+      <c r="BE29" s="56"/>
+      <c r="BF29" s="56"/>
+      <c r="BG29" s="56"/>
+      <c r="BH29" s="56"/>
+      <c r="BI29" s="56"/>
+      <c r="BJ29" s="56"/>
+      <c r="BK29" s="56"/>
+      <c r="BL29" s="56"/>
+      <c r="BM29" s="56"/>
+      <c r="BN29" s="56"/>
+      <c r="BO29" s="56"/>
+      <c r="BP29" s="56"/>
+      <c r="BQ29" s="56"/>
+      <c r="BR29" s="56"/>
+      <c r="BS29" s="56"/>
+      <c r="BT29" s="56"/>
+      <c r="BU29" s="56"/>
+      <c r="BV29" s="56"/>
+      <c r="BW29" s="56"/>
+      <c r="BX29" s="56"/>
+      <c r="BY29" s="56"/>
+      <c r="BZ29" s="56"/>
+      <c r="CA29" s="56"/>
+      <c r="CB29" s="56"/>
+      <c r="CC29" s="56"/>
+      <c r="CD29" s="56"/>
+      <c r="CE29" s="56"/>
     </row>
-    <row r="30" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="17"/>
-      <c r="T30" s="51"/>
-      <c r="U30" s="52"/>
-      <c r="V30" s="52"/>
-      <c r="W30" s="52"/>
-      <c r="X30" s="52"/>
-      <c r="Y30" s="52"/>
-      <c r="Z30" s="52"/>
-      <c r="AA30" s="53"/>
-      <c r="AB30" s="15"/>
-      <c r="AC30" s="16"/>
-      <c r="AD30" s="16"/>
-      <c r="AE30" s="16"/>
-      <c r="AF30" s="16"/>
-      <c r="AG30" s="16"/>
-      <c r="AH30" s="16"/>
-      <c r="AI30" s="17"/>
-      <c r="AJ30" s="15"/>
-      <c r="AK30" s="16"/>
-      <c r="AL30" s="16"/>
-      <c r="AM30" s="16"/>
-      <c r="AN30" s="16"/>
-      <c r="AO30" s="16"/>
-      <c r="AP30" s="16"/>
-      <c r="AQ30" s="17"/>
-      <c r="AR30" s="15"/>
-      <c r="AS30" s="16"/>
-      <c r="AT30" s="16"/>
-      <c r="AU30" s="16"/>
-      <c r="AV30" s="16"/>
-      <c r="AW30" s="16"/>
-      <c r="AX30" s="16"/>
-      <c r="AY30" s="17"/>
-      <c r="AZ30" s="15"/>
-      <c r="BA30" s="16"/>
-      <c r="BB30" s="16"/>
-      <c r="BC30" s="16"/>
-      <c r="BD30" s="16"/>
-      <c r="BE30" s="16"/>
-      <c r="BF30" s="16"/>
-      <c r="BG30" s="17"/>
-      <c r="BH30" s="15"/>
-      <c r="BI30" s="16"/>
-      <c r="BJ30" s="16"/>
-      <c r="BK30" s="16"/>
-      <c r="BL30" s="16"/>
-      <c r="BM30" s="16"/>
-      <c r="BN30" s="16"/>
-      <c r="BO30" s="17"/>
-      <c r="BP30" s="15"/>
-      <c r="BQ30" s="16"/>
-      <c r="BR30" s="16"/>
-      <c r="BS30" s="16"/>
-      <c r="BT30" s="16"/>
-      <c r="BU30" s="16"/>
-      <c r="BV30" s="16"/>
-      <c r="BW30" s="17"/>
-      <c r="BX30" s="15"/>
-      <c r="BY30" s="16"/>
-      <c r="BZ30" s="16"/>
-      <c r="CA30" s="16"/>
-      <c r="CB30" s="16"/>
-      <c r="CC30" s="16"/>
-      <c r="CD30" s="16"/>
-      <c r="CE30" s="17"/>
-      <c r="CF30" s="44"/>
+    <row r="32" spans="1:84" x14ac:dyDescent="0.15">
+      <c r="B32" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="40"/>
     </row>
-    <row r="31" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16"/>
-      <c r="S31" s="17"/>
-      <c r="T31" s="51"/>
-      <c r="U31" s="52"/>
-      <c r="V31" s="52"/>
-      <c r="W31" s="52"/>
-      <c r="X31" s="52"/>
-      <c r="Y31" s="52"/>
-      <c r="Z31" s="52"/>
-      <c r="AA31" s="53"/>
-      <c r="AB31" s="15"/>
-      <c r="AC31" s="16"/>
-      <c r="AD31" s="16"/>
-      <c r="AE31" s="16"/>
-      <c r="AF31" s="16"/>
-      <c r="AG31" s="16"/>
-      <c r="AH31" s="16"/>
-      <c r="AI31" s="17"/>
-      <c r="AJ31" s="15"/>
-      <c r="AK31" s="16"/>
-      <c r="AL31" s="16"/>
-      <c r="AM31" s="16"/>
-      <c r="AN31" s="16"/>
-      <c r="AO31" s="16"/>
-      <c r="AP31" s="16"/>
-      <c r="AQ31" s="17"/>
-      <c r="AR31" s="15"/>
-      <c r="AS31" s="16"/>
-      <c r="AT31" s="16"/>
-      <c r="AU31" s="16"/>
-      <c r="AV31" s="16"/>
-      <c r="AW31" s="16"/>
-      <c r="AX31" s="16"/>
-      <c r="AY31" s="17"/>
-      <c r="AZ31" s="15"/>
-      <c r="BA31" s="16"/>
-      <c r="BB31" s="16"/>
-      <c r="BC31" s="16"/>
-      <c r="BD31" s="16"/>
-      <c r="BE31" s="16"/>
-      <c r="BF31" s="16"/>
-      <c r="BG31" s="17"/>
-      <c r="BH31" s="15"/>
-      <c r="BI31" s="16"/>
-      <c r="BJ31" s="16"/>
-      <c r="BK31" s="16"/>
-      <c r="BL31" s="16"/>
-      <c r="BM31" s="16"/>
-      <c r="BN31" s="16"/>
-      <c r="BO31" s="17"/>
-      <c r="BP31" s="15"/>
-      <c r="BQ31" s="16"/>
-      <c r="BR31" s="16"/>
-      <c r="BS31" s="16"/>
-      <c r="BT31" s="16"/>
-      <c r="BU31" s="16"/>
-      <c r="BV31" s="16"/>
-      <c r="BW31" s="17"/>
-      <c r="BX31" s="15"/>
-      <c r="BY31" s="16"/>
-      <c r="BZ31" s="16"/>
-      <c r="CA31" s="16"/>
-      <c r="CB31" s="16"/>
-      <c r="CC31" s="16"/>
-      <c r="CD31" s="16"/>
-      <c r="CE31" s="17"/>
-      <c r="CF31" s="44"/>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B33" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="41"/>
     </row>
-    <row r="32" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="34"/>
-      <c r="P32" s="34"/>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="34"/>
-      <c r="S32" s="35"/>
-      <c r="T32" s="51"/>
-      <c r="U32" s="52"/>
-      <c r="V32" s="52"/>
-      <c r="W32" s="52"/>
-      <c r="X32" s="52"/>
-      <c r="Y32" s="52"/>
-      <c r="Z32" s="52"/>
-      <c r="AA32" s="53"/>
-      <c r="AB32" s="36"/>
-      <c r="AC32" s="37"/>
-      <c r="AD32" s="37"/>
-      <c r="AE32" s="37"/>
-      <c r="AF32" s="37"/>
-      <c r="AG32" s="37"/>
-      <c r="AH32" s="37"/>
-      <c r="AI32" s="38"/>
-      <c r="AJ32" s="36"/>
-      <c r="AK32" s="37"/>
-      <c r="AL32" s="37"/>
-      <c r="AM32" s="37"/>
-      <c r="AN32" s="37"/>
-      <c r="AO32" s="37"/>
-      <c r="AP32" s="37"/>
-      <c r="AQ32" s="38"/>
-      <c r="AR32" s="36"/>
-      <c r="AS32" s="37"/>
-      <c r="AT32" s="37"/>
-      <c r="AU32" s="37"/>
-      <c r="AV32" s="37"/>
-      <c r="AW32" s="37"/>
-      <c r="AX32" s="37"/>
-      <c r="AY32" s="38"/>
-      <c r="AZ32" s="36"/>
-      <c r="BA32" s="37"/>
-      <c r="BB32" s="37"/>
-      <c r="BC32" s="37"/>
-      <c r="BD32" s="37"/>
-      <c r="BE32" s="37"/>
-      <c r="BF32" s="37"/>
-      <c r="BG32" s="38"/>
-      <c r="BH32" s="36"/>
-      <c r="BI32" s="37"/>
-      <c r="BJ32" s="37"/>
-      <c r="BK32" s="37"/>
-      <c r="BL32" s="37"/>
-      <c r="BM32" s="37"/>
-      <c r="BN32" s="37"/>
-      <c r="BO32" s="38"/>
-      <c r="BP32" s="36"/>
-      <c r="BQ32" s="37"/>
-      <c r="BR32" s="37"/>
-      <c r="BS32" s="37"/>
-      <c r="BT32" s="37"/>
-      <c r="BU32" s="37"/>
-      <c r="BV32" s="37"/>
-      <c r="BW32" s="38"/>
-      <c r="BX32" s="36"/>
-      <c r="BY32" s="37"/>
-      <c r="BZ32" s="37"/>
-      <c r="CA32" s="37"/>
-      <c r="CB32" s="37"/>
-      <c r="CC32" s="37"/>
-      <c r="CD32" s="37"/>
-      <c r="CE32" s="38"/>
-      <c r="CF32" s="44"/>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B34" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="42"/>
     </row>
-    <row r="33" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="17"/>
-      <c r="T33" s="51"/>
-      <c r="U33" s="52"/>
-      <c r="V33" s="52"/>
-      <c r="W33" s="52"/>
-      <c r="X33" s="52"/>
-      <c r="Y33" s="52"/>
-      <c r="Z33" s="52"/>
-      <c r="AA33" s="53"/>
-      <c r="AB33" s="15"/>
-      <c r="AC33" s="16"/>
-      <c r="AD33" s="16"/>
-      <c r="AE33" s="16"/>
-      <c r="AF33" s="16"/>
-      <c r="AG33" s="16"/>
-      <c r="AH33" s="16"/>
-      <c r="AI33" s="17"/>
-      <c r="AJ33" s="15"/>
-      <c r="AK33" s="16"/>
-      <c r="AL33" s="16"/>
-      <c r="AM33" s="16"/>
-      <c r="AN33" s="16"/>
-      <c r="AO33" s="16"/>
-      <c r="AP33" s="16"/>
-      <c r="AQ33" s="17"/>
-      <c r="AR33" s="15"/>
-      <c r="AS33" s="16"/>
-      <c r="AT33" s="16"/>
-      <c r="AU33" s="16"/>
-      <c r="AV33" s="16"/>
-      <c r="AW33" s="16"/>
-      <c r="AX33" s="16"/>
-      <c r="AY33" s="17"/>
-      <c r="AZ33" s="15"/>
-      <c r="BA33" s="16"/>
-      <c r="BB33" s="16"/>
-      <c r="BC33" s="16"/>
-      <c r="BD33" s="16"/>
-      <c r="BE33" s="16"/>
-      <c r="BF33" s="16"/>
-      <c r="BG33" s="17"/>
-      <c r="BH33" s="15"/>
-      <c r="BI33" s="16"/>
-      <c r="BJ33" s="16"/>
-      <c r="BK33" s="16"/>
-      <c r="BL33" s="16"/>
-      <c r="BM33" s="16"/>
-      <c r="BN33" s="16"/>
-      <c r="BO33" s="17"/>
-      <c r="BP33" s="15"/>
-      <c r="BQ33" s="16"/>
-      <c r="BR33" s="16"/>
-      <c r="BS33" s="16"/>
-      <c r="BT33" s="16"/>
-      <c r="BU33" s="16"/>
-      <c r="BV33" s="16"/>
-      <c r="BW33" s="17"/>
-      <c r="BX33" s="15"/>
-      <c r="BY33" s="16"/>
-      <c r="BZ33" s="16"/>
-      <c r="CA33" s="16"/>
-      <c r="CB33" s="16"/>
-      <c r="CC33" s="16"/>
-      <c r="CD33" s="16"/>
-      <c r="CE33" s="17"/>
-      <c r="CF33" s="44"/>
-    </row>
-    <row r="34" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="16"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="17"/>
-      <c r="T34" s="51"/>
-      <c r="U34" s="52"/>
-      <c r="V34" s="52"/>
-      <c r="W34" s="52"/>
-      <c r="X34" s="52"/>
-      <c r="Y34" s="52"/>
-      <c r="Z34" s="52"/>
-      <c r="AA34" s="53"/>
-      <c r="AB34" s="15"/>
-      <c r="AC34" s="16"/>
-      <c r="AD34" s="16"/>
-      <c r="AE34" s="16"/>
-      <c r="AF34" s="16"/>
-      <c r="AG34" s="16"/>
-      <c r="AH34" s="16"/>
-      <c r="AI34" s="17"/>
-      <c r="AJ34" s="15"/>
-      <c r="AK34" s="16"/>
-      <c r="AL34" s="16"/>
-      <c r="AM34" s="16"/>
-      <c r="AN34" s="16"/>
-      <c r="AO34" s="16"/>
-      <c r="AP34" s="16"/>
-      <c r="AQ34" s="17"/>
-      <c r="AR34" s="15"/>
-      <c r="AS34" s="16"/>
-      <c r="AT34" s="16"/>
-      <c r="AU34" s="16"/>
-      <c r="AV34" s="16"/>
-      <c r="AW34" s="16"/>
-      <c r="AX34" s="16"/>
-      <c r="AY34" s="17"/>
-      <c r="AZ34" s="15"/>
-      <c r="BA34" s="16"/>
-      <c r="BB34" s="16"/>
-      <c r="BC34" s="16"/>
-      <c r="BD34" s="16"/>
-      <c r="BE34" s="16"/>
-      <c r="BF34" s="16"/>
-      <c r="BG34" s="17"/>
-      <c r="BH34" s="15"/>
-      <c r="BI34" s="16"/>
-      <c r="BJ34" s="16"/>
-      <c r="BK34" s="16"/>
-      <c r="BL34" s="16"/>
-      <c r="BM34" s="16"/>
-      <c r="BN34" s="16"/>
-      <c r="BO34" s="17"/>
-      <c r="BP34" s="15"/>
-      <c r="BQ34" s="16"/>
-      <c r="BR34" s="16"/>
-      <c r="BS34" s="16"/>
-      <c r="BT34" s="16"/>
-      <c r="BU34" s="16"/>
-      <c r="BV34" s="16"/>
-      <c r="BW34" s="17"/>
-      <c r="BX34" s="15"/>
-      <c r="BY34" s="16"/>
-      <c r="BZ34" s="16"/>
-      <c r="CA34" s="16"/>
-      <c r="CB34" s="16"/>
-      <c r="CC34" s="16"/>
-      <c r="CD34" s="16"/>
-      <c r="CE34" s="17"/>
-      <c r="CF34" s="44"/>
-    </row>
-    <row r="35" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
-      <c r="O35" s="16"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="17"/>
-      <c r="T35" s="51"/>
-      <c r="U35" s="52"/>
-      <c r="V35" s="52"/>
-      <c r="W35" s="52"/>
-      <c r="X35" s="52"/>
-      <c r="Y35" s="52"/>
-      <c r="Z35" s="52"/>
-      <c r="AA35" s="53"/>
-      <c r="AB35" s="15"/>
-      <c r="AC35" s="16"/>
-      <c r="AD35" s="16"/>
-      <c r="AE35" s="16"/>
-      <c r="AF35" s="16"/>
-      <c r="AG35" s="16"/>
-      <c r="AH35" s="16"/>
-      <c r="AI35" s="17"/>
-      <c r="AJ35" s="15"/>
-      <c r="AK35" s="16"/>
-      <c r="AL35" s="16"/>
-      <c r="AM35" s="16"/>
-      <c r="AN35" s="16"/>
-      <c r="AO35" s="16"/>
-      <c r="AP35" s="16"/>
-      <c r="AQ35" s="17"/>
-      <c r="AR35" s="15"/>
-      <c r="AS35" s="16"/>
-      <c r="AT35" s="16"/>
-      <c r="AU35" s="16"/>
-      <c r="AV35" s="16"/>
-      <c r="AW35" s="16"/>
-      <c r="AX35" s="16"/>
-      <c r="AY35" s="17"/>
-      <c r="AZ35" s="15"/>
-      <c r="BA35" s="16"/>
-      <c r="BB35" s="16"/>
-      <c r="BC35" s="16"/>
-      <c r="BD35" s="16"/>
-      <c r="BE35" s="16"/>
-      <c r="BF35" s="16"/>
-      <c r="BG35" s="17"/>
-      <c r="BH35" s="15"/>
-      <c r="BI35" s="16"/>
-      <c r="BJ35" s="16"/>
-      <c r="BK35" s="16"/>
-      <c r="BL35" s="16"/>
-      <c r="BM35" s="16"/>
-      <c r="BN35" s="16"/>
-      <c r="BO35" s="17"/>
-      <c r="BP35" s="15"/>
-      <c r="BQ35" s="16"/>
-      <c r="BR35" s="16"/>
-      <c r="BS35" s="16"/>
-      <c r="BT35" s="16"/>
-      <c r="BU35" s="16"/>
-      <c r="BV35" s="16"/>
-      <c r="BW35" s="17"/>
-      <c r="BX35" s="15"/>
-      <c r="BY35" s="16"/>
-      <c r="BZ35" s="16"/>
-      <c r="CA35" s="16"/>
-      <c r="CB35" s="16"/>
-      <c r="CC35" s="16"/>
-      <c r="CD35" s="16"/>
-      <c r="CE35" s="17"/>
-      <c r="CF35" s="44"/>
-    </row>
-    <row r="36" spans="1:84" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="21"/>
-      <c r="O36" s="21"/>
-      <c r="P36" s="21"/>
-      <c r="Q36" s="21"/>
-      <c r="R36" s="21"/>
-      <c r="S36" s="22"/>
-      <c r="T36" s="54"/>
-      <c r="U36" s="55"/>
-      <c r="V36" s="55"/>
-      <c r="W36" s="55"/>
-      <c r="X36" s="55"/>
-      <c r="Y36" s="55"/>
-      <c r="Z36" s="55"/>
-      <c r="AA36" s="56"/>
-      <c r="AB36" s="20"/>
-      <c r="AC36" s="21"/>
-      <c r="AD36" s="21"/>
-      <c r="AE36" s="21"/>
-      <c r="AF36" s="21"/>
-      <c r="AG36" s="21"/>
-      <c r="AH36" s="21"/>
-      <c r="AI36" s="22"/>
-      <c r="AJ36" s="20"/>
-      <c r="AK36" s="21"/>
-      <c r="AL36" s="21"/>
-      <c r="AM36" s="21"/>
-      <c r="AN36" s="21"/>
-      <c r="AO36" s="21"/>
-      <c r="AP36" s="21"/>
-      <c r="AQ36" s="22"/>
-      <c r="AR36" s="20"/>
-      <c r="AS36" s="21"/>
-      <c r="AT36" s="21"/>
-      <c r="AU36" s="21"/>
-      <c r="AV36" s="21"/>
-      <c r="AW36" s="21"/>
-      <c r="AX36" s="21"/>
-      <c r="AY36" s="22"/>
-      <c r="AZ36" s="20"/>
-      <c r="BA36" s="21"/>
-      <c r="BB36" s="21"/>
-      <c r="BC36" s="21"/>
-      <c r="BD36" s="21"/>
-      <c r="BE36" s="21"/>
-      <c r="BF36" s="21"/>
-      <c r="BG36" s="22"/>
-      <c r="BH36" s="20"/>
-      <c r="BI36" s="21"/>
-      <c r="BJ36" s="21"/>
-      <c r="BK36" s="21"/>
-      <c r="BL36" s="21"/>
-      <c r="BM36" s="21"/>
-      <c r="BN36" s="21"/>
-      <c r="BO36" s="22"/>
-      <c r="BP36" s="20"/>
-      <c r="BQ36" s="21"/>
-      <c r="BR36" s="21"/>
-      <c r="BS36" s="21"/>
-      <c r="BT36" s="21"/>
-      <c r="BU36" s="21"/>
-      <c r="BV36" s="21"/>
-      <c r="BW36" s="22"/>
-      <c r="BX36" s="20"/>
-      <c r="BY36" s="21"/>
-      <c r="BZ36" s="21"/>
-      <c r="CA36" s="21"/>
-      <c r="CB36" s="21"/>
-      <c r="CC36" s="21"/>
-      <c r="CD36" s="21"/>
-      <c r="CE36" s="22"/>
-      <c r="CF36" s="44"/>
-    </row>
-    <row r="37" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A37" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="45"/>
-      <c r="R37" s="45"/>
-      <c r="S37" s="45"/>
-      <c r="T37" s="45"/>
-      <c r="U37" s="45"/>
-      <c r="V37" s="45"/>
-      <c r="W37" s="45"/>
-      <c r="X37" s="45"/>
-      <c r="Y37" s="45"/>
-      <c r="Z37" s="45"/>
-      <c r="AA37" s="45"/>
-      <c r="AB37" s="45"/>
-      <c r="AC37" s="45"/>
-      <c r="AD37" s="45"/>
-      <c r="AE37" s="45"/>
-      <c r="AF37" s="45"/>
-      <c r="AG37" s="45"/>
-      <c r="AH37" s="45"/>
-      <c r="AI37" s="45"/>
-      <c r="AJ37" s="45"/>
-      <c r="AK37" s="45"/>
-      <c r="AL37" s="45"/>
-      <c r="AM37" s="45"/>
-      <c r="AN37" s="45"/>
-      <c r="AO37" s="45"/>
-      <c r="AP37" s="45"/>
-      <c r="AQ37" s="45"/>
-      <c r="AR37" s="45"/>
-      <c r="AS37" s="45"/>
-      <c r="AT37" s="45"/>
-      <c r="AU37" s="45"/>
-      <c r="AV37" s="45"/>
-      <c r="AW37" s="45"/>
-      <c r="AX37" s="45"/>
-      <c r="AY37" s="45"/>
-      <c r="AZ37" s="45"/>
-      <c r="BA37" s="45"/>
-      <c r="BB37" s="45"/>
-      <c r="BC37" s="45"/>
-      <c r="BD37" s="45"/>
-      <c r="BE37" s="45"/>
-      <c r="BF37" s="45"/>
-      <c r="BG37" s="45"/>
-      <c r="BH37" s="45"/>
-      <c r="BI37" s="45"/>
-      <c r="BJ37" s="45"/>
-      <c r="BK37" s="45"/>
-      <c r="BL37" s="45"/>
-      <c r="BM37" s="45"/>
-      <c r="BN37" s="45"/>
-      <c r="BO37" s="45"/>
-      <c r="BP37" s="45"/>
-      <c r="BQ37" s="45"/>
-      <c r="BR37" s="45"/>
-      <c r="BS37" s="45"/>
-      <c r="BT37" s="45"/>
-      <c r="BU37" s="45"/>
-      <c r="BV37" s="45"/>
-      <c r="BW37" s="45"/>
-      <c r="BX37" s="45"/>
-      <c r="BY37" s="45"/>
-      <c r="BZ37" s="45"/>
-      <c r="CA37" s="45"/>
-      <c r="CB37" s="45"/>
-      <c r="CC37" s="45"/>
-      <c r="CD37" s="45"/>
-      <c r="CE37" s="45"/>
-    </row>
-    <row r="40" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="B40" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="40"/>
-    </row>
-    <row r="41" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="B41" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="41"/>
-    </row>
-    <row r="42" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="B42" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" s="42"/>
-    </row>
-    <row r="43" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="B43" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="43"/>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B35" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="T4:W4"/>
-    <mergeCell ref="X4:AA4"/>
-    <mergeCell ref="D2:AQ3"/>
+    <mergeCell ref="CF4:CF28"/>
+    <mergeCell ref="A29:CE29"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="T6:AA28"/>
+    <mergeCell ref="AZ4:BC4"/>
+    <mergeCell ref="BD4:BG4"/>
+    <mergeCell ref="BH4:BK4"/>
+    <mergeCell ref="BL4:BO4"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="AR2:CE3"/>
     <mergeCell ref="AJ4:AM4"/>
@@ -5031,30 +4341,19 @@
     <mergeCell ref="BP4:BS4"/>
     <mergeCell ref="BX4:CA4"/>
     <mergeCell ref="CB4:CE4"/>
-    <mergeCell ref="CF4:CF36"/>
-    <mergeCell ref="A37:CE37"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="T6:AA36"/>
-    <mergeCell ref="AZ4:BC4"/>
-    <mergeCell ref="BD4:BG4"/>
-    <mergeCell ref="BH4:BK4"/>
-    <mergeCell ref="BL4:BO4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="T4:W4"/>
+    <mergeCell ref="X4:AA4"/>
+    <mergeCell ref="D2:AQ3"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
-  <conditionalFormatting sqref="B6:B10">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Terminé">
+  <conditionalFormatting sqref="B6:B28">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",B6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B36">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",B13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -5086,6 +4385,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2041c0d2b30335279095007fcb0a9d7c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="56b9c1bb8339570eda07374d036e5caf" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -5298,29 +4606,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F2702F0-3EB0-496B-8166-A9BB237AECA6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
-    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E70815D-A53F-41E3-B87E-1E164A9F927C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5337,12 +4648,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
planning mis a jour
</commit_message>
<xml_diff>
--- a/documentation/3_2_Modele_PlanningLundiMardi.xlsx
+++ b/documentation/3_2_Modele_PlanningLundiMardi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11130"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/gabriel_beer_studentfr_ch/Documents/EMF/Informatique EMF/Troisième année/306/306project-G4/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:1_{9A30F631-669B-4B85-80D9-41CC652520C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C825F6B-FBEE-EF4A-A437-817D91B600B1}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="13_ncr:1_{9A30F631-669B-4B85-80D9-41CC652520C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B245B74-AD4F-9449-8935-6449324198AC}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-2180" windowWidth="38400" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Tâches</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>Terminé</t>
-  </si>
-  <si>
-    <t>En cours</t>
   </si>
   <si>
     <t>Cyril</t>
@@ -767,7 +764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -936,6 +933,109 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -944,118 +1044,10 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1110,8 +1102,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>93135</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>160867</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>148828</xdr:rowOff>
     </xdr:to>
@@ -1128,8 +1120,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4126178" y="702733"/>
-          <a:ext cx="911490" cy="5542095"/>
+          <a:off x="4507178" y="702733"/>
+          <a:ext cx="4535222" cy="4187428"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1187,7 +1179,197 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>8468</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>16936</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>160868</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4805D7BD-A81C-A4EF-3856-A24753972147}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="16200000">
+          <a:off x="11616268" y="2878666"/>
+          <a:ext cx="3869268" cy="177802"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00">
+            <a:alpha val="33820"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>V1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>154215</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180219</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>162683</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>159658</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4565EBD-C6F1-7D47-B5AA-60746F3017FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="16200000">
+          <a:off x="12655551" y="2819097"/>
+          <a:ext cx="3744082" cy="171754"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00">
+            <a:alpha val="33820"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>V2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>7258</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>6047</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>74</xdr:col>
+      <xdr:colOff>15726</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>166915</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37EFC46D-E4DC-D241-8214-5DC2773AF048}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="16200000">
+          <a:off x="14631308" y="2826354"/>
+          <a:ext cx="3744082" cy="171754"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00">
+            <a:alpha val="33820"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>V3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1562,11 +1744,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="94" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="O6" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="94" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="AG6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="A29:CE29"/>
+      <selection pane="bottomRight" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1581,18 +1763,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:84" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="A1" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1631,173 +1813,173 @@
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="52"/>
-      <c r="AA2" s="52"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="52"/>
-      <c r="AD2" s="52"/>
-      <c r="AE2" s="52"/>
-      <c r="AF2" s="52"/>
-      <c r="AG2" s="52"/>
-      <c r="AH2" s="52"/>
-      <c r="AI2" s="52"/>
-      <c r="AJ2" s="52"/>
-      <c r="AK2" s="52"/>
-      <c r="AL2" s="52"/>
-      <c r="AM2" s="52"/>
-      <c r="AN2" s="52"/>
-      <c r="AO2" s="52"/>
-      <c r="AP2" s="52"/>
-      <c r="AQ2" s="52"/>
-      <c r="AR2" s="52"/>
-      <c r="AS2" s="52"/>
-      <c r="AT2" s="52"/>
-      <c r="AU2" s="52"/>
-      <c r="AV2" s="52"/>
-      <c r="AW2" s="52"/>
-      <c r="AX2" s="52"/>
-      <c r="AY2" s="52"/>
-      <c r="AZ2" s="52"/>
-      <c r="BA2" s="52"/>
-      <c r="BB2" s="52"/>
-      <c r="BC2" s="52"/>
-      <c r="BD2" s="52"/>
-      <c r="BE2" s="52"/>
-      <c r="BF2" s="52"/>
-      <c r="BG2" s="52"/>
-      <c r="BH2" s="52"/>
-      <c r="BI2" s="52"/>
-      <c r="BJ2" s="52"/>
-      <c r="BK2" s="52"/>
-      <c r="BL2" s="52"/>
-      <c r="BM2" s="52"/>
-      <c r="BN2" s="52"/>
-      <c r="BO2" s="52"/>
-      <c r="BP2" s="52"/>
-      <c r="BQ2" s="52"/>
-      <c r="BR2" s="52"/>
-      <c r="BS2" s="52"/>
-      <c r="BT2" s="52"/>
-      <c r="BU2" s="52"/>
-      <c r="BV2" s="52"/>
-      <c r="BW2" s="52"/>
-      <c r="BX2" s="52"/>
-      <c r="BY2" s="52"/>
-      <c r="BZ2" s="52"/>
-      <c r="CA2" s="52"/>
-      <c r="CB2" s="52"/>
-      <c r="CC2" s="52"/>
-      <c r="CD2" s="52"/>
-      <c r="CE2" s="52"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="70"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="70"/>
+      <c r="AF2" s="70"/>
+      <c r="AG2" s="70"/>
+      <c r="AH2" s="70"/>
+      <c r="AI2" s="70"/>
+      <c r="AJ2" s="70"/>
+      <c r="AK2" s="70"/>
+      <c r="AL2" s="70"/>
+      <c r="AM2" s="70"/>
+      <c r="AN2" s="70"/>
+      <c r="AO2" s="70"/>
+      <c r="AP2" s="70"/>
+      <c r="AQ2" s="70"/>
+      <c r="AR2" s="70"/>
+      <c r="AS2" s="70"/>
+      <c r="AT2" s="70"/>
+      <c r="AU2" s="70"/>
+      <c r="AV2" s="70"/>
+      <c r="AW2" s="70"/>
+      <c r="AX2" s="70"/>
+      <c r="AY2" s="70"/>
+      <c r="AZ2" s="70"/>
+      <c r="BA2" s="70"/>
+      <c r="BB2" s="70"/>
+      <c r="BC2" s="70"/>
+      <c r="BD2" s="70"/>
+      <c r="BE2" s="70"/>
+      <c r="BF2" s="70"/>
+      <c r="BG2" s="70"/>
+      <c r="BH2" s="70"/>
+      <c r="BI2" s="70"/>
+      <c r="BJ2" s="70"/>
+      <c r="BK2" s="70"/>
+      <c r="BL2" s="70"/>
+      <c r="BM2" s="70"/>
+      <c r="BN2" s="70"/>
+      <c r="BO2" s="70"/>
+      <c r="BP2" s="70"/>
+      <c r="BQ2" s="70"/>
+      <c r="BR2" s="70"/>
+      <c r="BS2" s="70"/>
+      <c r="BT2" s="70"/>
+      <c r="BU2" s="70"/>
+      <c r="BV2" s="70"/>
+      <c r="BW2" s="70"/>
+      <c r="BX2" s="70"/>
+      <c r="BY2" s="70"/>
+      <c r="BZ2" s="70"/>
+      <c r="CA2" s="70"/>
+      <c r="CB2" s="70"/>
+      <c r="CC2" s="70"/>
+      <c r="CD2" s="70"/>
+      <c r="CE2" s="70"/>
     </row>
     <row r="3" spans="1:84" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53"/>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="53"/>
-      <c r="AA3" s="53"/>
-      <c r="AB3" s="53"/>
-      <c r="AC3" s="53"/>
-      <c r="AD3" s="53"/>
-      <c r="AE3" s="53"/>
-      <c r="AF3" s="53"/>
-      <c r="AG3" s="53"/>
-      <c r="AH3" s="53"/>
-      <c r="AI3" s="53"/>
-      <c r="AJ3" s="53"/>
-      <c r="AK3" s="53"/>
-      <c r="AL3" s="53"/>
-      <c r="AM3" s="53"/>
-      <c r="AN3" s="53"/>
-      <c r="AO3" s="53"/>
-      <c r="AP3" s="53"/>
-      <c r="AQ3" s="53"/>
-      <c r="AR3" s="53"/>
-      <c r="AS3" s="53"/>
-      <c r="AT3" s="53"/>
-      <c r="AU3" s="53"/>
-      <c r="AV3" s="53"/>
-      <c r="AW3" s="53"/>
-      <c r="AX3" s="53"/>
-      <c r="AY3" s="53"/>
-      <c r="AZ3" s="53"/>
-      <c r="BA3" s="53"/>
-      <c r="BB3" s="53"/>
-      <c r="BC3" s="53"/>
-      <c r="BD3" s="53"/>
-      <c r="BE3" s="53"/>
-      <c r="BF3" s="53"/>
-      <c r="BG3" s="53"/>
-      <c r="BH3" s="53"/>
-      <c r="BI3" s="53"/>
-      <c r="BJ3" s="53"/>
-      <c r="BK3" s="53"/>
-      <c r="BL3" s="53"/>
-      <c r="BM3" s="53"/>
-      <c r="BN3" s="53"/>
-      <c r="BO3" s="53"/>
-      <c r="BP3" s="53"/>
-      <c r="BQ3" s="53"/>
-      <c r="BR3" s="53"/>
-      <c r="BS3" s="53"/>
-      <c r="BT3" s="53"/>
-      <c r="BU3" s="53"/>
-      <c r="BV3" s="53"/>
-      <c r="BW3" s="53"/>
-      <c r="BX3" s="53"/>
-      <c r="BY3" s="53"/>
-      <c r="BZ3" s="53"/>
-      <c r="CA3" s="53"/>
-      <c r="CB3" s="53"/>
-      <c r="CC3" s="53"/>
-      <c r="CD3" s="53"/>
-      <c r="CE3" s="53"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="71"/>
+      <c r="X3" s="71"/>
+      <c r="Y3" s="71"/>
+      <c r="Z3" s="71"/>
+      <c r="AA3" s="71"/>
+      <c r="AB3" s="71"/>
+      <c r="AC3" s="71"/>
+      <c r="AD3" s="71"/>
+      <c r="AE3" s="71"/>
+      <c r="AF3" s="71"/>
+      <c r="AG3" s="71"/>
+      <c r="AH3" s="71"/>
+      <c r="AI3" s="71"/>
+      <c r="AJ3" s="71"/>
+      <c r="AK3" s="71"/>
+      <c r="AL3" s="71"/>
+      <c r="AM3" s="71"/>
+      <c r="AN3" s="71"/>
+      <c r="AO3" s="71"/>
+      <c r="AP3" s="71"/>
+      <c r="AQ3" s="71"/>
+      <c r="AR3" s="71"/>
+      <c r="AS3" s="71"/>
+      <c r="AT3" s="71"/>
+      <c r="AU3" s="71"/>
+      <c r="AV3" s="71"/>
+      <c r="AW3" s="71"/>
+      <c r="AX3" s="71"/>
+      <c r="AY3" s="71"/>
+      <c r="AZ3" s="71"/>
+      <c r="BA3" s="71"/>
+      <c r="BB3" s="71"/>
+      <c r="BC3" s="71"/>
+      <c r="BD3" s="71"/>
+      <c r="BE3" s="71"/>
+      <c r="BF3" s="71"/>
+      <c r="BG3" s="71"/>
+      <c r="BH3" s="71"/>
+      <c r="BI3" s="71"/>
+      <c r="BJ3" s="71"/>
+      <c r="BK3" s="71"/>
+      <c r="BL3" s="71"/>
+      <c r="BM3" s="71"/>
+      <c r="BN3" s="71"/>
+      <c r="BO3" s="71"/>
+      <c r="BP3" s="71"/>
+      <c r="BQ3" s="71"/>
+      <c r="BR3" s="71"/>
+      <c r="BS3" s="71"/>
+      <c r="BT3" s="71"/>
+      <c r="BU3" s="71"/>
+      <c r="BV3" s="71"/>
+      <c r="BW3" s="71"/>
+      <c r="BX3" s="71"/>
+      <c r="BY3" s="71"/>
+      <c r="BZ3" s="71"/>
+      <c r="CA3" s="71"/>
+      <c r="CB3" s="71"/>
+      <c r="CC3" s="71"/>
+      <c r="CD3" s="71"/>
+      <c r="CE3" s="71"/>
     </row>
     <row r="4" spans="1:84" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="54" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="26" t="s">
@@ -1806,132 +1988,132 @@
       <c r="C4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="48">
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="67">
         <v>45992</v>
       </c>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="50" t="s">
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="48">
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="67">
         <v>45993</v>
       </c>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="50" t="s">
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="68"/>
+      <c r="T4" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="U4" s="51"/>
-      <c r="V4" s="51"/>
-      <c r="W4" s="51"/>
-      <c r="X4" s="48">
+      <c r="U4" s="66"/>
+      <c r="V4" s="66"/>
+      <c r="W4" s="66"/>
+      <c r="X4" s="67">
         <v>45999</v>
       </c>
-      <c r="Y4" s="48"/>
-      <c r="Z4" s="48"/>
-      <c r="AA4" s="49"/>
-      <c r="AB4" s="50" t="s">
+      <c r="Y4" s="67"/>
+      <c r="Z4" s="67"/>
+      <c r="AA4" s="68"/>
+      <c r="AB4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="AC4" s="51"/>
-      <c r="AD4" s="51"/>
-      <c r="AE4" s="51"/>
-      <c r="AF4" s="48">
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="66"/>
+      <c r="AE4" s="66"/>
+      <c r="AF4" s="67">
         <v>46000</v>
       </c>
-      <c r="AG4" s="48"/>
-      <c r="AH4" s="48"/>
-      <c r="AI4" s="49"/>
-      <c r="AJ4" s="50" t="s">
+      <c r="AG4" s="67"/>
+      <c r="AH4" s="67"/>
+      <c r="AI4" s="68"/>
+      <c r="AJ4" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="AK4" s="51"/>
-      <c r="AL4" s="51"/>
-      <c r="AM4" s="51"/>
-      <c r="AN4" s="48">
+      <c r="AK4" s="66"/>
+      <c r="AL4" s="66"/>
+      <c r="AM4" s="66"/>
+      <c r="AN4" s="67">
         <v>46006</v>
       </c>
-      <c r="AO4" s="48"/>
-      <c r="AP4" s="48"/>
-      <c r="AQ4" s="49"/>
-      <c r="AR4" s="50" t="s">
+      <c r="AO4" s="67"/>
+      <c r="AP4" s="67"/>
+      <c r="AQ4" s="68"/>
+      <c r="AR4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="AS4" s="51"/>
-      <c r="AT4" s="51"/>
-      <c r="AU4" s="51"/>
-      <c r="AV4" s="48">
+      <c r="AS4" s="66"/>
+      <c r="AT4" s="66"/>
+      <c r="AU4" s="66"/>
+      <c r="AV4" s="67">
         <v>46007</v>
       </c>
-      <c r="AW4" s="48"/>
-      <c r="AX4" s="48"/>
-      <c r="AY4" s="49"/>
-      <c r="AZ4" s="50" t="s">
+      <c r="AW4" s="67"/>
+      <c r="AX4" s="67"/>
+      <c r="AY4" s="68"/>
+      <c r="AZ4" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="BA4" s="51"/>
-      <c r="BB4" s="51"/>
-      <c r="BC4" s="51"/>
-      <c r="BD4" s="48">
+      <c r="BA4" s="66"/>
+      <c r="BB4" s="66"/>
+      <c r="BC4" s="66"/>
+      <c r="BD4" s="67">
         <v>46027</v>
       </c>
-      <c r="BE4" s="48"/>
-      <c r="BF4" s="48"/>
-      <c r="BG4" s="49"/>
-      <c r="BH4" s="50" t="s">
+      <c r="BE4" s="67"/>
+      <c r="BF4" s="67"/>
+      <c r="BG4" s="68"/>
+      <c r="BH4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="BI4" s="51"/>
-      <c r="BJ4" s="51"/>
-      <c r="BK4" s="51"/>
-      <c r="BL4" s="48">
+      <c r="BI4" s="66"/>
+      <c r="BJ4" s="66"/>
+      <c r="BK4" s="66"/>
+      <c r="BL4" s="67">
         <v>46028</v>
       </c>
-      <c r="BM4" s="48"/>
-      <c r="BN4" s="48"/>
-      <c r="BO4" s="49"/>
-      <c r="BP4" s="50" t="s">
+      <c r="BM4" s="67"/>
+      <c r="BN4" s="67"/>
+      <c r="BO4" s="68"/>
+      <c r="BP4" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="BQ4" s="51"/>
-      <c r="BR4" s="51"/>
-      <c r="BS4" s="51"/>
-      <c r="BT4" s="48">
+      <c r="BQ4" s="66"/>
+      <c r="BR4" s="66"/>
+      <c r="BS4" s="66"/>
+      <c r="BT4" s="67">
         <v>46034</v>
       </c>
-      <c r="BU4" s="48"/>
-      <c r="BV4" s="48"/>
-      <c r="BW4" s="49"/>
-      <c r="BX4" s="50" t="s">
+      <c r="BU4" s="67"/>
+      <c r="BV4" s="67"/>
+      <c r="BW4" s="68"/>
+      <c r="BX4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="BY4" s="51"/>
-      <c r="BZ4" s="51"/>
-      <c r="CA4" s="51"/>
-      <c r="CB4" s="48">
+      <c r="BY4" s="66"/>
+      <c r="BZ4" s="66"/>
+      <c r="CA4" s="66"/>
+      <c r="CB4" s="67">
         <v>46035</v>
       </c>
-      <c r="CC4" s="48"/>
-      <c r="CD4" s="48"/>
-      <c r="CE4" s="49"/>
-      <c r="CF4" s="55" t="s">
+      <c r="CC4" s="67"/>
+      <c r="CD4" s="67"/>
+      <c r="CE4" s="68"/>
+      <c r="CF4" s="52" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:84" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="58"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
@@ -2178,7 +2360,7 @@
       <c r="CE5" s="7">
         <v>8</v>
       </c>
-      <c r="CF5" s="55"/>
+      <c r="CF5" s="52"/>
     </row>
     <row r="6" spans="1:84" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
@@ -2204,16 +2386,16 @@
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
       <c r="S6" s="11"/>
-      <c r="T6" s="59" t="s">
+      <c r="T6" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="60"/>
-      <c r="V6" s="60"/>
-      <c r="W6" s="60"/>
-      <c r="X6" s="60"/>
-      <c r="Y6" s="60"/>
-      <c r="Z6" s="60"/>
-      <c r="AA6" s="61"/>
+      <c r="U6" s="57"/>
+      <c r="V6" s="57"/>
+      <c r="W6" s="57"/>
+      <c r="X6" s="57"/>
+      <c r="Y6" s="57"/>
+      <c r="Z6" s="57"/>
+      <c r="AA6" s="58"/>
       <c r="AB6" s="12"/>
       <c r="AC6" s="10"/>
       <c r="AD6" s="10"/>
@@ -2270,14 +2452,14 @@
       <c r="CC6" s="10"/>
       <c r="CD6" s="10"/>
       <c r="CE6" s="11"/>
-      <c r="CF6" s="55"/>
+      <c r="CF6" s="52"/>
     </row>
     <row r="7" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="15"/>
@@ -2296,14 +2478,14 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
       <c r="S7" s="17"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="63"/>
-      <c r="V7" s="63"/>
-      <c r="W7" s="63"/>
-      <c r="X7" s="63"/>
-      <c r="Y7" s="63"/>
-      <c r="Z7" s="63"/>
-      <c r="AA7" s="64"/>
+      <c r="T7" s="59"/>
+      <c r="U7" s="60"/>
+      <c r="V7" s="60"/>
+      <c r="W7" s="60"/>
+      <c r="X7" s="60"/>
+      <c r="Y7" s="60"/>
+      <c r="Z7" s="60"/>
+      <c r="AA7" s="61"/>
       <c r="AB7" s="15"/>
       <c r="AC7" s="16"/>
       <c r="AD7" s="16"/>
@@ -2360,7 +2542,7 @@
       <c r="CC7" s="16"/>
       <c r="CD7" s="16"/>
       <c r="CE7" s="17"/>
-      <c r="CF7" s="55"/>
+      <c r="CF7" s="52"/>
     </row>
     <row r="8" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
@@ -2386,14 +2568,14 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
       <c r="S8" s="17"/>
-      <c r="T8" s="62"/>
-      <c r="U8" s="63"/>
-      <c r="V8" s="63"/>
-      <c r="W8" s="63"/>
-      <c r="X8" s="63"/>
-      <c r="Y8" s="63"/>
-      <c r="Z8" s="63"/>
-      <c r="AA8" s="64"/>
+      <c r="T8" s="59"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="60"/>
+      <c r="W8" s="60"/>
+      <c r="X8" s="60"/>
+      <c r="Y8" s="60"/>
+      <c r="Z8" s="60"/>
+      <c r="AA8" s="61"/>
       <c r="AB8" s="15"/>
       <c r="AC8" s="16"/>
       <c r="AD8" s="16"/>
@@ -2450,13 +2632,15 @@
       <c r="CC8" s="16"/>
       <c r="CD8" s="16"/>
       <c r="CE8" s="17"/>
-      <c r="CF8" s="55"/>
+      <c r="CF8" s="52"/>
     </row>
     <row r="9" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="24"/>
+      <c r="B9" s="24" t="s">
+        <v>19</v>
+      </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
@@ -2474,14 +2658,14 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
       <c r="S9" s="17"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="63"/>
-      <c r="V9" s="63"/>
-      <c r="W9" s="63"/>
-      <c r="X9" s="63"/>
-      <c r="Y9" s="63"/>
-      <c r="Z9" s="63"/>
-      <c r="AA9" s="64"/>
+      <c r="T9" s="59"/>
+      <c r="U9" s="60"/>
+      <c r="V9" s="60"/>
+      <c r="W9" s="60"/>
+      <c r="X9" s="60"/>
+      <c r="Y9" s="60"/>
+      <c r="Z9" s="60"/>
+      <c r="AA9" s="61"/>
       <c r="AB9" s="15"/>
       <c r="AC9" s="16"/>
       <c r="AD9" s="16"/>
@@ -2538,11 +2722,11 @@
       <c r="CC9" s="16"/>
       <c r="CD9" s="16"/>
       <c r="CE9" s="17"/>
-      <c r="CF9" s="55"/>
+      <c r="CF9" s="52"/>
     </row>
     <row r="10" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A10" s="39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="24" t="s">
         <v>19</v>
@@ -2564,14 +2748,14 @@
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
       <c r="S10" s="17"/>
-      <c r="T10" s="62"/>
-      <c r="U10" s="63"/>
-      <c r="V10" s="63"/>
-      <c r="W10" s="63"/>
-      <c r="X10" s="63"/>
-      <c r="Y10" s="63"/>
-      <c r="Z10" s="63"/>
-      <c r="AA10" s="64"/>
+      <c r="T10" s="59"/>
+      <c r="U10" s="60"/>
+      <c r="V10" s="60"/>
+      <c r="W10" s="60"/>
+      <c r="X10" s="60"/>
+      <c r="Y10" s="60"/>
+      <c r="Z10" s="60"/>
+      <c r="AA10" s="61"/>
       <c r="AB10" s="15"/>
       <c r="AC10" s="16"/>
       <c r="AD10" s="16"/>
@@ -2628,11 +2812,11 @@
       <c r="CC10" s="16"/>
       <c r="CD10" s="16"/>
       <c r="CE10" s="17"/>
-      <c r="CF10" s="55"/>
+      <c r="CF10" s="52"/>
     </row>
     <row r="11" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A11" s="68" t="s">
-        <v>27</v>
+      <c r="A11" s="46" t="s">
+        <v>26</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="14"/>
@@ -2652,34 +2836,34 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
       <c r="S11" s="17"/>
-      <c r="T11" s="62"/>
-      <c r="U11" s="63"/>
-      <c r="V11" s="63"/>
-      <c r="W11" s="63"/>
-      <c r="X11" s="63"/>
-      <c r="Y11" s="63"/>
-      <c r="Z11" s="63"/>
-      <c r="AA11" s="64"/>
-      <c r="AB11" s="69"/>
-      <c r="AC11" s="69"/>
-      <c r="AD11" s="69"/>
-      <c r="AE11" s="69"/>
+      <c r="T11" s="59"/>
+      <c r="U11" s="60"/>
+      <c r="V11" s="60"/>
+      <c r="W11" s="60"/>
+      <c r="X11" s="60"/>
+      <c r="Y11" s="60"/>
+      <c r="Z11" s="60"/>
+      <c r="AA11" s="61"/>
+      <c r="AB11" s="47"/>
+      <c r="AC11" s="47"/>
+      <c r="AD11" s="47"/>
+      <c r="AE11" s="47"/>
       <c r="AF11" s="16"/>
       <c r="AG11" s="16"/>
       <c r="AH11" s="16"/>
       <c r="AI11" s="17"/>
-      <c r="AJ11" s="69"/>
-      <c r="AK11" s="69"/>
-      <c r="AL11" s="69"/>
-      <c r="AM11" s="69"/>
-      <c r="AN11" s="69"/>
-      <c r="AO11" s="69"/>
-      <c r="AP11" s="69"/>
-      <c r="AQ11" s="69"/>
-      <c r="AR11" s="69"/>
-      <c r="AS11" s="69"/>
-      <c r="AT11" s="69"/>
-      <c r="AU11" s="69"/>
+      <c r="AJ11" s="47"/>
+      <c r="AK11" s="47"/>
+      <c r="AL11" s="47"/>
+      <c r="AM11" s="47"/>
+      <c r="AN11" s="47"/>
+      <c r="AO11" s="47"/>
+      <c r="AP11" s="47"/>
+      <c r="AQ11" s="47"/>
+      <c r="AR11" s="47"/>
+      <c r="AS11" s="47"/>
+      <c r="AT11" s="47"/>
+      <c r="AU11" s="47"/>
       <c r="AV11" s="16"/>
       <c r="AW11" s="16"/>
       <c r="AX11" s="16"/>
@@ -2716,11 +2900,11 @@
       <c r="CC11" s="16"/>
       <c r="CD11" s="16"/>
       <c r="CE11" s="17"/>
-      <c r="CF11" s="55"/>
+      <c r="CF11" s="52"/>
     </row>
     <row r="12" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A12" s="68" t="s">
-        <v>35</v>
+      <c r="A12" s="46" t="s">
+        <v>34</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="14"/>
@@ -2740,46 +2924,46 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
       <c r="S12" s="17"/>
-      <c r="T12" s="62"/>
-      <c r="U12" s="63"/>
-      <c r="V12" s="63"/>
-      <c r="W12" s="63"/>
-      <c r="X12" s="63"/>
-      <c r="Y12" s="63"/>
-      <c r="Z12" s="63"/>
-      <c r="AA12" s="64"/>
-      <c r="AB12" s="72"/>
-      <c r="AC12" s="72"/>
-      <c r="AD12" s="73"/>
-      <c r="AE12" s="73"/>
-      <c r="AF12" s="74"/>
-      <c r="AG12" s="74"/>
-      <c r="AH12" s="74"/>
-      <c r="AI12" s="75"/>
-      <c r="AJ12" s="72"/>
-      <c r="AK12" s="73"/>
-      <c r="AL12" s="73"/>
-      <c r="AM12" s="73"/>
-      <c r="AN12" s="73"/>
-      <c r="AO12" s="73"/>
-      <c r="AP12" s="73"/>
-      <c r="AQ12" s="76"/>
-      <c r="AR12" s="72"/>
-      <c r="AS12" s="73"/>
-      <c r="AT12" s="73"/>
-      <c r="AU12" s="73"/>
+      <c r="T12" s="59"/>
+      <c r="U12" s="60"/>
+      <c r="V12" s="60"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="60"/>
+      <c r="Y12" s="60"/>
+      <c r="Z12" s="60"/>
+      <c r="AA12" s="61"/>
+      <c r="AB12" s="15"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="50"/>
+      <c r="AE12" s="50"/>
+      <c r="AF12" s="16"/>
+      <c r="AG12" s="16"/>
+      <c r="AH12" s="16"/>
+      <c r="AI12" s="17"/>
+      <c r="AJ12" s="15"/>
+      <c r="AK12" s="50"/>
+      <c r="AL12" s="50"/>
+      <c r="AM12" s="50"/>
+      <c r="AN12" s="50"/>
+      <c r="AO12" s="50"/>
+      <c r="AP12" s="50"/>
+      <c r="AQ12" s="51"/>
+      <c r="AR12" s="15"/>
+      <c r="AS12" s="50"/>
+      <c r="AT12" s="50"/>
+      <c r="AU12" s="50"/>
       <c r="AV12" s="16"/>
       <c r="AW12" s="16"/>
       <c r="AX12" s="16"/>
       <c r="AY12" s="17"/>
-      <c r="AZ12" s="3"/>
-      <c r="BA12" s="3"/>
-      <c r="BB12" s="3"/>
-      <c r="BC12" s="69"/>
-      <c r="BD12" s="69"/>
-      <c r="BE12" s="69"/>
-      <c r="BF12" s="69"/>
-      <c r="BG12" s="69"/>
+      <c r="AZ12" s="74"/>
+      <c r="BA12" s="74"/>
+      <c r="BB12" s="74"/>
+      <c r="BC12" s="74"/>
+      <c r="BD12" s="74"/>
+      <c r="BE12" s="75"/>
+      <c r="BF12" s="75"/>
+      <c r="BG12" s="75"/>
       <c r="BH12" s="15"/>
       <c r="BI12" s="16"/>
       <c r="BJ12" s="16"/>
@@ -2804,11 +2988,11 @@
       <c r="CC12" s="16"/>
       <c r="CD12" s="16"/>
       <c r="CE12" s="17"/>
-      <c r="CF12" s="55"/>
+      <c r="CF12" s="52"/>
     </row>
     <row r="13" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A13" s="68" t="s">
-        <v>28</v>
+      <c r="A13" s="46" t="s">
+        <v>27</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="14"/>
@@ -2828,16 +3012,16 @@
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
       <c r="S13" s="17"/>
-      <c r="T13" s="62"/>
-      <c r="U13" s="63"/>
-      <c r="V13" s="63"/>
-      <c r="W13" s="63"/>
-      <c r="X13" s="63"/>
-      <c r="Y13" s="63"/>
-      <c r="Z13" s="63"/>
-      <c r="AA13" s="64"/>
-      <c r="AB13" s="70"/>
-      <c r="AC13" s="70"/>
+      <c r="T13" s="59"/>
+      <c r="U13" s="60"/>
+      <c r="V13" s="60"/>
+      <c r="W13" s="60"/>
+      <c r="X13" s="60"/>
+      <c r="Y13" s="60"/>
+      <c r="Z13" s="60"/>
+      <c r="AA13" s="61"/>
+      <c r="AB13" s="48"/>
+      <c r="AC13" s="48"/>
       <c r="AD13" s="16"/>
       <c r="AE13" s="16"/>
       <c r="AF13" s="16"/>
@@ -2892,11 +3076,11 @@
       <c r="CC13" s="16"/>
       <c r="CD13" s="16"/>
       <c r="CE13" s="17"/>
-      <c r="CF13" s="55"/>
+      <c r="CF13" s="52"/>
     </row>
     <row r="14" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A14" s="68" t="s">
-        <v>29</v>
+      <c r="A14" s="46" t="s">
+        <v>28</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="14"/>
@@ -2916,14 +3100,14 @@
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
       <c r="S14" s="17"/>
-      <c r="T14" s="62"/>
-      <c r="U14" s="63"/>
-      <c r="V14" s="63"/>
-      <c r="W14" s="63"/>
-      <c r="X14" s="63"/>
-      <c r="Y14" s="63"/>
-      <c r="Z14" s="63"/>
-      <c r="AA14" s="64"/>
+      <c r="T14" s="59"/>
+      <c r="U14" s="60"/>
+      <c r="V14" s="60"/>
+      <c r="W14" s="60"/>
+      <c r="X14" s="60"/>
+      <c r="Y14" s="60"/>
+      <c r="Z14" s="60"/>
+      <c r="AA14" s="61"/>
       <c r="AB14" s="15"/>
       <c r="AC14" s="16"/>
       <c r="AD14" s="32"/>
@@ -2980,11 +3164,11 @@
       <c r="CC14" s="16"/>
       <c r="CD14" s="16"/>
       <c r="CE14" s="17"/>
-      <c r="CF14" s="55"/>
+      <c r="CF14" s="52"/>
     </row>
     <row r="15" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A15" s="68" t="s">
-        <v>30</v>
+      <c r="A15" s="46" t="s">
+        <v>29</v>
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="14"/>
@@ -3004,14 +3188,14 @@
       <c r="Q15" s="16"/>
       <c r="R15" s="16"/>
       <c r="S15" s="17"/>
-      <c r="T15" s="62"/>
-      <c r="U15" s="63"/>
-      <c r="V15" s="63"/>
-      <c r="W15" s="63"/>
-      <c r="X15" s="63"/>
-      <c r="Y15" s="63"/>
-      <c r="Z15" s="63"/>
-      <c r="AA15" s="64"/>
+      <c r="T15" s="59"/>
+      <c r="U15" s="60"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="60"/>
+      <c r="X15" s="60"/>
+      <c r="Y15" s="60"/>
+      <c r="Z15" s="60"/>
+      <c r="AA15" s="61"/>
       <c r="AB15" s="15"/>
       <c r="AC15" s="16"/>
       <c r="AD15" s="16"/>
@@ -3020,24 +3204,24 @@
       <c r="AG15" s="16"/>
       <c r="AH15" s="16"/>
       <c r="AI15" s="17"/>
-      <c r="AJ15" s="70"/>
-      <c r="AK15" s="70"/>
-      <c r="AL15" s="70"/>
-      <c r="AM15" s="70"/>
-      <c r="AN15" s="70"/>
-      <c r="AO15" s="70"/>
-      <c r="AP15" s="70"/>
-      <c r="AQ15" s="70"/>
-      <c r="AR15" s="70"/>
-      <c r="AS15" s="70"/>
-      <c r="AT15" s="70"/>
-      <c r="AU15" s="70"/>
+      <c r="AJ15" s="48"/>
+      <c r="AK15" s="48"/>
+      <c r="AL15" s="48"/>
+      <c r="AM15" s="48"/>
+      <c r="AN15" s="48"/>
+      <c r="AO15" s="48"/>
+      <c r="AP15" s="48"/>
+      <c r="AQ15" s="48"/>
+      <c r="AR15" s="48"/>
+      <c r="AS15" s="48"/>
+      <c r="AT15" s="48"/>
+      <c r="AU15" s="48"/>
       <c r="AV15" s="16"/>
       <c r="AW15" s="16"/>
       <c r="AX15" s="16"/>
       <c r="AY15" s="17"/>
-      <c r="AZ15" s="70"/>
-      <c r="BA15" s="70"/>
+      <c r="AZ15" s="48"/>
+      <c r="BA15" s="48"/>
       <c r="BB15" s="16"/>
       <c r="BC15" s="16"/>
       <c r="BD15" s="16"/>
@@ -3068,11 +3252,11 @@
       <c r="CC15" s="16"/>
       <c r="CD15" s="16"/>
       <c r="CE15" s="17"/>
-      <c r="CF15" s="55"/>
+      <c r="CF15" s="52"/>
     </row>
     <row r="16" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A16" s="68" t="s">
-        <v>36</v>
+      <c r="A16" s="46" t="s">
+        <v>35</v>
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="14"/>
@@ -3092,14 +3276,14 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
       <c r="S16" s="17"/>
-      <c r="T16" s="62"/>
-      <c r="U16" s="63"/>
-      <c r="V16" s="63"/>
-      <c r="W16" s="63"/>
-      <c r="X16" s="63"/>
-      <c r="Y16" s="63"/>
-      <c r="Z16" s="63"/>
-      <c r="AA16" s="64"/>
+      <c r="T16" s="59"/>
+      <c r="U16" s="60"/>
+      <c r="V16" s="60"/>
+      <c r="W16" s="60"/>
+      <c r="X16" s="60"/>
+      <c r="Y16" s="60"/>
+      <c r="Z16" s="60"/>
+      <c r="AA16" s="61"/>
       <c r="AB16" s="15"/>
       <c r="AC16" s="16"/>
       <c r="AD16" s="16"/>
@@ -3124,29 +3308,29 @@
       <c r="AW16" s="16"/>
       <c r="AX16" s="16"/>
       <c r="AY16" s="17"/>
-      <c r="AZ16" s="45"/>
-      <c r="BA16" s="45"/>
-      <c r="BB16" s="45"/>
-      <c r="BC16" s="45"/>
-      <c r="BD16" s="45"/>
+      <c r="AZ16" s="17"/>
+      <c r="BA16" s="17"/>
+      <c r="BB16" s="17"/>
+      <c r="BC16" s="17"/>
+      <c r="BD16" s="17"/>
       <c r="BE16" s="45"/>
       <c r="BF16" s="45"/>
       <c r="BG16" s="45"/>
       <c r="BH16" s="45"/>
       <c r="BI16" s="45"/>
-      <c r="BJ16" s="71"/>
-      <c r="BK16" s="71"/>
+      <c r="BJ16" s="49"/>
+      <c r="BK16" s="49"/>
       <c r="BL16" s="16"/>
       <c r="BM16" s="16"/>
       <c r="BN16" s="16"/>
       <c r="BO16" s="17"/>
-      <c r="BP16" s="71"/>
-      <c r="BQ16" s="71"/>
-      <c r="BR16" s="3"/>
-      <c r="BS16" s="3"/>
-      <c r="BT16" s="16"/>
-      <c r="BU16" s="16"/>
-      <c r="BV16" s="16"/>
+      <c r="BP16" s="49"/>
+      <c r="BQ16" s="49"/>
+      <c r="BR16" s="49"/>
+      <c r="BS16" s="49"/>
+      <c r="BT16" s="49"/>
+      <c r="BU16" s="49"/>
+      <c r="BV16" s="49"/>
       <c r="BW16" s="17"/>
       <c r="BX16" s="15"/>
       <c r="BY16" s="16"/>
@@ -3156,11 +3340,11 @@
       <c r="CC16" s="16"/>
       <c r="CD16" s="16"/>
       <c r="CE16" s="17"/>
-      <c r="CF16" s="55"/>
+      <c r="CF16" s="52"/>
     </row>
     <row r="17" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A17" s="68" t="s">
-        <v>31</v>
+      <c r="A17" s="46" t="s">
+        <v>30</v>
       </c>
       <c r="B17" s="24"/>
       <c r="C17" s="14"/>
@@ -3180,14 +3364,14 @@
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
       <c r="S17" s="17"/>
-      <c r="T17" s="62"/>
-      <c r="U17" s="63"/>
-      <c r="V17" s="63"/>
-      <c r="W17" s="63"/>
-      <c r="X17" s="63"/>
-      <c r="Y17" s="63"/>
-      <c r="Z17" s="63"/>
-      <c r="AA17" s="64"/>
+      <c r="T17" s="59"/>
+      <c r="U17" s="60"/>
+      <c r="V17" s="60"/>
+      <c r="W17" s="60"/>
+      <c r="X17" s="60"/>
+      <c r="Y17" s="60"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
       <c r="AB17" s="15"/>
       <c r="AC17" s="16"/>
       <c r="AD17" s="16"/>
@@ -3215,23 +3399,18 @@
       <c r="AZ17" s="15"/>
       <c r="BA17" s="16"/>
       <c r="BB17" s="16"/>
-      <c r="BC17" s="16"/>
-      <c r="BD17" s="16"/>
-      <c r="BE17" s="16"/>
-      <c r="BF17" s="16"/>
-      <c r="BG17" s="17"/>
-      <c r="BH17" s="69"/>
-      <c r="BI17" s="69"/>
-      <c r="BJ17" s="69"/>
-      <c r="BK17" s="69"/>
+      <c r="BC17" s="47"/>
+      <c r="BD17" s="47"/>
+      <c r="BE17" s="47"/>
+      <c r="BF17" s="47"/>
+      <c r="BG17" s="47"/>
+      <c r="BH17" s="44"/>
+      <c r="BI17" s="47"/>
+      <c r="BJ17" s="44"/>
       <c r="BL17" s="16"/>
       <c r="BM17" s="16"/>
       <c r="BN17" s="16"/>
       <c r="BO17" s="17"/>
-      <c r="BP17" s="69"/>
-      <c r="BQ17" s="44"/>
-      <c r="BR17" s="69"/>
-      <c r="BS17" s="44"/>
       <c r="BT17" s="16"/>
       <c r="BU17" s="16"/>
       <c r="BV17" s="16"/>
@@ -3244,11 +3423,11 @@
       <c r="CC17" s="16"/>
       <c r="CD17" s="16"/>
       <c r="CE17" s="17"/>
-      <c r="CF17" s="55"/>
+      <c r="CF17" s="52"/>
     </row>
     <row r="18" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A18" s="68" t="s">
-        <v>32</v>
+      <c r="A18" s="46" t="s">
+        <v>31</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="14"/>
@@ -3268,40 +3447,40 @@
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
       <c r="S18" s="17"/>
-      <c r="T18" s="62"/>
-      <c r="U18" s="63"/>
-      <c r="V18" s="63"/>
-      <c r="W18" s="63"/>
-      <c r="X18" s="63"/>
-      <c r="Y18" s="63"/>
-      <c r="Z18" s="63"/>
-      <c r="AA18" s="64"/>
-      <c r="AB18" s="71"/>
-      <c r="AC18" s="71"/>
-      <c r="AD18" s="71"/>
-      <c r="AE18" s="71"/>
+      <c r="T18" s="59"/>
+      <c r="U18" s="60"/>
+      <c r="V18" s="60"/>
+      <c r="W18" s="60"/>
+      <c r="X18" s="60"/>
+      <c r="Y18" s="60"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="49"/>
+      <c r="AC18" s="49"/>
+      <c r="AD18" s="49"/>
+      <c r="AE18" s="49"/>
       <c r="AF18" s="16"/>
       <c r="AG18" s="16"/>
       <c r="AH18" s="16"/>
       <c r="AI18" s="17"/>
-      <c r="AJ18" s="71"/>
-      <c r="AK18" s="71"/>
-      <c r="AL18" s="71"/>
-      <c r="AM18" s="71"/>
-      <c r="AN18" s="71"/>
-      <c r="AO18" s="71"/>
-      <c r="AP18" s="71"/>
-      <c r="AQ18" s="71"/>
-      <c r="AR18" s="71"/>
-      <c r="AS18" s="71"/>
-      <c r="AT18" s="71"/>
-      <c r="AU18" s="71"/>
+      <c r="AJ18" s="49"/>
+      <c r="AK18" s="49"/>
+      <c r="AL18" s="49"/>
+      <c r="AM18" s="49"/>
+      <c r="AN18" s="49"/>
+      <c r="AO18" s="49"/>
+      <c r="AP18" s="49"/>
+      <c r="AQ18" s="49"/>
+      <c r="AR18" s="49"/>
+      <c r="AS18" s="49"/>
+      <c r="AT18" s="49"/>
+      <c r="AU18" s="49"/>
       <c r="AV18" s="16"/>
       <c r="AW18" s="16"/>
       <c r="AX18" s="16"/>
       <c r="AY18" s="17"/>
-      <c r="AZ18" s="72"/>
-      <c r="BA18" s="72"/>
+      <c r="AZ18" s="15"/>
+      <c r="BA18" s="15"/>
       <c r="BB18" s="16"/>
       <c r="BC18" s="16"/>
       <c r="BD18" s="16"/>
@@ -3332,11 +3511,11 @@
       <c r="CC18" s="16"/>
       <c r="CD18" s="16"/>
       <c r="CE18" s="17"/>
-      <c r="CF18" s="55"/>
+      <c r="CF18" s="52"/>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A19" s="68" t="s">
-        <v>33</v>
+      <c r="A19" s="46" t="s">
+        <v>32</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="14"/>
@@ -3356,14 +3535,14 @@
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
       <c r="S19" s="17"/>
-      <c r="T19" s="62"/>
-      <c r="U19" s="63"/>
-      <c r="V19" s="63"/>
-      <c r="W19" s="63"/>
-      <c r="X19" s="63"/>
-      <c r="Y19" s="63"/>
-      <c r="Z19" s="63"/>
-      <c r="AA19" s="64"/>
+      <c r="T19" s="59"/>
+      <c r="U19" s="60"/>
+      <c r="V19" s="60"/>
+      <c r="W19" s="60"/>
+      <c r="X19" s="60"/>
+      <c r="Y19" s="60"/>
+      <c r="Z19" s="60"/>
+      <c r="AA19" s="61"/>
       <c r="AB19" s="15"/>
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
@@ -3396,16 +3575,16 @@
       <c r="BE19" s="16"/>
       <c r="BF19" s="16"/>
       <c r="BG19" s="17"/>
-      <c r="BH19" s="70"/>
-      <c r="BI19" s="70"/>
-      <c r="BJ19" s="70"/>
-      <c r="BK19" s="70"/>
+      <c r="BH19" s="48"/>
+      <c r="BI19" s="48"/>
+      <c r="BJ19" s="48"/>
+      <c r="BK19" s="48"/>
       <c r="BL19" s="16"/>
       <c r="BM19" s="16"/>
       <c r="BN19" s="16"/>
       <c r="BO19" s="17"/>
-      <c r="BP19" s="70"/>
-      <c r="BQ19" s="70"/>
+      <c r="BP19" s="48"/>
+      <c r="BQ19" s="48"/>
       <c r="BR19" s="16"/>
       <c r="BS19" s="16"/>
       <c r="BT19" s="16"/>
@@ -3420,7 +3599,7 @@
       <c r="CC19" s="16"/>
       <c r="CD19" s="16"/>
       <c r="CE19" s="17"/>
-      <c r="CF19" s="55"/>
+      <c r="CF19" s="52"/>
     </row>
     <row r="20" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A20" s="13" t="s">
@@ -3444,14 +3623,14 @@
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
       <c r="S20" s="17"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="63"/>
-      <c r="V20" s="63"/>
-      <c r="W20" s="63"/>
-      <c r="X20" s="63"/>
-      <c r="Y20" s="63"/>
-      <c r="Z20" s="63"/>
-      <c r="AA20" s="64"/>
+      <c r="T20" s="59"/>
+      <c r="U20" s="60"/>
+      <c r="V20" s="60"/>
+      <c r="W20" s="60"/>
+      <c r="X20" s="60"/>
+      <c r="Y20" s="60"/>
+      <c r="Z20" s="60"/>
+      <c r="AA20" s="61"/>
       <c r="AB20" s="15"/>
       <c r="AC20" s="16"/>
       <c r="AD20" s="16"/>
@@ -3476,9 +3655,9 @@
       <c r="AW20" s="16"/>
       <c r="AX20" s="16"/>
       <c r="AY20" s="17"/>
-      <c r="AZ20" s="69"/>
-      <c r="BA20" s="69"/>
-      <c r="BB20" s="69"/>
+      <c r="AZ20" s="47"/>
+      <c r="BA20" s="47"/>
+      <c r="BB20" s="47"/>
       <c r="BC20" s="16"/>
       <c r="BD20" s="16"/>
       <c r="BE20" s="16"/>
@@ -3508,11 +3687,11 @@
       <c r="CC20" s="16"/>
       <c r="CD20" s="16"/>
       <c r="CE20" s="17"/>
-      <c r="CF20" s="55"/>
+      <c r="CF20" s="52"/>
     </row>
     <row r="21" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A21" s="68" t="s">
-        <v>37</v>
+      <c r="A21" s="46" t="s">
+        <v>36</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="14"/>
@@ -3532,14 +3711,14 @@
       <c r="Q21" s="16"/>
       <c r="R21" s="16"/>
       <c r="S21" s="17"/>
-      <c r="T21" s="62"/>
-      <c r="U21" s="63"/>
-      <c r="V21" s="63"/>
-      <c r="W21" s="63"/>
-      <c r="X21" s="63"/>
-      <c r="Y21" s="63"/>
-      <c r="Z21" s="63"/>
-      <c r="AA21" s="64"/>
+      <c r="T21" s="59"/>
+      <c r="U21" s="60"/>
+      <c r="V21" s="60"/>
+      <c r="W21" s="60"/>
+      <c r="X21" s="60"/>
+      <c r="Y21" s="60"/>
+      <c r="Z21" s="60"/>
+      <c r="AA21" s="61"/>
       <c r="AB21" s="15"/>
       <c r="AC21" s="16"/>
       <c r="AD21" s="16"/>
@@ -3596,11 +3775,11 @@
       <c r="CC21" s="16"/>
       <c r="CD21" s="16"/>
       <c r="CE21" s="17"/>
-      <c r="CF21" s="55"/>
+      <c r="CF21" s="52"/>
     </row>
     <row r="22" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A22" s="68" t="s">
-        <v>34</v>
+      <c r="A22" s="46" t="s">
+        <v>33</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="14"/>
@@ -3620,14 +3799,14 @@
       <c r="Q22" s="16"/>
       <c r="R22" s="16"/>
       <c r="S22" s="17"/>
-      <c r="T22" s="62"/>
-      <c r="U22" s="63"/>
-      <c r="V22" s="63"/>
-      <c r="W22" s="63"/>
-      <c r="X22" s="63"/>
-      <c r="Y22" s="63"/>
-      <c r="Z22" s="63"/>
-      <c r="AA22" s="64"/>
+      <c r="T22" s="59"/>
+      <c r="U22" s="60"/>
+      <c r="V22" s="60"/>
+      <c r="W22" s="60"/>
+      <c r="X22" s="60"/>
+      <c r="Y22" s="60"/>
+      <c r="Z22" s="60"/>
+      <c r="AA22" s="61"/>
       <c r="AB22" s="15"/>
       <c r="AC22" s="16"/>
       <c r="AD22" s="16"/>
@@ -3684,7 +3863,7 @@
       <c r="CC22" s="16"/>
       <c r="CD22" s="16"/>
       <c r="CE22" s="17"/>
-      <c r="CF22" s="55"/>
+      <c r="CF22" s="52"/>
     </row>
     <row r="23" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A23" s="13" t="s">
@@ -3708,14 +3887,14 @@
       <c r="Q23" s="16"/>
       <c r="R23" s="16"/>
       <c r="S23" s="17"/>
-      <c r="T23" s="62"/>
-      <c r="U23" s="63"/>
-      <c r="V23" s="63"/>
-      <c r="W23" s="63"/>
-      <c r="X23" s="63"/>
-      <c r="Y23" s="63"/>
-      <c r="Z23" s="63"/>
-      <c r="AA23" s="64"/>
+      <c r="T23" s="59"/>
+      <c r="U23" s="60"/>
+      <c r="V23" s="60"/>
+      <c r="W23" s="60"/>
+      <c r="X23" s="60"/>
+      <c r="Y23" s="60"/>
+      <c r="Z23" s="60"/>
+      <c r="AA23" s="61"/>
       <c r="AB23" s="15"/>
       <c r="AC23" s="16"/>
       <c r="AD23" s="16"/>
@@ -3772,7 +3951,7 @@
       <c r="CC23" s="16"/>
       <c r="CD23" s="16"/>
       <c r="CE23" s="17"/>
-      <c r="CF23" s="55"/>
+      <c r="CF23" s="52"/>
     </row>
     <row r="24" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A24" s="13" t="s">
@@ -3796,14 +3975,14 @@
       <c r="Q24" s="34"/>
       <c r="R24" s="34"/>
       <c r="S24" s="35"/>
-      <c r="T24" s="62"/>
-      <c r="U24" s="63"/>
-      <c r="V24" s="63"/>
-      <c r="W24" s="63"/>
-      <c r="X24" s="63"/>
-      <c r="Y24" s="63"/>
-      <c r="Z24" s="63"/>
-      <c r="AA24" s="64"/>
+      <c r="T24" s="59"/>
+      <c r="U24" s="60"/>
+      <c r="V24" s="60"/>
+      <c r="W24" s="60"/>
+      <c r="X24" s="60"/>
+      <c r="Y24" s="60"/>
+      <c r="Z24" s="60"/>
+      <c r="AA24" s="61"/>
       <c r="AB24" s="36"/>
       <c r="AC24" s="37"/>
       <c r="AD24" s="37"/>
@@ -3860,7 +4039,7 @@
       <c r="CC24" s="37"/>
       <c r="CD24" s="37"/>
       <c r="CE24" s="38"/>
-      <c r="CF24" s="55"/>
+      <c r="CF24" s="52"/>
     </row>
     <row r="25" spans="1:84" x14ac:dyDescent="0.15">
       <c r="B25" s="24"/>
@@ -3881,14 +4060,14 @@
       <c r="Q25" s="16"/>
       <c r="R25" s="16"/>
       <c r="S25" s="17"/>
-      <c r="T25" s="62"/>
-      <c r="U25" s="63"/>
-      <c r="V25" s="63"/>
-      <c r="W25" s="63"/>
-      <c r="X25" s="63"/>
-      <c r="Y25" s="63"/>
-      <c r="Z25" s="63"/>
-      <c r="AA25" s="64"/>
+      <c r="T25" s="59"/>
+      <c r="U25" s="60"/>
+      <c r="V25" s="60"/>
+      <c r="W25" s="60"/>
+      <c r="X25" s="60"/>
+      <c r="Y25" s="60"/>
+      <c r="Z25" s="60"/>
+      <c r="AA25" s="61"/>
       <c r="AB25" s="15"/>
       <c r="AC25" s="16"/>
       <c r="AD25" s="16"/>
@@ -3945,7 +4124,7 @@
       <c r="CC25" s="16"/>
       <c r="CD25" s="16"/>
       <c r="CE25" s="17"/>
-      <c r="CF25" s="55"/>
+      <c r="CF25" s="52"/>
     </row>
     <row r="26" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A26" s="13"/>
@@ -3967,14 +4146,14 @@
       <c r="Q26" s="16"/>
       <c r="R26" s="16"/>
       <c r="S26" s="17"/>
-      <c r="T26" s="62"/>
-      <c r="U26" s="63"/>
-      <c r="V26" s="63"/>
-      <c r="W26" s="63"/>
-      <c r="X26" s="63"/>
-      <c r="Y26" s="63"/>
-      <c r="Z26" s="63"/>
-      <c r="AA26" s="64"/>
+      <c r="T26" s="59"/>
+      <c r="U26" s="60"/>
+      <c r="V26" s="60"/>
+      <c r="W26" s="60"/>
+      <c r="X26" s="60"/>
+      <c r="Y26" s="60"/>
+      <c r="Z26" s="60"/>
+      <c r="AA26" s="61"/>
       <c r="AB26" s="15"/>
       <c r="AC26" s="16"/>
       <c r="AD26" s="16"/>
@@ -4031,7 +4210,7 @@
       <c r="CC26" s="16"/>
       <c r="CD26" s="16"/>
       <c r="CE26" s="17"/>
-      <c r="CF26" s="55"/>
+      <c r="CF26" s="52"/>
     </row>
     <row r="27" spans="1:84" x14ac:dyDescent="0.15">
       <c r="A27" s="13"/>
@@ -4053,14 +4232,14 @@
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
       <c r="S27" s="17"/>
-      <c r="T27" s="62"/>
-      <c r="U27" s="63"/>
-      <c r="V27" s="63"/>
-      <c r="W27" s="63"/>
-      <c r="X27" s="63"/>
-      <c r="Y27" s="63"/>
-      <c r="Z27" s="63"/>
-      <c r="AA27" s="64"/>
+      <c r="T27" s="59"/>
+      <c r="U27" s="60"/>
+      <c r="V27" s="60"/>
+      <c r="W27" s="60"/>
+      <c r="X27" s="60"/>
+      <c r="Y27" s="60"/>
+      <c r="Z27" s="60"/>
+      <c r="AA27" s="61"/>
       <c r="AB27" s="15"/>
       <c r="AC27" s="16"/>
       <c r="AD27" s="16"/>
@@ -4117,7 +4296,7 @@
       <c r="CC27" s="16"/>
       <c r="CD27" s="16"/>
       <c r="CE27" s="17"/>
-      <c r="CF27" s="55"/>
+      <c r="CF27" s="52"/>
     </row>
     <row r="28" spans="1:84" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18"/>
@@ -4139,14 +4318,14 @@
       <c r="Q28" s="21"/>
       <c r="R28" s="21"/>
       <c r="S28" s="22"/>
-      <c r="T28" s="65"/>
-      <c r="U28" s="66"/>
-      <c r="V28" s="66"/>
-      <c r="W28" s="66"/>
-      <c r="X28" s="66"/>
-      <c r="Y28" s="66"/>
-      <c r="Z28" s="66"/>
-      <c r="AA28" s="67"/>
+      <c r="T28" s="62"/>
+      <c r="U28" s="63"/>
+      <c r="V28" s="63"/>
+      <c r="W28" s="63"/>
+      <c r="X28" s="63"/>
+      <c r="Y28" s="63"/>
+      <c r="Z28" s="63"/>
+      <c r="AA28" s="64"/>
       <c r="AB28" s="20"/>
       <c r="AC28" s="21"/>
       <c r="AD28" s="21"/>
@@ -4203,129 +4382,122 @@
       <c r="CC28" s="21"/>
       <c r="CD28" s="21"/>
       <c r="CE28" s="22"/>
-      <c r="CF28" s="55"/>
+      <c r="CF28" s="52"/>
     </row>
     <row r="29" spans="1:84" x14ac:dyDescent="0.15">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="56"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="56"/>
-      <c r="O29" s="56"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="56"/>
-      <c r="R29" s="56"/>
-      <c r="S29" s="56"/>
-      <c r="T29" s="56"/>
-      <c r="U29" s="56"/>
-      <c r="V29" s="56"/>
-      <c r="W29" s="56"/>
-      <c r="X29" s="56"/>
-      <c r="Y29" s="56"/>
-      <c r="Z29" s="56"/>
-      <c r="AA29" s="56"/>
-      <c r="AB29" s="56"/>
-      <c r="AC29" s="56"/>
-      <c r="AD29" s="56"/>
-      <c r="AE29" s="56"/>
-      <c r="AF29" s="56"/>
-      <c r="AG29" s="56"/>
-      <c r="AH29" s="56"/>
-      <c r="AI29" s="56"/>
-      <c r="AJ29" s="56"/>
-      <c r="AK29" s="56"/>
-      <c r="AL29" s="56"/>
-      <c r="AM29" s="56"/>
-      <c r="AN29" s="56"/>
-      <c r="AO29" s="56"/>
-      <c r="AP29" s="56"/>
-      <c r="AQ29" s="56"/>
-      <c r="AR29" s="56"/>
-      <c r="AS29" s="56"/>
-      <c r="AT29" s="56"/>
-      <c r="AU29" s="56"/>
-      <c r="AV29" s="56"/>
-      <c r="AW29" s="56"/>
-      <c r="AX29" s="56"/>
-      <c r="AY29" s="56"/>
-      <c r="AZ29" s="56"/>
-      <c r="BA29" s="56"/>
-      <c r="BB29" s="56"/>
-      <c r="BC29" s="56"/>
-      <c r="BD29" s="56"/>
-      <c r="BE29" s="56"/>
-      <c r="BF29" s="56"/>
-      <c r="BG29" s="56"/>
-      <c r="BH29" s="56"/>
-      <c r="BI29" s="56"/>
-      <c r="BJ29" s="56"/>
-      <c r="BK29" s="56"/>
-      <c r="BL29" s="56"/>
-      <c r="BM29" s="56"/>
-      <c r="BN29" s="56"/>
-      <c r="BO29" s="56"/>
-      <c r="BP29" s="56"/>
-      <c r="BQ29" s="56"/>
-      <c r="BR29" s="56"/>
-      <c r="BS29" s="56"/>
-      <c r="BT29" s="56"/>
-      <c r="BU29" s="56"/>
-      <c r="BV29" s="56"/>
-      <c r="BW29" s="56"/>
-      <c r="BX29" s="56"/>
-      <c r="BY29" s="56"/>
-      <c r="BZ29" s="56"/>
-      <c r="CA29" s="56"/>
-      <c r="CB29" s="56"/>
-      <c r="CC29" s="56"/>
-      <c r="CD29" s="56"/>
-      <c r="CE29" s="56"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="53"/>
+      <c r="P29" s="53"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="53"/>
+      <c r="S29" s="53"/>
+      <c r="T29" s="53"/>
+      <c r="U29" s="53"/>
+      <c r="V29" s="53"/>
+      <c r="W29" s="53"/>
+      <c r="X29" s="53"/>
+      <c r="Y29" s="53"/>
+      <c r="Z29" s="53"/>
+      <c r="AA29" s="53"/>
+      <c r="AB29" s="53"/>
+      <c r="AC29" s="53"/>
+      <c r="AD29" s="53"/>
+      <c r="AE29" s="53"/>
+      <c r="AF29" s="53"/>
+      <c r="AG29" s="53"/>
+      <c r="AH29" s="53"/>
+      <c r="AI29" s="53"/>
+      <c r="AJ29" s="53"/>
+      <c r="AK29" s="53"/>
+      <c r="AL29" s="53"/>
+      <c r="AM29" s="53"/>
+      <c r="AN29" s="53"/>
+      <c r="AO29" s="53"/>
+      <c r="AP29" s="53"/>
+      <c r="AQ29" s="53"/>
+      <c r="AR29" s="53"/>
+      <c r="AS29" s="53"/>
+      <c r="AT29" s="53"/>
+      <c r="AU29" s="53"/>
+      <c r="AV29" s="53"/>
+      <c r="AW29" s="53"/>
+      <c r="AX29" s="53"/>
+      <c r="AY29" s="53"/>
+      <c r="AZ29" s="53"/>
+      <c r="BA29" s="53"/>
+      <c r="BB29" s="53"/>
+      <c r="BC29" s="53"/>
+      <c r="BD29" s="53"/>
+      <c r="BE29" s="53"/>
+      <c r="BF29" s="53"/>
+      <c r="BG29" s="53"/>
+      <c r="BH29" s="53"/>
+      <c r="BI29" s="53"/>
+      <c r="BJ29" s="53"/>
+      <c r="BK29" s="53"/>
+      <c r="BL29" s="53"/>
+      <c r="BM29" s="53"/>
+      <c r="BN29" s="53"/>
+      <c r="BO29" s="53"/>
+      <c r="BP29" s="53"/>
+      <c r="BQ29" s="53"/>
+      <c r="BR29" s="53"/>
+      <c r="BS29" s="53"/>
+      <c r="BT29" s="53"/>
+      <c r="BU29" s="53"/>
+      <c r="BV29" s="53"/>
+      <c r="BW29" s="53"/>
+      <c r="BX29" s="53"/>
+      <c r="BY29" s="53"/>
+      <c r="BZ29" s="53"/>
+      <c r="CA29" s="53"/>
+      <c r="CB29" s="53"/>
+      <c r="CC29" s="53"/>
+      <c r="CD29" s="53"/>
+      <c r="CE29" s="53"/>
     </row>
     <row r="32" spans="1:84" x14ac:dyDescent="0.15">
       <c r="B32" s="39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C32" s="40"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B33" s="39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33" s="41"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B34" s="39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="42"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B35" s="39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="CF4:CF28"/>
-    <mergeCell ref="A29:CE29"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="T6:AA28"/>
-    <mergeCell ref="AZ4:BC4"/>
-    <mergeCell ref="BD4:BG4"/>
-    <mergeCell ref="BH4:BK4"/>
-    <mergeCell ref="BL4:BO4"/>
+    <mergeCell ref="D2:AQ3"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="AR2:CE3"/>
     <mergeCell ref="AJ4:AM4"/>
@@ -4342,10 +4514,17 @@
     <mergeCell ref="BX4:CA4"/>
     <mergeCell ref="CB4:CE4"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="CF4:CF28"/>
+    <mergeCell ref="A29:CE29"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="T6:AA28"/>
+    <mergeCell ref="AZ4:BC4"/>
+    <mergeCell ref="BD4:BG4"/>
+    <mergeCell ref="BH4:BK4"/>
+    <mergeCell ref="BL4:BO4"/>
     <mergeCell ref="P4:S4"/>
     <mergeCell ref="T4:W4"/>
     <mergeCell ref="X4:AA4"/>
-    <mergeCell ref="D2:AQ3"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="B6:B28">
@@ -4385,15 +4564,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2041c0d2b30335279095007fcb0a9d7c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="56b9c1bb8339570eda07374d036e5caf" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -4606,32 +4776,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F2702F0-3EB0-496B-8166-A9BB237AECA6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E70815D-A53F-41E3-B87E-1E164A9F927C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4648,4 +4819,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Documentation pour les RPI
</commit_message>
<xml_diff>
--- a/documentation/3_2_Modele_PlanningLundiMardi.xlsx
+++ b/documentation/3_2_Modele_PlanningLundiMardi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wickil01\Downloads\306project-G4\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Emf\306\306project-G4\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5093F91-6E43-4C47-8D2F-B0655AAE4905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B78822-A6CC-4E43-828D-BC431C3592A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="8" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
   <si>
     <t>Tâches</t>
   </si>
@@ -1114,18 +1114,61 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" textRotation="90"/>
       <protection locked="0"/>
@@ -1172,49 +1215,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1822,36 +1822,36 @@
   <dimension ref="A1:CF43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="AA6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomRight" activeCell="BH23" sqref="BH23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="46.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="9" style="3" customWidth="1"/>
-    <col min="4" max="83" width="2.140625" style="2" customWidth="1"/>
-    <col min="84" max="84" width="3.140625" style="3" customWidth="1"/>
-    <col min="85" max="297" width="9.140625" style="3" customWidth="1"/>
-    <col min="298" max="16384" width="11.42578125" style="3"/>
+    <col min="4" max="83" width="2.1796875" style="2" customWidth="1"/>
+    <col min="84" max="84" width="3.1796875" style="3" customWidth="1"/>
+    <col min="85" max="297" width="9.1796875" style="3" customWidth="1"/>
+    <col min="298" max="16384" width="11.453125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:84" ht="23" x14ac:dyDescent="0.5">
+      <c r="A1" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1886,177 +1886,177 @@
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
     </row>
-    <row r="2" spans="1:84" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:84" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77"/>
-      <c r="U2" s="77"/>
-      <c r="V2" s="77"/>
-      <c r="W2" s="77"/>
-      <c r="X2" s="77"/>
-      <c r="Y2" s="77"/>
-      <c r="Z2" s="77"/>
-      <c r="AA2" s="77"/>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="77"/>
-      <c r="AD2" s="77"/>
-      <c r="AE2" s="77"/>
-      <c r="AF2" s="77"/>
-      <c r="AG2" s="77"/>
-      <c r="AH2" s="77"/>
-      <c r="AI2" s="77"/>
-      <c r="AJ2" s="77"/>
-      <c r="AK2" s="77"/>
-      <c r="AL2" s="77"/>
-      <c r="AM2" s="77"/>
-      <c r="AN2" s="77"/>
-      <c r="AO2" s="77"/>
-      <c r="AP2" s="77"/>
-      <c r="AQ2" s="77"/>
-      <c r="AR2" s="77"/>
-      <c r="AS2" s="77"/>
-      <c r="AT2" s="77"/>
-      <c r="AU2" s="77"/>
-      <c r="AV2" s="77"/>
-      <c r="AW2" s="77"/>
-      <c r="AX2" s="77"/>
-      <c r="AY2" s="77"/>
-      <c r="AZ2" s="77"/>
-      <c r="BA2" s="77"/>
-      <c r="BB2" s="77"/>
-      <c r="BC2" s="77"/>
-      <c r="BD2" s="77"/>
-      <c r="BE2" s="77"/>
-      <c r="BF2" s="77"/>
-      <c r="BG2" s="77"/>
-      <c r="BH2" s="77"/>
-      <c r="BI2" s="77"/>
-      <c r="BJ2" s="77"/>
-      <c r="BK2" s="77"/>
-      <c r="BL2" s="77"/>
-      <c r="BM2" s="77"/>
-      <c r="BN2" s="77"/>
-      <c r="BO2" s="77"/>
-      <c r="BP2" s="77"/>
-      <c r="BQ2" s="77"/>
-      <c r="BR2" s="77"/>
-      <c r="BS2" s="77"/>
-      <c r="BT2" s="77"/>
-      <c r="BU2" s="77"/>
-      <c r="BV2" s="77"/>
-      <c r="BW2" s="77"/>
-      <c r="BX2" s="77"/>
-      <c r="BY2" s="77"/>
-      <c r="BZ2" s="77"/>
-      <c r="CA2" s="77"/>
-      <c r="CB2" s="77"/>
-      <c r="CC2" s="77"/>
-      <c r="CD2" s="77"/>
-      <c r="CE2" s="77"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="82"/>
+      <c r="V2" s="82"/>
+      <c r="W2" s="82"/>
+      <c r="X2" s="82"/>
+      <c r="Y2" s="82"/>
+      <c r="Z2" s="82"/>
+      <c r="AA2" s="82"/>
+      <c r="AB2" s="82"/>
+      <c r="AC2" s="82"/>
+      <c r="AD2" s="82"/>
+      <c r="AE2" s="82"/>
+      <c r="AF2" s="82"/>
+      <c r="AG2" s="82"/>
+      <c r="AH2" s="82"/>
+      <c r="AI2" s="82"/>
+      <c r="AJ2" s="82"/>
+      <c r="AK2" s="82"/>
+      <c r="AL2" s="82"/>
+      <c r="AM2" s="82"/>
+      <c r="AN2" s="82"/>
+      <c r="AO2" s="82"/>
+      <c r="AP2" s="82"/>
+      <c r="AQ2" s="82"/>
+      <c r="AR2" s="82"/>
+      <c r="AS2" s="82"/>
+      <c r="AT2" s="82"/>
+      <c r="AU2" s="82"/>
+      <c r="AV2" s="82"/>
+      <c r="AW2" s="82"/>
+      <c r="AX2" s="82"/>
+      <c r="AY2" s="82"/>
+      <c r="AZ2" s="82"/>
+      <c r="BA2" s="82"/>
+      <c r="BB2" s="82"/>
+      <c r="BC2" s="82"/>
+      <c r="BD2" s="82"/>
+      <c r="BE2" s="82"/>
+      <c r="BF2" s="82"/>
+      <c r="BG2" s="82"/>
+      <c r="BH2" s="82"/>
+      <c r="BI2" s="82"/>
+      <c r="BJ2" s="82"/>
+      <c r="BK2" s="82"/>
+      <c r="BL2" s="82"/>
+      <c r="BM2" s="82"/>
+      <c r="BN2" s="82"/>
+      <c r="BO2" s="82"/>
+      <c r="BP2" s="82"/>
+      <c r="BQ2" s="82"/>
+      <c r="BR2" s="82"/>
+      <c r="BS2" s="82"/>
+      <c r="BT2" s="82"/>
+      <c r="BU2" s="82"/>
+      <c r="BV2" s="82"/>
+      <c r="BW2" s="82"/>
+      <c r="BX2" s="82"/>
+      <c r="BY2" s="82"/>
+      <c r="BZ2" s="82"/>
+      <c r="CA2" s="82"/>
+      <c r="CB2" s="82"/>
+      <c r="CC2" s="82"/>
+      <c r="CD2" s="82"/>
+      <c r="CE2" s="82"/>
     </row>
-    <row r="3" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78"/>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="78"/>
-      <c r="AB3" s="78"/>
-      <c r="AC3" s="78"/>
-      <c r="AD3" s="78"/>
-      <c r="AE3" s="78"/>
-      <c r="AF3" s="78"/>
-      <c r="AG3" s="78"/>
-      <c r="AH3" s="78"/>
-      <c r="AI3" s="78"/>
-      <c r="AJ3" s="78"/>
-      <c r="AK3" s="78"/>
-      <c r="AL3" s="78"/>
-      <c r="AM3" s="78"/>
-      <c r="AN3" s="78"/>
-      <c r="AO3" s="78"/>
-      <c r="AP3" s="78"/>
-      <c r="AQ3" s="78"/>
-      <c r="AR3" s="78"/>
-      <c r="AS3" s="78"/>
-      <c r="AT3" s="78"/>
-      <c r="AU3" s="78"/>
-      <c r="AV3" s="78"/>
-      <c r="AW3" s="78"/>
-      <c r="AX3" s="78"/>
-      <c r="AY3" s="78"/>
-      <c r="AZ3" s="78"/>
-      <c r="BA3" s="78"/>
-      <c r="BB3" s="78"/>
-      <c r="BC3" s="78"/>
-      <c r="BD3" s="78"/>
-      <c r="BE3" s="78"/>
-      <c r="BF3" s="78"/>
-      <c r="BG3" s="78"/>
-      <c r="BH3" s="78"/>
-      <c r="BI3" s="78"/>
-      <c r="BJ3" s="78"/>
-      <c r="BK3" s="78"/>
-      <c r="BL3" s="78"/>
-      <c r="BM3" s="78"/>
-      <c r="BN3" s="78"/>
-      <c r="BO3" s="78"/>
-      <c r="BP3" s="78"/>
-      <c r="BQ3" s="78"/>
-      <c r="BR3" s="78"/>
-      <c r="BS3" s="78"/>
-      <c r="BT3" s="78"/>
-      <c r="BU3" s="78"/>
-      <c r="BV3" s="78"/>
-      <c r="BW3" s="78"/>
-      <c r="BX3" s="78"/>
-      <c r="BY3" s="78"/>
-      <c r="BZ3" s="78"/>
-      <c r="CA3" s="78"/>
-      <c r="CB3" s="78"/>
-      <c r="CC3" s="78"/>
-      <c r="CD3" s="78"/>
-      <c r="CE3" s="78"/>
+    <row r="3" spans="1:84" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="83"/>
+      <c r="S3" s="83"/>
+      <c r="T3" s="83"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="83"/>
+      <c r="AA3" s="83"/>
+      <c r="AB3" s="83"/>
+      <c r="AC3" s="83"/>
+      <c r="AD3" s="83"/>
+      <c r="AE3" s="83"/>
+      <c r="AF3" s="83"/>
+      <c r="AG3" s="83"/>
+      <c r="AH3" s="83"/>
+      <c r="AI3" s="83"/>
+      <c r="AJ3" s="83"/>
+      <c r="AK3" s="83"/>
+      <c r="AL3" s="83"/>
+      <c r="AM3" s="83"/>
+      <c r="AN3" s="83"/>
+      <c r="AO3" s="83"/>
+      <c r="AP3" s="83"/>
+      <c r="AQ3" s="83"/>
+      <c r="AR3" s="83"/>
+      <c r="AS3" s="83"/>
+      <c r="AT3" s="83"/>
+      <c r="AU3" s="83"/>
+      <c r="AV3" s="83"/>
+      <c r="AW3" s="83"/>
+      <c r="AX3" s="83"/>
+      <c r="AY3" s="83"/>
+      <c r="AZ3" s="83"/>
+      <c r="BA3" s="83"/>
+      <c r="BB3" s="83"/>
+      <c r="BC3" s="83"/>
+      <c r="BD3" s="83"/>
+      <c r="BE3" s="83"/>
+      <c r="BF3" s="83"/>
+      <c r="BG3" s="83"/>
+      <c r="BH3" s="83"/>
+      <c r="BI3" s="83"/>
+      <c r="BJ3" s="83"/>
+      <c r="BK3" s="83"/>
+      <c r="BL3" s="83"/>
+      <c r="BM3" s="83"/>
+      <c r="BN3" s="83"/>
+      <c r="BO3" s="83"/>
+      <c r="BP3" s="83"/>
+      <c r="BQ3" s="83"/>
+      <c r="BR3" s="83"/>
+      <c r="BS3" s="83"/>
+      <c r="BT3" s="83"/>
+      <c r="BU3" s="83"/>
+      <c r="BV3" s="83"/>
+      <c r="BW3" s="83"/>
+      <c r="BX3" s="83"/>
+      <c r="BY3" s="83"/>
+      <c r="BZ3" s="83"/>
+      <c r="CA3" s="83"/>
+      <c r="CB3" s="83"/>
+      <c r="CC3" s="83"/>
+      <c r="CD3" s="83"/>
+      <c r="CE3" s="83"/>
     </row>
-    <row r="4" spans="1:84" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="80" t="s">
+    <row r="4" spans="1:84" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="25" t="s">
@@ -2065,132 +2065,132 @@
       <c r="C4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="91" t="s">
+      <c r="D4" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="93">
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="86">
         <v>45992</v>
       </c>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="91" t="s">
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="93">
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="86">
         <v>45993</v>
       </c>
-      <c r="Q4" s="93"/>
-      <c r="R4" s="93"/>
-      <c r="S4" s="94"/>
-      <c r="T4" s="91" t="s">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="92"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="92"/>
-      <c r="X4" s="93">
+      <c r="U4" s="85"/>
+      <c r="V4" s="85"/>
+      <c r="W4" s="85"/>
+      <c r="X4" s="86">
         <v>45999</v>
       </c>
-      <c r="Y4" s="93"/>
-      <c r="Z4" s="93"/>
-      <c r="AA4" s="94"/>
-      <c r="AB4" s="91" t="s">
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="87"/>
+      <c r="AB4" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="AC4" s="92"/>
-      <c r="AD4" s="92"/>
-      <c r="AE4" s="92"/>
-      <c r="AF4" s="93">
+      <c r="AC4" s="85"/>
+      <c r="AD4" s="85"/>
+      <c r="AE4" s="85"/>
+      <c r="AF4" s="86">
         <v>46000</v>
       </c>
-      <c r="AG4" s="93"/>
-      <c r="AH4" s="93"/>
-      <c r="AI4" s="94"/>
-      <c r="AJ4" s="91" t="s">
+      <c r="AG4" s="86"/>
+      <c r="AH4" s="86"/>
+      <c r="AI4" s="87"/>
+      <c r="AJ4" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="AK4" s="92"/>
-      <c r="AL4" s="92"/>
-      <c r="AM4" s="92"/>
-      <c r="AN4" s="93">
+      <c r="AK4" s="85"/>
+      <c r="AL4" s="85"/>
+      <c r="AM4" s="85"/>
+      <c r="AN4" s="86">
         <v>46006</v>
       </c>
-      <c r="AO4" s="93"/>
-      <c r="AP4" s="93"/>
-      <c r="AQ4" s="94"/>
-      <c r="AR4" s="91" t="s">
+      <c r="AO4" s="86"/>
+      <c r="AP4" s="86"/>
+      <c r="AQ4" s="87"/>
+      <c r="AR4" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="AS4" s="92"/>
-      <c r="AT4" s="92"/>
-      <c r="AU4" s="92"/>
-      <c r="AV4" s="93">
+      <c r="AS4" s="85"/>
+      <c r="AT4" s="85"/>
+      <c r="AU4" s="85"/>
+      <c r="AV4" s="86">
         <v>46007</v>
       </c>
-      <c r="AW4" s="93"/>
-      <c r="AX4" s="93"/>
-      <c r="AY4" s="94"/>
-      <c r="AZ4" s="91" t="s">
+      <c r="AW4" s="86"/>
+      <c r="AX4" s="86"/>
+      <c r="AY4" s="87"/>
+      <c r="AZ4" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="BA4" s="92"/>
-      <c r="BB4" s="92"/>
-      <c r="BC4" s="92"/>
-      <c r="BD4" s="93">
+      <c r="BA4" s="85"/>
+      <c r="BB4" s="85"/>
+      <c r="BC4" s="85"/>
+      <c r="BD4" s="86">
         <v>46027</v>
       </c>
-      <c r="BE4" s="93"/>
-      <c r="BF4" s="93"/>
-      <c r="BG4" s="94"/>
-      <c r="BH4" s="91" t="s">
+      <c r="BE4" s="86"/>
+      <c r="BF4" s="86"/>
+      <c r="BG4" s="87"/>
+      <c r="BH4" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="BI4" s="92"/>
-      <c r="BJ4" s="92"/>
-      <c r="BK4" s="92"/>
-      <c r="BL4" s="93">
+      <c r="BI4" s="85"/>
+      <c r="BJ4" s="85"/>
+      <c r="BK4" s="85"/>
+      <c r="BL4" s="86">
         <v>46028</v>
       </c>
-      <c r="BM4" s="93"/>
-      <c r="BN4" s="93"/>
-      <c r="BO4" s="94"/>
-      <c r="BP4" s="91" t="s">
+      <c r="BM4" s="86"/>
+      <c r="BN4" s="86"/>
+      <c r="BO4" s="87"/>
+      <c r="BP4" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="BQ4" s="92"/>
-      <c r="BR4" s="92"/>
-      <c r="BS4" s="92"/>
-      <c r="BT4" s="93">
+      <c r="BQ4" s="85"/>
+      <c r="BR4" s="85"/>
+      <c r="BS4" s="85"/>
+      <c r="BT4" s="86">
         <v>46034</v>
       </c>
-      <c r="BU4" s="93"/>
-      <c r="BV4" s="93"/>
-      <c r="BW4" s="94"/>
-      <c r="BX4" s="91" t="s">
+      <c r="BU4" s="86"/>
+      <c r="BV4" s="86"/>
+      <c r="BW4" s="87"/>
+      <c r="BX4" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="BY4" s="92"/>
-      <c r="BZ4" s="92"/>
-      <c r="CA4" s="92"/>
-      <c r="CB4" s="93">
+      <c r="BY4" s="85"/>
+      <c r="BZ4" s="85"/>
+      <c r="CA4" s="85"/>
+      <c r="CB4" s="86">
         <v>46035</v>
       </c>
-      <c r="CC4" s="93"/>
-      <c r="CD4" s="93"/>
-      <c r="CE4" s="94"/>
-      <c r="CF4" s="79" t="s">
+      <c r="CC4" s="86"/>
+      <c r="CD4" s="86"/>
+      <c r="CE4" s="87"/>
+      <c r="CF4" s="91" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="81"/>
+    <row r="5" spans="1:84" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="93"/>
       <c r="B5" s="26" t="s">
         <v>2</v>
       </c>
@@ -2437,9 +2437,9 @@
       <c r="CE5" s="7">
         <v>8</v>
       </c>
-      <c r="CF5" s="79"/>
+      <c r="CF5" s="91"/>
     </row>
-    <row r="6" spans="1:84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:84" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="75" t="s">
         <v>43</v>
       </c>
@@ -2463,16 +2463,16 @@
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="10"/>
-      <c r="T6" s="82" t="s">
+      <c r="T6" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="U6" s="83"/>
-      <c r="V6" s="83"/>
-      <c r="W6" s="83"/>
-      <c r="X6" s="83"/>
-      <c r="Y6" s="83"/>
-      <c r="Z6" s="83"/>
-      <c r="AA6" s="84"/>
+      <c r="U6" s="95"/>
+      <c r="V6" s="95"/>
+      <c r="W6" s="95"/>
+      <c r="X6" s="95"/>
+      <c r="Y6" s="95"/>
+      <c r="Z6" s="95"/>
+      <c r="AA6" s="96"/>
       <c r="AB6" s="11"/>
       <c r="AC6" s="9"/>
       <c r="AD6" s="9"/>
@@ -2529,9 +2529,9 @@
       <c r="CC6" s="9"/>
       <c r="CD6" s="9"/>
       <c r="CE6" s="10"/>
-      <c r="CF6" s="79"/>
+      <c r="CF6" s="91"/>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
@@ -2555,14 +2555,14 @@
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
       <c r="S7" s="16"/>
-      <c r="T7" s="85"/>
-      <c r="U7" s="86"/>
-      <c r="V7" s="86"/>
-      <c r="W7" s="86"/>
-      <c r="X7" s="86"/>
-      <c r="Y7" s="86"/>
-      <c r="Z7" s="86"/>
-      <c r="AA7" s="87"/>
+      <c r="T7" s="97"/>
+      <c r="U7" s="98"/>
+      <c r="V7" s="98"/>
+      <c r="W7" s="98"/>
+      <c r="X7" s="98"/>
+      <c r="Y7" s="98"/>
+      <c r="Z7" s="98"/>
+      <c r="AA7" s="99"/>
       <c r="AB7" s="14"/>
       <c r="AC7" s="15"/>
       <c r="AD7" s="15"/>
@@ -2619,9 +2619,9 @@
       <c r="CC7" s="15"/>
       <c r="CD7" s="15"/>
       <c r="CE7" s="16"/>
-      <c r="CF7" s="79"/>
+      <c r="CF7" s="91"/>
     </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>11</v>
       </c>
@@ -2645,14 +2645,14 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="16"/>
-      <c r="T8" s="85"/>
-      <c r="U8" s="86"/>
-      <c r="V8" s="86"/>
-      <c r="W8" s="86"/>
-      <c r="X8" s="86"/>
-      <c r="Y8" s="86"/>
-      <c r="Z8" s="86"/>
-      <c r="AA8" s="87"/>
+      <c r="T8" s="97"/>
+      <c r="U8" s="98"/>
+      <c r="V8" s="98"/>
+      <c r="W8" s="98"/>
+      <c r="X8" s="98"/>
+      <c r="Y8" s="98"/>
+      <c r="Z8" s="98"/>
+      <c r="AA8" s="99"/>
       <c r="AB8" s="14"/>
       <c r="AC8" s="15"/>
       <c r="AD8" s="15"/>
@@ -2709,9 +2709,9 @@
       <c r="CC8" s="15"/>
       <c r="CD8" s="15"/>
       <c r="CE8" s="16"/>
-      <c r="CF8" s="79"/>
+      <c r="CF8" s="91"/>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -2735,14 +2735,14 @@
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
       <c r="S9" s="16"/>
-      <c r="T9" s="85"/>
-      <c r="U9" s="86"/>
-      <c r="V9" s="86"/>
-      <c r="W9" s="86"/>
-      <c r="X9" s="86"/>
-      <c r="Y9" s="86"/>
-      <c r="Z9" s="86"/>
-      <c r="AA9" s="87"/>
+      <c r="T9" s="97"/>
+      <c r="U9" s="98"/>
+      <c r="V9" s="98"/>
+      <c r="W9" s="98"/>
+      <c r="X9" s="98"/>
+      <c r="Y9" s="98"/>
+      <c r="Z9" s="98"/>
+      <c r="AA9" s="99"/>
       <c r="AB9" s="14"/>
       <c r="AC9" s="15"/>
       <c r="AD9" s="15"/>
@@ -2799,9 +2799,9 @@
       <c r="CC9" s="15"/>
       <c r="CD9" s="15"/>
       <c r="CE9" s="16"/>
-      <c r="CF9" s="79"/>
+      <c r="CF9" s="91"/>
     </row>
-    <row r="10" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>22</v>
       </c>
@@ -2825,14 +2825,14 @@
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
       <c r="S10" s="16"/>
-      <c r="T10" s="85"/>
-      <c r="U10" s="86"/>
-      <c r="V10" s="86"/>
-      <c r="W10" s="86"/>
-      <c r="X10" s="86"/>
-      <c r="Y10" s="86"/>
-      <c r="Z10" s="86"/>
-      <c r="AA10" s="87"/>
+      <c r="T10" s="97"/>
+      <c r="U10" s="98"/>
+      <c r="V10" s="98"/>
+      <c r="W10" s="98"/>
+      <c r="X10" s="98"/>
+      <c r="Y10" s="98"/>
+      <c r="Z10" s="98"/>
+      <c r="AA10" s="99"/>
       <c r="AB10" s="14"/>
       <c r="AC10" s="15"/>
       <c r="AD10" s="15"/>
@@ -2889,9 +2889,9 @@
       <c r="CC10" s="15"/>
       <c r="CD10" s="15"/>
       <c r="CE10" s="16"/>
-      <c r="CF10" s="79"/>
+      <c r="CF10" s="91"/>
     </row>
-    <row r="11" spans="1:84" s="63" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:84" s="63" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="68" t="s">
         <v>36</v>
       </c>
@@ -2913,14 +2913,14 @@
       <c r="Q11" s="58"/>
       <c r="R11" s="58"/>
       <c r="S11" s="61"/>
-      <c r="T11" s="85"/>
-      <c r="U11" s="86"/>
-      <c r="V11" s="86"/>
-      <c r="W11" s="86"/>
-      <c r="X11" s="86"/>
-      <c r="Y11" s="86"/>
-      <c r="Z11" s="86"/>
-      <c r="AA11" s="87"/>
+      <c r="T11" s="97"/>
+      <c r="U11" s="98"/>
+      <c r="V11" s="98"/>
+      <c r="W11" s="98"/>
+      <c r="X11" s="98"/>
+      <c r="Y11" s="98"/>
+      <c r="Z11" s="98"/>
+      <c r="AA11" s="99"/>
       <c r="AB11" s="57"/>
       <c r="AC11" s="60"/>
       <c r="AD11" s="60"/>
@@ -2977,10 +2977,10 @@
       <c r="CC11" s="58"/>
       <c r="CD11" s="58"/>
       <c r="CE11" s="61"/>
-      <c r="CF11" s="79"/>
+      <c r="CF11" s="91"/>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A12" s="98" t="s">
+    <row r="12" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A12" s="76" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -3003,14 +3003,14 @@
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
       <c r="S12" s="16"/>
-      <c r="T12" s="85"/>
-      <c r="U12" s="86"/>
-      <c r="V12" s="86"/>
-      <c r="W12" s="86"/>
-      <c r="X12" s="86"/>
-      <c r="Y12" s="86"/>
-      <c r="Z12" s="86"/>
-      <c r="AA12" s="87"/>
+      <c r="T12" s="97"/>
+      <c r="U12" s="98"/>
+      <c r="V12" s="98"/>
+      <c r="W12" s="98"/>
+      <c r="X12" s="98"/>
+      <c r="Y12" s="98"/>
+      <c r="Z12" s="98"/>
+      <c r="AA12" s="99"/>
       <c r="AB12" s="52" t="s">
         <v>34</v>
       </c>
@@ -3077,10 +3077,10 @@
       <c r="CC12" s="15"/>
       <c r="CD12" s="15"/>
       <c r="CE12" s="16"/>
-      <c r="CF12" s="79"/>
+      <c r="CF12" s="91"/>
     </row>
-    <row r="13" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A13" s="98" t="s">
+    <row r="13" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A13" s="76" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="23" t="s">
@@ -3103,14 +3103,14 @@
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
       <c r="S13" s="16"/>
-      <c r="T13" s="85"/>
-      <c r="U13" s="86"/>
-      <c r="V13" s="86"/>
-      <c r="W13" s="86"/>
-      <c r="X13" s="86"/>
-      <c r="Y13" s="86"/>
-      <c r="Z13" s="86"/>
-      <c r="AA13" s="87"/>
+      <c r="T13" s="97"/>
+      <c r="U13" s="98"/>
+      <c r="V13" s="98"/>
+      <c r="W13" s="98"/>
+      <c r="X13" s="98"/>
+      <c r="Y13" s="98"/>
+      <c r="Z13" s="98"/>
+      <c r="AA13" s="99"/>
       <c r="AB13" s="14"/>
       <c r="AC13" s="15"/>
       <c r="AD13" s="31"/>
@@ -3171,10 +3171,10 @@
       <c r="CC13" s="15"/>
       <c r="CD13" s="15"/>
       <c r="CE13" s="16"/>
-      <c r="CF13" s="79"/>
+      <c r="CF13" s="91"/>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A14" s="98" t="s">
+    <row r="14" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A14" s="76" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="23" t="s">
@@ -3197,14 +3197,14 @@
       <c r="Q14" s="15"/>
       <c r="R14" s="15"/>
       <c r="S14" s="16"/>
-      <c r="T14" s="85"/>
-      <c r="U14" s="86"/>
-      <c r="V14" s="86"/>
-      <c r="W14" s="86"/>
-      <c r="X14" s="86"/>
-      <c r="Y14" s="86"/>
-      <c r="Z14" s="86"/>
-      <c r="AA14" s="87"/>
+      <c r="T14" s="97"/>
+      <c r="U14" s="98"/>
+      <c r="V14" s="98"/>
+      <c r="W14" s="98"/>
+      <c r="X14" s="98"/>
+      <c r="Y14" s="98"/>
+      <c r="Z14" s="98"/>
+      <c r="AA14" s="99"/>
       <c r="AB14" s="54" t="s">
         <v>34</v>
       </c>
@@ -3293,10 +3293,10 @@
       <c r="CC14" s="15"/>
       <c r="CD14" s="15"/>
       <c r="CE14" s="16"/>
-      <c r="CF14" s="79"/>
+      <c r="CF14" s="91"/>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A15" s="98" t="s">
+    <row r="15" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A15" s="76" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="23"/>
@@ -3317,14 +3317,14 @@
       <c r="Q15" s="15"/>
       <c r="R15" s="15"/>
       <c r="S15" s="16"/>
-      <c r="T15" s="85"/>
-      <c r="U15" s="86"/>
-      <c r="V15" s="86"/>
-      <c r="W15" s="86"/>
-      <c r="X15" s="86"/>
-      <c r="Y15" s="86"/>
-      <c r="Z15" s="86"/>
-      <c r="AA15" s="87"/>
+      <c r="T15" s="97"/>
+      <c r="U15" s="98"/>
+      <c r="V15" s="98"/>
+      <c r="W15" s="98"/>
+      <c r="X15" s="98"/>
+      <c r="Y15" s="98"/>
+      <c r="Z15" s="98"/>
+      <c r="AA15" s="99"/>
       <c r="AB15" s="14"/>
       <c r="AC15" s="15"/>
       <c r="AD15" s="15"/>
@@ -3350,7 +3350,9 @@
       <c r="AX15" s="15"/>
       <c r="AY15" s="16"/>
       <c r="AZ15" s="14"/>
-      <c r="BA15" s="15"/>
+      <c r="BA15" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="BB15" s="15"/>
       <c r="BC15" s="31"/>
       <c r="BD15" s="31"/>
@@ -3381,10 +3383,10 @@
       <c r="CC15" s="15"/>
       <c r="CD15" s="15"/>
       <c r="CE15" s="16"/>
-      <c r="CF15" s="79"/>
+      <c r="CF15" s="91"/>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A16" s="99" t="s">
+    <row r="16" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A16" s="77" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="23"/>
@@ -3405,14 +3407,14 @@
       <c r="Q16" s="15"/>
       <c r="R16" s="15"/>
       <c r="S16" s="16"/>
-      <c r="T16" s="85"/>
-      <c r="U16" s="86"/>
-      <c r="V16" s="86"/>
-      <c r="W16" s="86"/>
-      <c r="X16" s="86"/>
-      <c r="Y16" s="86"/>
-      <c r="Z16" s="86"/>
-      <c r="AA16" s="87"/>
+      <c r="T16" s="97"/>
+      <c r="U16" s="98"/>
+      <c r="V16" s="98"/>
+      <c r="W16" s="98"/>
+      <c r="X16" s="98"/>
+      <c r="Y16" s="98"/>
+      <c r="Z16" s="98"/>
+      <c r="AA16" s="99"/>
       <c r="AB16" s="14"/>
       <c r="AC16" s="15"/>
       <c r="AD16" s="15"/>
@@ -3469,10 +3471,10 @@
       <c r="CC16" s="15"/>
       <c r="CD16" s="15"/>
       <c r="CE16" s="16"/>
-      <c r="CF16" s="79"/>
+      <c r="CF16" s="91"/>
     </row>
-    <row r="17" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A17" s="98" t="s">
+    <row r="17" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A17" s="76" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="23" t="s">
@@ -3495,14 +3497,14 @@
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
       <c r="S17" s="16"/>
-      <c r="T17" s="85"/>
-      <c r="U17" s="86"/>
-      <c r="V17" s="86"/>
-      <c r="W17" s="86"/>
-      <c r="X17" s="86"/>
-      <c r="Y17" s="86"/>
-      <c r="Z17" s="86"/>
-      <c r="AA17" s="87"/>
+      <c r="T17" s="97"/>
+      <c r="U17" s="98"/>
+      <c r="V17" s="98"/>
+      <c r="W17" s="98"/>
+      <c r="X17" s="98"/>
+      <c r="Y17" s="98"/>
+      <c r="Z17" s="98"/>
+      <c r="AA17" s="99"/>
       <c r="AB17" s="14"/>
       <c r="AC17" s="15"/>
       <c r="AD17" s="15"/>
@@ -3535,13 +3537,19 @@
       <c r="AS17" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AT17" s="46"/>
-      <c r="AU17" s="46"/>
+      <c r="AT17" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU17" s="46" t="s">
+        <v>34</v>
+      </c>
       <c r="AV17" s="15"/>
       <c r="AW17" s="15"/>
       <c r="AX17" s="15"/>
       <c r="AY17" s="16"/>
-      <c r="AZ17" s="46"/>
+      <c r="AZ17" s="46" t="s">
+        <v>34</v>
+      </c>
       <c r="BA17" s="46"/>
       <c r="BB17" s="15"/>
       <c r="BC17" s="15"/>
@@ -3573,10 +3581,10 @@
       <c r="CC17" s="15"/>
       <c r="CD17" s="15"/>
       <c r="CE17" s="16"/>
-      <c r="CF17" s="79"/>
+      <c r="CF17" s="91"/>
     </row>
-    <row r="18" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A18" s="98" t="s">
+    <row r="18" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A18" s="76" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="23" t="s">
@@ -3599,14 +3607,14 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
       <c r="S18" s="16"/>
-      <c r="T18" s="85"/>
-      <c r="U18" s="86"/>
-      <c r="V18" s="86"/>
-      <c r="W18" s="86"/>
-      <c r="X18" s="86"/>
-      <c r="Y18" s="86"/>
-      <c r="Z18" s="86"/>
-      <c r="AA18" s="87"/>
+      <c r="T18" s="97"/>
+      <c r="U18" s="98"/>
+      <c r="V18" s="98"/>
+      <c r="W18" s="98"/>
+      <c r="X18" s="98"/>
+      <c r="Y18" s="98"/>
+      <c r="Z18" s="98"/>
+      <c r="AA18" s="99"/>
       <c r="AB18" s="51" t="s">
         <v>34</v>
       </c>
@@ -3681,9 +3689,9 @@
       <c r="CC18" s="15"/>
       <c r="CD18" s="15"/>
       <c r="CE18" s="16"/>
-      <c r="CF18" s="79"/>
+      <c r="CF18" s="91"/>
     </row>
-    <row r="19" spans="1:84" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:84" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
         <v>35</v>
       </c>
@@ -3705,14 +3713,14 @@
       <c r="Q19" s="58"/>
       <c r="R19" s="58"/>
       <c r="S19" s="61"/>
-      <c r="T19" s="85"/>
-      <c r="U19" s="86"/>
-      <c r="V19" s="86"/>
-      <c r="W19" s="86"/>
-      <c r="X19" s="86"/>
-      <c r="Y19" s="86"/>
-      <c r="Z19" s="86"/>
-      <c r="AA19" s="87"/>
+      <c r="T19" s="97"/>
+      <c r="U19" s="98"/>
+      <c r="V19" s="98"/>
+      <c r="W19" s="98"/>
+      <c r="X19" s="98"/>
+      <c r="Y19" s="98"/>
+      <c r="Z19" s="98"/>
+      <c r="AA19" s="99"/>
       <c r="AB19" s="57"/>
       <c r="AC19" s="60"/>
       <c r="AD19" s="60"/>
@@ -3769,9 +3777,9 @@
       <c r="CC19" s="58"/>
       <c r="CD19" s="58"/>
       <c r="CE19" s="61"/>
-      <c r="CF19" s="79"/>
+      <c r="CF19" s="91"/>
     </row>
-    <row r="20" spans="1:84" s="63" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:84" s="63" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="70" t="s">
         <v>37</v>
       </c>
@@ -3793,14 +3801,14 @@
       <c r="Q20" s="58"/>
       <c r="R20" s="58"/>
       <c r="S20" s="61"/>
-      <c r="T20" s="85"/>
-      <c r="U20" s="86"/>
-      <c r="V20" s="86"/>
-      <c r="W20" s="86"/>
-      <c r="X20" s="86"/>
-      <c r="Y20" s="86"/>
-      <c r="Z20" s="86"/>
-      <c r="AA20" s="87"/>
+      <c r="T20" s="97"/>
+      <c r="U20" s="98"/>
+      <c r="V20" s="98"/>
+      <c r="W20" s="98"/>
+      <c r="X20" s="98"/>
+      <c r="Y20" s="98"/>
+      <c r="Z20" s="98"/>
+      <c r="AA20" s="99"/>
       <c r="AB20" s="57"/>
       <c r="AC20" s="60"/>
       <c r="AD20" s="60"/>
@@ -3857,10 +3865,10 @@
       <c r="CC20" s="58"/>
       <c r="CD20" s="58"/>
       <c r="CE20" s="61"/>
-      <c r="CF20" s="79"/>
+      <c r="CF20" s="91"/>
     </row>
-    <row r="21" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A21" s="100" t="s">
+    <row r="21" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A21" s="78" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="23"/>
@@ -3881,14 +3889,14 @@
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
       <c r="S21" s="16"/>
-      <c r="T21" s="85"/>
-      <c r="U21" s="86"/>
-      <c r="V21" s="86"/>
-      <c r="W21" s="86"/>
-      <c r="X21" s="86"/>
-      <c r="Y21" s="86"/>
-      <c r="Z21" s="86"/>
-      <c r="AA21" s="87"/>
+      <c r="T21" s="97"/>
+      <c r="U21" s="98"/>
+      <c r="V21" s="98"/>
+      <c r="W21" s="98"/>
+      <c r="X21" s="98"/>
+      <c r="Y21" s="98"/>
+      <c r="Z21" s="98"/>
+      <c r="AA21" s="99"/>
       <c r="AB21" s="14"/>
       <c r="AC21" s="15"/>
       <c r="AD21" s="15"/>
@@ -3945,10 +3953,10 @@
       <c r="CC21" s="15"/>
       <c r="CD21" s="15"/>
       <c r="CE21" s="16"/>
-      <c r="CF21" s="79"/>
+      <c r="CF21" s="91"/>
     </row>
-    <row r="22" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A22" s="101" t="s">
+    <row r="22" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A22" s="79" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="23"/>
@@ -3969,14 +3977,14 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
       <c r="S22" s="16"/>
-      <c r="T22" s="85"/>
-      <c r="U22" s="86"/>
-      <c r="V22" s="86"/>
-      <c r="W22" s="86"/>
-      <c r="X22" s="86"/>
-      <c r="Y22" s="86"/>
-      <c r="Z22" s="86"/>
-      <c r="AA22" s="87"/>
+      <c r="T22" s="97"/>
+      <c r="U22" s="98"/>
+      <c r="V22" s="98"/>
+      <c r="W22" s="98"/>
+      <c r="X22" s="98"/>
+      <c r="Y22" s="98"/>
+      <c r="Z22" s="98"/>
+      <c r="AA22" s="99"/>
       <c r="AB22" s="14"/>
       <c r="AC22" s="15"/>
       <c r="AD22" s="15"/>
@@ -4033,10 +4041,10 @@
       <c r="CC22" s="15"/>
       <c r="CD22" s="15"/>
       <c r="CE22" s="16"/>
-      <c r="CF22" s="79"/>
+      <c r="CF22" s="91"/>
     </row>
-    <row r="23" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A23" s="100" t="s">
+    <row r="23" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A23" s="78" t="s">
         <v>29</v>
       </c>
       <c r="B23" s="23"/>
@@ -4057,14 +4065,14 @@
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
       <c r="S23" s="16"/>
-      <c r="T23" s="85"/>
-      <c r="U23" s="86"/>
-      <c r="V23" s="86"/>
-      <c r="W23" s="86"/>
-      <c r="X23" s="86"/>
-      <c r="Y23" s="86"/>
-      <c r="Z23" s="86"/>
-      <c r="AA23" s="87"/>
+      <c r="T23" s="97"/>
+      <c r="U23" s="98"/>
+      <c r="V23" s="98"/>
+      <c r="W23" s="98"/>
+      <c r="X23" s="98"/>
+      <c r="Y23" s="98"/>
+      <c r="Z23" s="98"/>
+      <c r="AA23" s="99"/>
       <c r="AB23" s="14"/>
       <c r="AC23" s="15"/>
       <c r="AD23" s="15"/>
@@ -4121,10 +4129,10 @@
       <c r="CC23" s="15"/>
       <c r="CD23" s="15"/>
       <c r="CE23" s="16"/>
-      <c r="CF23" s="79"/>
+      <c r="CF23" s="91"/>
     </row>
-    <row r="24" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A24" s="100" t="s">
+    <row r="24" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A24" s="78" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="23"/>
@@ -4145,14 +4153,14 @@
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
       <c r="S24" s="16"/>
-      <c r="T24" s="85"/>
-      <c r="U24" s="86"/>
-      <c r="V24" s="86"/>
-      <c r="W24" s="86"/>
-      <c r="X24" s="86"/>
-      <c r="Y24" s="86"/>
-      <c r="Z24" s="86"/>
-      <c r="AA24" s="87"/>
+      <c r="T24" s="97"/>
+      <c r="U24" s="98"/>
+      <c r="V24" s="98"/>
+      <c r="W24" s="98"/>
+      <c r="X24" s="98"/>
+      <c r="Y24" s="98"/>
+      <c r="Z24" s="98"/>
+      <c r="AA24" s="99"/>
       <c r="AB24" s="14"/>
       <c r="AC24" s="14"/>
       <c r="AD24" s="48"/>
@@ -4209,10 +4217,10 @@
       <c r="CC24" s="15"/>
       <c r="CD24" s="15"/>
       <c r="CE24" s="16"/>
-      <c r="CF24" s="79"/>
+      <c r="CF24" s="91"/>
     </row>
-    <row r="25" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A25" s="100" t="s">
+    <row r="25" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A25" s="78" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="23"/>
@@ -4233,14 +4241,14 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
       <c r="S25" s="16"/>
-      <c r="T25" s="85"/>
-      <c r="U25" s="86"/>
-      <c r="V25" s="86"/>
-      <c r="W25" s="86"/>
-      <c r="X25" s="86"/>
-      <c r="Y25" s="86"/>
-      <c r="Z25" s="86"/>
-      <c r="AA25" s="87"/>
+      <c r="T25" s="97"/>
+      <c r="U25" s="98"/>
+      <c r="V25" s="98"/>
+      <c r="W25" s="98"/>
+      <c r="X25" s="98"/>
+      <c r="Y25" s="98"/>
+      <c r="Z25" s="98"/>
+      <c r="AA25" s="99"/>
       <c r="AB25" s="14"/>
       <c r="AC25" s="15"/>
       <c r="AD25" s="15"/>
@@ -4292,9 +4300,9 @@
       <c r="CC25" s="15"/>
       <c r="CD25" s="15"/>
       <c r="CE25" s="16"/>
-      <c r="CF25" s="79"/>
+      <c r="CF25" s="91"/>
     </row>
-    <row r="26" spans="1:84" s="63" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:84" s="63" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="71" t="s">
         <v>38</v>
       </c>
@@ -4315,14 +4323,14 @@
       <c r="Q26" s="60"/>
       <c r="R26" s="60"/>
       <c r="S26" s="62"/>
-      <c r="T26" s="85"/>
-      <c r="U26" s="86"/>
-      <c r="V26" s="86"/>
-      <c r="W26" s="86"/>
-      <c r="X26" s="86"/>
-      <c r="Y26" s="86"/>
-      <c r="Z26" s="86"/>
-      <c r="AA26" s="87"/>
+      <c r="T26" s="97"/>
+      <c r="U26" s="98"/>
+      <c r="V26" s="98"/>
+      <c r="W26" s="98"/>
+      <c r="X26" s="98"/>
+      <c r="Y26" s="98"/>
+      <c r="Z26" s="98"/>
+      <c r="AA26" s="99"/>
       <c r="AB26" s="60"/>
       <c r="AC26" s="60"/>
       <c r="AD26" s="60"/>
@@ -4379,9 +4387,9 @@
       <c r="CC26" s="60"/>
       <c r="CD26" s="60"/>
       <c r="CE26" s="62"/>
-      <c r="CF26" s="79"/>
+      <c r="CF26" s="91"/>
     </row>
-    <row r="27" spans="1:84" s="66" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:84" s="66" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="72" t="s">
         <v>39</v>
       </c>
@@ -4402,14 +4410,14 @@
       <c r="Q27" s="64"/>
       <c r="R27" s="64"/>
       <c r="S27" s="67"/>
-      <c r="T27" s="85"/>
-      <c r="U27" s="86"/>
-      <c r="V27" s="86"/>
-      <c r="W27" s="86"/>
-      <c r="X27" s="86"/>
-      <c r="Y27" s="86"/>
-      <c r="Z27" s="86"/>
-      <c r="AA27" s="87"/>
+      <c r="T27" s="97"/>
+      <c r="U27" s="98"/>
+      <c r="V27" s="98"/>
+      <c r="W27" s="98"/>
+      <c r="X27" s="98"/>
+      <c r="Y27" s="98"/>
+      <c r="Z27" s="98"/>
+      <c r="AA27" s="99"/>
       <c r="AB27" s="64"/>
       <c r="AC27" s="64"/>
       <c r="AD27" s="64"/>
@@ -4466,9 +4474,9 @@
       <c r="CC27" s="64"/>
       <c r="CD27" s="64"/>
       <c r="CE27" s="67"/>
-      <c r="CF27" s="79"/>
+      <c r="CF27" s="91"/>
     </row>
-    <row r="28" spans="1:84" s="66" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:84" s="66" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72" t="s">
         <v>40</v>
       </c>
@@ -4489,14 +4497,14 @@
       <c r="Q28" s="64"/>
       <c r="R28" s="64"/>
       <c r="S28" s="67"/>
-      <c r="T28" s="85"/>
-      <c r="U28" s="86"/>
-      <c r="V28" s="86"/>
-      <c r="W28" s="86"/>
-      <c r="X28" s="86"/>
-      <c r="Y28" s="86"/>
-      <c r="Z28" s="86"/>
-      <c r="AA28" s="87"/>
+      <c r="T28" s="97"/>
+      <c r="U28" s="98"/>
+      <c r="V28" s="98"/>
+      <c r="W28" s="98"/>
+      <c r="X28" s="98"/>
+      <c r="Y28" s="98"/>
+      <c r="Z28" s="98"/>
+      <c r="AA28" s="99"/>
       <c r="AB28" s="64"/>
       <c r="AC28" s="64"/>
       <c r="AD28" s="64"/>
@@ -4553,9 +4561,9 @@
       <c r="CC28" s="64"/>
       <c r="CD28" s="64"/>
       <c r="CE28" s="67"/>
-      <c r="CF28" s="79"/>
+      <c r="CF28" s="91"/>
     </row>
-    <row r="29" spans="1:84" s="63" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:84" s="63" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="73" t="s">
         <v>41</v>
       </c>
@@ -4577,14 +4585,14 @@
       <c r="Q29" s="58"/>
       <c r="R29" s="58"/>
       <c r="S29" s="61"/>
-      <c r="T29" s="85"/>
-      <c r="U29" s="86"/>
-      <c r="V29" s="86"/>
-      <c r="W29" s="86"/>
-      <c r="X29" s="86"/>
-      <c r="Y29" s="86"/>
-      <c r="Z29" s="86"/>
-      <c r="AA29" s="87"/>
+      <c r="T29" s="97"/>
+      <c r="U29" s="98"/>
+      <c r="V29" s="98"/>
+      <c r="W29" s="98"/>
+      <c r="X29" s="98"/>
+      <c r="Y29" s="98"/>
+      <c r="Z29" s="98"/>
+      <c r="AA29" s="99"/>
       <c r="AB29" s="57"/>
       <c r="AC29" s="60"/>
       <c r="AD29" s="60"/>
@@ -4641,10 +4649,10 @@
       <c r="CC29" s="58"/>
       <c r="CD29" s="58"/>
       <c r="CE29" s="61"/>
-      <c r="CF29" s="79"/>
+      <c r="CF29" s="91"/>
     </row>
-    <row r="30" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A30" s="102" t="s">
+    <row r="30" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A30" s="80" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="23"/>
@@ -4665,14 +4673,14 @@
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
       <c r="S30" s="16"/>
-      <c r="T30" s="85"/>
-      <c r="U30" s="86"/>
-      <c r="V30" s="86"/>
-      <c r="W30" s="86"/>
-      <c r="X30" s="86"/>
-      <c r="Y30" s="86"/>
-      <c r="Z30" s="86"/>
-      <c r="AA30" s="87"/>
+      <c r="T30" s="97"/>
+      <c r="U30" s="98"/>
+      <c r="V30" s="98"/>
+      <c r="W30" s="98"/>
+      <c r="X30" s="98"/>
+      <c r="Y30" s="98"/>
+      <c r="Z30" s="98"/>
+      <c r="AA30" s="99"/>
       <c r="AB30" s="14"/>
       <c r="AC30" s="15"/>
       <c r="AD30" s="15"/>
@@ -4729,9 +4737,9 @@
       <c r="CC30" s="15"/>
       <c r="CD30" s="15"/>
       <c r="CE30" s="16"/>
-      <c r="CF30" s="79"/>
+      <c r="CF30" s="91"/>
     </row>
-    <row r="31" spans="1:84" s="63" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:84" s="63" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="74" t="s">
         <v>42</v>
       </c>
@@ -4753,14 +4761,14 @@
       <c r="Q31" s="58"/>
       <c r="R31" s="58"/>
       <c r="S31" s="61"/>
-      <c r="T31" s="85"/>
-      <c r="U31" s="86"/>
-      <c r="V31" s="86"/>
-      <c r="W31" s="86"/>
-      <c r="X31" s="86"/>
-      <c r="Y31" s="86"/>
-      <c r="Z31" s="86"/>
-      <c r="AA31" s="87"/>
+      <c r="T31" s="97"/>
+      <c r="U31" s="98"/>
+      <c r="V31" s="98"/>
+      <c r="W31" s="98"/>
+      <c r="X31" s="98"/>
+      <c r="Y31" s="98"/>
+      <c r="Z31" s="98"/>
+      <c r="AA31" s="99"/>
       <c r="AB31" s="57"/>
       <c r="AC31" s="60"/>
       <c r="AD31" s="60"/>
@@ -4817,9 +4825,9 @@
       <c r="CC31" s="58"/>
       <c r="CD31" s="58"/>
       <c r="CE31" s="61"/>
-      <c r="CF31" s="79"/>
+      <c r="CF31" s="91"/>
     </row>
-    <row r="32" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>15</v>
       </c>
@@ -4841,14 +4849,14 @@
       <c r="Q32" s="33"/>
       <c r="R32" s="33"/>
       <c r="S32" s="34"/>
-      <c r="T32" s="85"/>
-      <c r="U32" s="86"/>
-      <c r="V32" s="86"/>
-      <c r="W32" s="86"/>
-      <c r="X32" s="86"/>
-      <c r="Y32" s="86"/>
-      <c r="Z32" s="86"/>
-      <c r="AA32" s="87"/>
+      <c r="T32" s="97"/>
+      <c r="U32" s="98"/>
+      <c r="V32" s="98"/>
+      <c r="W32" s="98"/>
+      <c r="X32" s="98"/>
+      <c r="Y32" s="98"/>
+      <c r="Z32" s="98"/>
+      <c r="AA32" s="99"/>
       <c r="AB32" s="35"/>
       <c r="AC32" s="36"/>
       <c r="AD32" s="36"/>
@@ -4905,9 +4913,9 @@
       <c r="CC32" s="36"/>
       <c r="CD32" s="36"/>
       <c r="CE32" s="37"/>
-      <c r="CF32" s="79"/>
+      <c r="CF32" s="91"/>
     </row>
-    <row r="33" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:84" x14ac:dyDescent="0.25">
       <c r="B33" s="23"/>
       <c r="C33" s="13"/>
       <c r="D33" s="14"/>
@@ -4926,14 +4934,14 @@
       <c r="Q33" s="15"/>
       <c r="R33" s="15"/>
       <c r="S33" s="16"/>
-      <c r="T33" s="85"/>
-      <c r="U33" s="86"/>
-      <c r="V33" s="86"/>
-      <c r="W33" s="86"/>
-      <c r="X33" s="86"/>
-      <c r="Y33" s="86"/>
-      <c r="Z33" s="86"/>
-      <c r="AA33" s="87"/>
+      <c r="T33" s="97"/>
+      <c r="U33" s="98"/>
+      <c r="V33" s="98"/>
+      <c r="W33" s="98"/>
+      <c r="X33" s="98"/>
+      <c r="Y33" s="98"/>
+      <c r="Z33" s="98"/>
+      <c r="AA33" s="99"/>
       <c r="AB33" s="14"/>
       <c r="AC33" s="15"/>
       <c r="AD33" s="15"/>
@@ -4990,9 +4998,9 @@
       <c r="CC33" s="15"/>
       <c r="CD33" s="15"/>
       <c r="CE33" s="16"/>
-      <c r="CF33" s="79"/>
+      <c r="CF33" s="91"/>
     </row>
-    <row r="34" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="23"/>
       <c r="C34" s="13"/>
@@ -5012,14 +5020,14 @@
       <c r="Q34" s="15"/>
       <c r="R34" s="15"/>
       <c r="S34" s="16"/>
-      <c r="T34" s="85"/>
-      <c r="U34" s="86"/>
-      <c r="V34" s="86"/>
-      <c r="W34" s="86"/>
-      <c r="X34" s="86"/>
-      <c r="Y34" s="86"/>
-      <c r="Z34" s="86"/>
-      <c r="AA34" s="87"/>
+      <c r="T34" s="97"/>
+      <c r="U34" s="98"/>
+      <c r="V34" s="98"/>
+      <c r="W34" s="98"/>
+      <c r="X34" s="98"/>
+      <c r="Y34" s="98"/>
+      <c r="Z34" s="98"/>
+      <c r="AA34" s="99"/>
       <c r="AB34" s="14"/>
       <c r="AC34" s="15"/>
       <c r="AD34" s="15"/>
@@ -5076,9 +5084,9 @@
       <c r="CC34" s="15"/>
       <c r="CD34" s="15"/>
       <c r="CE34" s="16"/>
-      <c r="CF34" s="79"/>
+      <c r="CF34" s="91"/>
     </row>
-    <row r="35" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="23"/>
       <c r="C35" s="13"/>
@@ -5098,14 +5106,14 @@
       <c r="Q35" s="15"/>
       <c r="R35" s="15"/>
       <c r="S35" s="16"/>
-      <c r="T35" s="85"/>
-      <c r="U35" s="86"/>
-      <c r="V35" s="86"/>
-      <c r="W35" s="86"/>
-      <c r="X35" s="86"/>
-      <c r="Y35" s="86"/>
-      <c r="Z35" s="86"/>
-      <c r="AA35" s="87"/>
+      <c r="T35" s="97"/>
+      <c r="U35" s="98"/>
+      <c r="V35" s="98"/>
+      <c r="W35" s="98"/>
+      <c r="X35" s="98"/>
+      <c r="Y35" s="98"/>
+      <c r="Z35" s="98"/>
+      <c r="AA35" s="99"/>
       <c r="AB35" s="14"/>
       <c r="AC35" s="15"/>
       <c r="AD35" s="15"/>
@@ -5162,9 +5170,9 @@
       <c r="CC35" s="15"/>
       <c r="CD35" s="15"/>
       <c r="CE35" s="16"/>
-      <c r="CF35" s="79"/>
+      <c r="CF35" s="91"/>
     </row>
-    <row r="36" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:84" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17"/>
       <c r="B36" s="24"/>
       <c r="C36" s="18"/>
@@ -5184,14 +5192,14 @@
       <c r="Q36" s="20"/>
       <c r="R36" s="20"/>
       <c r="S36" s="21"/>
-      <c r="T36" s="88"/>
-      <c r="U36" s="89"/>
-      <c r="V36" s="89"/>
-      <c r="W36" s="89"/>
-      <c r="X36" s="89"/>
-      <c r="Y36" s="89"/>
-      <c r="Z36" s="89"/>
-      <c r="AA36" s="90"/>
+      <c r="T36" s="100"/>
+      <c r="U36" s="101"/>
+      <c r="V36" s="101"/>
+      <c r="W36" s="101"/>
+      <c r="X36" s="101"/>
+      <c r="Y36" s="101"/>
+      <c r="Z36" s="101"/>
+      <c r="AA36" s="102"/>
       <c r="AB36" s="19"/>
       <c r="AC36" s="20"/>
       <c r="AD36" s="20"/>
@@ -5248,112 +5256,112 @@
       <c r="CC36" s="20"/>
       <c r="CD36" s="20"/>
       <c r="CE36" s="21"/>
-      <c r="CF36" s="79"/>
+      <c r="CF36" s="91"/>
     </row>
-    <row r="37" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A37" s="76"/>
-      <c r="B37" s="76"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="76"/>
-      <c r="J37" s="76"/>
-      <c r="K37" s="76"/>
-      <c r="L37" s="76"/>
-      <c r="M37" s="76"/>
-      <c r="N37" s="76"/>
-      <c r="O37" s="76"/>
-      <c r="P37" s="76"/>
-      <c r="Q37" s="76"/>
-      <c r="R37" s="76"/>
-      <c r="S37" s="76"/>
-      <c r="T37" s="76"/>
-      <c r="U37" s="76"/>
-      <c r="V37" s="76"/>
-      <c r="W37" s="76"/>
-      <c r="X37" s="76"/>
-      <c r="Y37" s="76"/>
-      <c r="Z37" s="76"/>
-      <c r="AA37" s="76"/>
-      <c r="AB37" s="76"/>
-      <c r="AC37" s="76"/>
-      <c r="AD37" s="76"/>
-      <c r="AE37" s="76"/>
-      <c r="AF37" s="76"/>
-      <c r="AG37" s="76"/>
-      <c r="AH37" s="76"/>
-      <c r="AI37" s="76"/>
-      <c r="AJ37" s="76"/>
-      <c r="AK37" s="76"/>
-      <c r="AL37" s="76"/>
-      <c r="AM37" s="76"/>
-      <c r="AN37" s="76"/>
-      <c r="AO37" s="76"/>
-      <c r="AP37" s="76"/>
-      <c r="AQ37" s="76"/>
-      <c r="AR37" s="76"/>
-      <c r="AS37" s="76"/>
-      <c r="AT37" s="76"/>
-      <c r="AU37" s="76"/>
-      <c r="AV37" s="76"/>
-      <c r="AW37" s="76"/>
-      <c r="AX37" s="76"/>
-      <c r="AY37" s="76"/>
-      <c r="AZ37" s="76"/>
-      <c r="BA37" s="76"/>
-      <c r="BB37" s="76"/>
-      <c r="BC37" s="76"/>
-      <c r="BD37" s="76"/>
-      <c r="BE37" s="76"/>
-      <c r="BF37" s="76"/>
-      <c r="BG37" s="76"/>
-      <c r="BH37" s="76"/>
-      <c r="BI37" s="76"/>
-      <c r="BJ37" s="76"/>
-      <c r="BK37" s="76"/>
-      <c r="BL37" s="76"/>
-      <c r="BM37" s="76"/>
-      <c r="BN37" s="76"/>
-      <c r="BO37" s="76"/>
-      <c r="BP37" s="76"/>
-      <c r="BQ37" s="76"/>
-      <c r="BR37" s="76"/>
-      <c r="BS37" s="76"/>
-      <c r="BT37" s="76"/>
-      <c r="BU37" s="76"/>
-      <c r="BV37" s="76"/>
-      <c r="BW37" s="76"/>
-      <c r="BX37" s="76"/>
-      <c r="BY37" s="76"/>
-      <c r="BZ37" s="76"/>
-      <c r="CA37" s="76"/>
-      <c r="CB37" s="76"/>
-      <c r="CC37" s="76"/>
-      <c r="CD37" s="76"/>
-      <c r="CE37" s="76"/>
+    <row r="37" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A37" s="90"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="90"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="90"/>
+      <c r="F37" s="90"/>
+      <c r="G37" s="90"/>
+      <c r="H37" s="90"/>
+      <c r="I37" s="90"/>
+      <c r="J37" s="90"/>
+      <c r="K37" s="90"/>
+      <c r="L37" s="90"/>
+      <c r="M37" s="90"/>
+      <c r="N37" s="90"/>
+      <c r="O37" s="90"/>
+      <c r="P37" s="90"/>
+      <c r="Q37" s="90"/>
+      <c r="R37" s="90"/>
+      <c r="S37" s="90"/>
+      <c r="T37" s="90"/>
+      <c r="U37" s="90"/>
+      <c r="V37" s="90"/>
+      <c r="W37" s="90"/>
+      <c r="X37" s="90"/>
+      <c r="Y37" s="90"/>
+      <c r="Z37" s="90"/>
+      <c r="AA37" s="90"/>
+      <c r="AB37" s="90"/>
+      <c r="AC37" s="90"/>
+      <c r="AD37" s="90"/>
+      <c r="AE37" s="90"/>
+      <c r="AF37" s="90"/>
+      <c r="AG37" s="90"/>
+      <c r="AH37" s="90"/>
+      <c r="AI37" s="90"/>
+      <c r="AJ37" s="90"/>
+      <c r="AK37" s="90"/>
+      <c r="AL37" s="90"/>
+      <c r="AM37" s="90"/>
+      <c r="AN37" s="90"/>
+      <c r="AO37" s="90"/>
+      <c r="AP37" s="90"/>
+      <c r="AQ37" s="90"/>
+      <c r="AR37" s="90"/>
+      <c r="AS37" s="90"/>
+      <c r="AT37" s="90"/>
+      <c r="AU37" s="90"/>
+      <c r="AV37" s="90"/>
+      <c r="AW37" s="90"/>
+      <c r="AX37" s="90"/>
+      <c r="AY37" s="90"/>
+      <c r="AZ37" s="90"/>
+      <c r="BA37" s="90"/>
+      <c r="BB37" s="90"/>
+      <c r="BC37" s="90"/>
+      <c r="BD37" s="90"/>
+      <c r="BE37" s="90"/>
+      <c r="BF37" s="90"/>
+      <c r="BG37" s="90"/>
+      <c r="BH37" s="90"/>
+      <c r="BI37" s="90"/>
+      <c r="BJ37" s="90"/>
+      <c r="BK37" s="90"/>
+      <c r="BL37" s="90"/>
+      <c r="BM37" s="90"/>
+      <c r="BN37" s="90"/>
+      <c r="BO37" s="90"/>
+      <c r="BP37" s="90"/>
+      <c r="BQ37" s="90"/>
+      <c r="BR37" s="90"/>
+      <c r="BS37" s="90"/>
+      <c r="BT37" s="90"/>
+      <c r="BU37" s="90"/>
+      <c r="BV37" s="90"/>
+      <c r="BW37" s="90"/>
+      <c r="BX37" s="90"/>
+      <c r="BY37" s="90"/>
+      <c r="BZ37" s="90"/>
+      <c r="CA37" s="90"/>
+      <c r="CB37" s="90"/>
+      <c r="CC37" s="90"/>
+      <c r="CD37" s="90"/>
+      <c r="CE37" s="90"/>
     </row>
-    <row r="40" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:84" x14ac:dyDescent="0.25">
       <c r="B40" s="38" t="s">
         <v>17</v>
       </c>
       <c r="C40" s="39"/>
     </row>
-    <row r="41" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:84" x14ac:dyDescent="0.25">
       <c r="B41" s="38" t="s">
         <v>18</v>
       </c>
       <c r="C41" s="40"/>
     </row>
-    <row r="42" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:84" x14ac:dyDescent="0.25">
       <c r="B42" s="38" t="s">
         <v>19</v>
       </c>
       <c r="C42" s="41"/>
     </row>
-    <row r="43" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:84" x14ac:dyDescent="0.25">
       <c r="B43" s="38" t="s">
         <v>20</v>
       </c>
@@ -5361,6 +5369,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A37:CE37"/>
+    <mergeCell ref="D2:AQ3"/>
+    <mergeCell ref="CF4:CF36"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="T6:AA36"/>
+    <mergeCell ref="AZ4:BC4"/>
+    <mergeCell ref="BD4:BG4"/>
+    <mergeCell ref="BH4:BK4"/>
+    <mergeCell ref="BL4:BO4"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="T4:W4"/>
+    <mergeCell ref="X4:AA4"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="AR2:CE3"/>
     <mergeCell ref="AJ4:AM4"/>
@@ -5377,18 +5397,6 @@
     <mergeCell ref="BX4:CA4"/>
     <mergeCell ref="CB4:CE4"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A37:CE37"/>
-    <mergeCell ref="D2:AQ3"/>
-    <mergeCell ref="CF4:CF36"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="T6:AA36"/>
-    <mergeCell ref="AZ4:BC4"/>
-    <mergeCell ref="BD4:BG4"/>
-    <mergeCell ref="BH4:BK4"/>
-    <mergeCell ref="BL4:BO4"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="T4:W4"/>
-    <mergeCell ref="X4:AA4"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="B6:B26 B29:B36">
@@ -5417,26 +5425,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2041c0d2b30335279095007fcb0a9d7c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="56b9c1bb8339570eda07374d036e5caf" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -5649,10 +5637,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E70815D-A53F-41E3-B87E-1E164A9F927C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5675,20 +5694,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E70815D-A53F-41E3-B87E-1E164A9F927C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>